<commit_message>
added/cleaned variables usable to filter by site and tree number for 04 and 09
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5BDAEB-39FD-4766-B243-C606346CC2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20012960-A2FB-41F5-AAF8-FD12B35B9944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-7155" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
@@ -1694,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A5F083-2EA9-48B2-AF8F-72865D9CF0AB}">
   <dimension ref="A3:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2412,8 +2412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7AB688-5A0A-4572-BDE5-9C92B4B738E7}">
   <dimension ref="A4:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added sheet to Summary providing in depth information about the initially selected variables of the 'Arbolado' datasets
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20012960-A2FB-41F5-AAF8-FD12B35B9944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF768DE-B05D-4FF3-A3B2-3D7D9265E364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-7155" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Secciones_Data" sheetId="2" r:id="rId1"/>
     <sheet name="Arbolados_Data" sheetId="3" r:id="rId2"/>
-    <sheet name="Conglomerados_04" sheetId="1" r:id="rId3"/>
+    <sheet name="OldName-Newname" sheetId="4" r:id="rId3"/>
+    <sheet name="Conglomerados_04" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="592">
   <si>
     <t>Variable</t>
   </si>
@@ -1180,9 +1181,6 @@
     <t>AlturaFComercial</t>
   </si>
   <si>
-    <t>Tipo_Veg</t>
-  </si>
-  <si>
     <t xml:space="preserve">-&gt; </t>
   </si>
   <si>
@@ -1211,13 +1209,658 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>NumeroAnillos25</t>
+  </si>
+  <si>
+    <t>LongitudAnillos10</t>
+  </si>
+  <si>
+    <t>AreaBasal</t>
+  </si>
+  <si>
+    <t>AreaCopa</t>
+  </si>
+  <si>
+    <t>VigorEtapa</t>
+  </si>
+  <si>
+    <t>AlturaTotal</t>
+  </si>
+  <si>
+    <t>DiametroNormal</t>
+  </si>
+  <si>
+    <t>FormaBiologica</t>
+  </si>
+  <si>
+    <t>TipoVegSV</t>
+  </si>
+  <si>
+    <t>Arb.04</t>
+  </si>
+  <si>
+    <t>Arb.09</t>
+  </si>
+  <si>
+    <t>Arb.14</t>
+  </si>
+  <si>
+    <t>NewName</t>
+  </si>
+  <si>
+    <t>Nr.</t>
+  </si>
+  <si>
+    <t>NoIndividuo</t>
+  </si>
+  <si>
+    <t>Sitenumber</t>
+  </si>
+  <si>
+    <t>Clusternumber</t>
+  </si>
+  <si>
+    <t>IndividualTreeNumber</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Especie</t>
+  </si>
+  <si>
+    <t>familiy name</t>
+  </si>
+  <si>
+    <t>scientific name</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>biological form</t>
+  </si>
+  <si>
+    <t>clg_sit_arb</t>
+  </si>
+  <si>
+    <t>CCCC_S_T</t>
+  </si>
+  <si>
+    <t>2004 - 2020</t>
+  </si>
+  <si>
+    <t>n = 32</t>
+  </si>
+  <si>
+    <t>n = 4</t>
+  </si>
+  <si>
+    <t>NumAnillos26</t>
+  </si>
+  <si>
+    <t>Danio3</t>
+  </si>
+  <si>
+    <t>Severidad3</t>
+  </si>
+  <si>
+    <t>String of Cluster, Site, ITN</t>
+  </si>
+  <si>
+    <t>clg_sit_reg</t>
+  </si>
+  <si>
+    <t>NoRama</t>
+  </si>
+  <si>
+    <t>CveVeg_S5/S7</t>
+  </si>
+  <si>
+    <t>TipoVeg_S5/S7</t>
+  </si>
+  <si>
+    <t>Number of years to reach a height of 1.30m</t>
+  </si>
+  <si>
+    <t>common name</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>can be extracted from</t>
+  </si>
+  <si>
+    <t>Consecutive_C3</t>
+  </si>
+  <si>
+    <t>2004 - 2007</t>
+  </si>
+  <si>
+    <t>2009 - 2014</t>
+  </si>
+  <si>
+    <t>2015 - 2020</t>
+  </si>
+  <si>
+    <t>n = 33</t>
+  </si>
+  <si>
+    <t>n = 38</t>
+  </si>
+  <si>
+    <t>values (is)</t>
+  </si>
+  <si>
+    <t>values (raw)</t>
+  </si>
+  <si>
+    <t>values (to be)</t>
+  </si>
+  <si>
+    <t>for all</t>
+  </si>
+  <si>
+    <t>n= 32</t>
+  </si>
+  <si>
+    <t>n= 4</t>
+  </si>
+  <si>
+    <t>5-digit</t>
+  </si>
+  <si>
+    <t>n = 146</t>
+  </si>
+  <si>
+    <t>n = 201</t>
+  </si>
+  <si>
+    <t>n = 239</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>n= 146</t>
+  </si>
+  <si>
+    <t>n= 207</t>
+  </si>
+  <si>
+    <t>n= 255</t>
+  </si>
+  <si>
+    <t>don't know what this column is stating tbh</t>
+  </si>
+  <si>
+    <t>n = 201 (Registro == 316 + 213144_4_28)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">check/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fixed but to be implemented in final code</t>
+    </r>
+  </si>
+  <si>
+    <t>maybe cut it from ds?</t>
+  </si>
+  <si>
+    <t>n= 133</t>
+  </si>
+  <si>
+    <t>n= 131</t>
+  </si>
+  <si>
+    <t>n= 126</t>
+  </si>
+  <si>
+    <t>n= 17, NA and NULL</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>df individual entries but no mistakes</t>
+  </si>
+  <si>
+    <t>un fuste, dos o más fustes, NA</t>
+  </si>
+  <si>
+    <t>--&gt; simplyfied column?</t>
+  </si>
+  <si>
+    <t>n= 6</t>
+  </si>
+  <si>
+    <t>n= 11, doubles - spelling mistakes</t>
+  </si>
+  <si>
+    <t>n= 163</t>
+  </si>
+  <si>
+    <t>n= 162</t>
+  </si>
+  <si>
+    <t>n= 180</t>
+  </si>
+  <si>
+    <t>around 126 could be right</t>
+  </si>
+  <si>
+    <t>n= 62, because of inconsequent naming</t>
+  </si>
+  <si>
+    <t>n= 60, because of inceonsequent naming</t>
+  </si>
+  <si>
+    <t>amount of tree branching: 1, 2 or more</t>
+  </si>
+  <si>
+    <t>status of the stub after cutting the tree (test cut I guess)</t>
+  </si>
+  <si>
+    <t>n= 2703</t>
+  </si>
+  <si>
+    <t>n= 2838</t>
+  </si>
+  <si>
+    <t>n= 2500</t>
+  </si>
+  <si>
+    <t>not specifically checked so far, but could be fine, cause variability is expected</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">not availabe/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>probably not useable</t>
+    </r>
+  </si>
+  <si>
+    <t>n= 21319</t>
+  </si>
+  <si>
+    <t>n= 25474</t>
+  </si>
+  <si>
+    <t>n= 18343</t>
+  </si>
+  <si>
+    <t>n= 10</t>
+  </si>
+  <si>
+    <t>n= 11 ("NULL" and "Indeterminante" -&gt; can put them together)</t>
+  </si>
+  <si>
+    <t>Distance measured in meters from the center of the site to the intersection of the normal diameter and the central axis of the individual</t>
+  </si>
+  <si>
+    <t>n= 2667, NULL</t>
+  </si>
+  <si>
+    <t>n= 1275, 999991.00</t>
+  </si>
+  <si>
+    <t>there is duuplicates but shouldn't be relevant for data (except for checking)</t>
+  </si>
+  <si>
+    <t>n= 362 (class = "character")</t>
+  </si>
+  <si>
+    <t>n= 363 (2 values for NA)</t>
+  </si>
+  <si>
+    <t>n= 362 (360, 0, NA) + class numeric</t>
+  </si>
+  <si>
+    <t>Position measured in degrees from the center of the site to the intersection of the normal diameter and the central axis of the individual.</t>
+  </si>
+  <si>
+    <t>n= 412</t>
+  </si>
+  <si>
+    <t>n= 401</t>
+  </si>
+  <si>
+    <t>n= 1674</t>
+  </si>
+  <si>
+    <t>height in meters of the entire tree</t>
+  </si>
+  <si>
+    <t>height in meters from the base of the tree to the base of the canopy, i.e., the stem free of branches.</t>
+  </si>
+  <si>
+    <t>height in meters of the height of the trunk measured from the base of the tree to where it has a diameter of 10cm (only trees with a normal diameter greater than 10cm should be considered).</t>
+  </si>
+  <si>
+    <t>n= 1282 (999991.00 &amp; 999993.00)</t>
+  </si>
+  <si>
+    <t>n= 1186 (999991.00 &amp; 999993.00)</t>
+  </si>
+  <si>
+    <t>n= 1826 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 1646 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 1712 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 1384 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>Diameter in centimeters with tree bark at a height of 1.30 meters above the maximum slope of the surrounding terrain.</t>
+  </si>
+  <si>
+    <t>Measurement in metres of the vertical projection of the crown.</t>
+  </si>
+  <si>
+    <t>Tree diameter, measured at 30 cm from ground level and noted in centimetres.</t>
+  </si>
+  <si>
+    <t>n= 840</t>
+  </si>
+  <si>
+    <t>n= 714</t>
+  </si>
+  <si>
+    <t>n= 1282 (999993.00)</t>
+  </si>
+  <si>
+    <t>n= 1453 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 1448 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 1442 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 1250 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 1324 (999991.00 &amp; 999993.00)</t>
+  </si>
+  <si>
+    <t>n= 1032 (999991.00 &amp; 999993.00)</t>
+  </si>
+  <si>
+    <t>x coordinates</t>
+  </si>
+  <si>
+    <t>y coordinates</t>
+  </si>
+  <si>
+    <t>type of damage 1</t>
+  </si>
+  <si>
+    <t>severity of damage 1</t>
+  </si>
+  <si>
+    <t>type of damage 2</t>
+  </si>
+  <si>
+    <t>severity of damage 2</t>
+  </si>
+  <si>
+    <t>n= 2461 (NULL, Character)</t>
+  </si>
+  <si>
+    <t>n= 1447 (NULL, Character)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">categoric mistakes / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>single mistakes</t>
+    </r>
+  </si>
+  <si>
+    <t>n= 2599 (NULL, Character)</t>
+  </si>
+  <si>
+    <t>n= 1699 (NULL, Character)</t>
+  </si>
+  <si>
+    <t>missing values == NA, numeric</t>
+  </si>
+  <si>
+    <t>n= 2254 (999991.00 &amp; 9999993.00)</t>
+  </si>
+  <si>
+    <t>missing values == NA, numeric, m2</t>
+  </si>
+  <si>
+    <t>basal area in m2</t>
+  </si>
+  <si>
+    <t>crown area in m2</t>
+  </si>
+  <si>
+    <t>growth stage</t>
+  </si>
+  <si>
+    <t>n= 6 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 190 (999991.00 &amp; 999993.00)</t>
+  </si>
+  <si>
+    <t>n= 324 (NULL, 999, character)</t>
+  </si>
+  <si>
+    <t>n= 318 (NULL, 690?)</t>
+  </si>
+  <si>
+    <t>n= 4, no NA, same spelling across ds</t>
+  </si>
+  <si>
+    <t>n= 6, NA, same spelling across ds</t>
+  </si>
+  <si>
+    <t>n= 46 (NULL &amp; no aplica, spelling)</t>
+  </si>
+  <si>
+    <t>n= 41 (no definido)</t>
+  </si>
+  <si>
+    <t>missing values == NA, same spelling across ds</t>
+  </si>
+  <si>
+    <t>n= 30 (NULL, n/a, -9999, 05, "")</t>
+  </si>
+  <si>
+    <t>n= 27 (no aplica, no capturado)</t>
+  </si>
+  <si>
+    <t>n= 29 (NULL, n/a, -9999, 05, "", missing 85)</t>
+  </si>
+  <si>
+    <t>n= 25(no aplica, no capturado, missing 75, missing 95)</t>
+  </si>
+  <si>
+    <t>n= 39 (no definido, no capturado)</t>
+  </si>
+  <si>
+    <t>n= 42 (NULL &amp; no aplica, spelling)</t>
+  </si>
+  <si>
+    <t>radial length of the last 10 rings in millimeters.</t>
+  </si>
+  <si>
+    <t>Number of growth rings in the last 2.5cm of chip length.</t>
+  </si>
+  <si>
+    <t>hickness of the bark at the height of the normal diameter (1.30m) on the side of the tree pointing towards the center of the site in millimeters.</t>
+  </si>
+  <si>
+    <t>n= 79 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 98 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 130 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 52 (NULL)</t>
+  </si>
+  <si>
+    <t>Number of alive branches</t>
+  </si>
+  <si>
+    <t>n= 37 (NULL, 999, 9999)</t>
+  </si>
+  <si>
+    <t>n= 225 (999993, 2 weirdly high values 2134 &amp; 5357)</t>
+  </si>
+  <si>
+    <t>n= 124 (NULL, 999)</t>
+  </si>
+  <si>
+    <t>n= 151 (999991 &amp; 999993)</t>
+  </si>
+  <si>
+    <t>n= 117 (999991 &amp; 999993)</t>
+  </si>
+  <si>
+    <t>n= 104 (NULL, 999)</t>
+  </si>
+  <si>
+    <t>n= 84 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 92 (999991 &amp; 999993)</t>
+  </si>
+  <si>
+    <t>missing values == NA, integer</t>
+  </si>
+  <si>
+    <t>n= 60068 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 58436 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 64447 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 63193 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 9858</t>
+  </si>
+  <si>
+    <t>n= 9825</t>
+  </si>
+  <si>
+    <t>relative position of each tree in relation to the upper stratum.</t>
+  </si>
+  <si>
+    <t>Percentage of canopy branches, foliage and reproductive structures that block light passing through the canopy</t>
+  </si>
+  <si>
+    <t>Amount of light that the tree canopy lets through</t>
+  </si>
+  <si>
+    <t>light exposure</t>
+  </si>
+  <si>
+    <t>Estimate the severity of recent tree stress. Estimate this variable as a percentage of the live crown area, including the area with dieback.</t>
+  </si>
+  <si>
+    <t>n= 7 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 9 (No aplicacion = no aplica, no capturado + Posicion recta)</t>
+  </si>
+  <si>
+    <t>n= 8 (NULL)</t>
+  </si>
+  <si>
+    <t>n= 9 (No capturado, SI)</t>
+  </si>
+  <si>
+    <t>n= 8-9, NA, same spelling across ds</t>
+  </si>
+  <si>
+    <t>n= 7-8, NA, same spelling across ds</t>
+  </si>
+  <si>
+    <t>n= 22 (no capturado, sin parametro + ranges)</t>
+  </si>
+  <si>
+    <t>n= 25 (NULL, n/a, -9999, "" + specific values)</t>
+  </si>
+  <si>
+    <t>n= 21 (20 values + NA), ranges (not exact values)</t>
+  </si>
+  <si>
+    <t>n= 22 (42309, 44682, 44840 instead of 1-15, no capturado, sin parametro + ranges)</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>n= 1826 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1646 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1448 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1447 (NA, "numeric")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1254,8 +1897,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1322,8 +1987,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF38D8D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1340,11 +2035,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1378,12 +2183,127 @@
     <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF38D8D"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FF78C6DE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2239,7 +3159,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -2412,8 +3332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7AB688-5A0A-4572-BDE5-9C92B4B738E7}">
   <dimension ref="A4:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView topLeftCell="B17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2525,7 +3445,7 @@
       <c r="D9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>282</v>
       </c>
       <c r="F9" t="s">
@@ -2746,7 +3666,7 @@
         <v>235</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I22" s="22"/>
     </row>
@@ -2767,10 +3687,10 @@
         <v>234</v>
       </c>
       <c r="H23" s="22" t="s">
+        <v>385</v>
+      </c>
+      <c r="I23" s="22" t="s">
         <v>386</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2787,11 +3707,11 @@
         <v>356</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J24" s="22"/>
     </row>
@@ -2862,7 +3782,7 @@
         <v>302</v>
       </c>
       <c r="F29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2876,7 +3796,7 @@
         <v>303</v>
       </c>
       <c r="F30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -2926,7 +3846,7 @@
         <v>307</v>
       </c>
       <c r="F34" t="s">
-        <v>269</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.35">
@@ -3004,7 +3924,7 @@
         <v>313</v>
       </c>
       <c r="F40" t="s">
-        <v>275</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.35">
@@ -3018,7 +3938,7 @@
         <v>314</v>
       </c>
       <c r="F41" t="s">
-        <v>274</v>
+        <v>395</v>
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.35">
@@ -3119,7 +4039,7 @@
         <v>321</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G48" t="s">
         <v>373</v>
@@ -3230,7 +4150,7 @@
         <v>325</v>
       </c>
       <c r="F54" t="s">
-        <v>244</v>
+        <v>394</v>
       </c>
       <c r="G54" t="s">
         <v>359</v>
@@ -3258,7 +4178,7 @@
         <v>327</v>
       </c>
       <c r="F56" t="s">
-        <v>276</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.35">
@@ -3272,7 +4192,7 @@
         <v>328</v>
       </c>
       <c r="F57" t="s">
-        <v>277</v>
+        <v>393</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.35">
@@ -3406,7 +4326,7 @@
         <v>338</v>
       </c>
       <c r="F67" t="s">
-        <v>258</v>
+        <v>390</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.35">
@@ -3417,7 +4337,7 @@
         <v>339</v>
       </c>
       <c r="F68" t="s">
-        <v>257</v>
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.35">
@@ -3501,7 +4421,7 @@
         <v>346</v>
       </c>
       <c r="F77" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.35">
@@ -3520,7 +4440,7 @@
         <v>348</v>
       </c>
       <c r="F79" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.35">
@@ -3536,7 +4456,7 @@
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D85" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -3545,6 +4465,1960 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
+  <dimension ref="C1:P52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="26.36328125" customWidth="1"/>
+    <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
+    <col min="12" max="12" width="12.08984375" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="11.08984375" customWidth="1"/>
+    <col min="15" max="15" width="65.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I1" s="7"/>
+      <c r="J1" t="s">
+        <v>455</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I2" s="8"/>
+      <c r="J2" t="s">
+        <v>525</v>
+      </c>
+      <c r="N2" s="71"/>
+      <c r="O2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I3" s="6"/>
+      <c r="J3" t="s">
+        <v>479</v>
+      </c>
+      <c r="N3" s="43"/>
+      <c r="O3" s="101" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="G5" s="34"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="N5" s="28"/>
+      <c r="O5" s="38" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C6" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>401</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>401</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>401</v>
+      </c>
+      <c r="O6" s="39" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C7" s="29">
+        <v>1</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>435</v>
+      </c>
+      <c r="K7" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="M7" s="46" t="s">
+        <v>435</v>
+      </c>
+      <c r="N7" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C8" s="29">
+        <v>2</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="35" t="s">
+        <v>437</v>
+      </c>
+      <c r="J8" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="K8" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>419</v>
+      </c>
+      <c r="M8" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="N8" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="O8" s="40" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C9" s="29">
+        <v>3</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>279</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="46" t="s">
+        <v>406</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>445</v>
+      </c>
+      <c r="J9" s="61" t="s">
+        <v>445</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>445</v>
+      </c>
+      <c r="L9" s="41" t="s">
+        <v>445</v>
+      </c>
+      <c r="M9" s="61" t="s">
+        <v>445</v>
+      </c>
+      <c r="N9" s="61" t="s">
+        <v>445</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C10" s="29">
+        <v>4</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>294</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>420</v>
+      </c>
+      <c r="J10" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="L10" s="40" t="s">
+        <v>420</v>
+      </c>
+      <c r="M10" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="N10" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="O10" s="40" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C11" s="29">
+        <v>5</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>408</v>
+      </c>
+      <c r="J11" s="73" t="s">
+        <v>454</v>
+      </c>
+      <c r="K11" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="L11" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="M11" s="60" t="s">
+        <v>447</v>
+      </c>
+      <c r="N11" s="70" t="s">
+        <v>448</v>
+      </c>
+      <c r="O11" s="35" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C12" s="29">
+        <v>6</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>416</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>416</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>408</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>425</v>
+      </c>
+      <c r="H12" s="51" t="s">
+        <v>424</v>
+      </c>
+      <c r="I12" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="J12" s="94" t="s">
+        <v>417</v>
+      </c>
+      <c r="K12" s="64" t="s">
+        <v>408</v>
+      </c>
+      <c r="L12" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="M12" s="72" t="s">
+        <v>417</v>
+      </c>
+      <c r="N12" s="64" t="s">
+        <v>408</v>
+      </c>
+      <c r="O12" s="50" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C13" s="29">
+        <v>7</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>404</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>408</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>450</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>451</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>452</v>
+      </c>
+      <c r="L13" s="44" t="s">
+        <v>450</v>
+      </c>
+      <c r="M13" s="43" t="s">
+        <v>451</v>
+      </c>
+      <c r="N13" s="43" t="s">
+        <v>452</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>453</v>
+      </c>
+      <c r="P13" s="43" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C14" s="29">
+        <v>8</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>427</v>
+      </c>
+      <c r="H14" s="55"/>
+      <c r="I14" s="57" t="s">
+        <v>457</v>
+      </c>
+      <c r="J14" s="58" t="s">
+        <v>458</v>
+      </c>
+      <c r="K14" s="58" t="s">
+        <v>459</v>
+      </c>
+      <c r="L14" s="57" t="s">
+        <v>457</v>
+      </c>
+      <c r="M14" s="58" t="s">
+        <v>458</v>
+      </c>
+      <c r="N14" s="58" t="s">
+        <v>459</v>
+      </c>
+      <c r="O14" s="56" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C15" s="29">
+        <v>9</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>346</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>428</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52" t="s">
+        <v>471</v>
+      </c>
+      <c r="J15" s="47" t="s">
+        <v>472</v>
+      </c>
+      <c r="K15" s="53" t="s">
+        <v>459</v>
+      </c>
+      <c r="L15" s="52" t="s">
+        <v>471</v>
+      </c>
+      <c r="M15" s="47" t="s">
+        <v>472</v>
+      </c>
+      <c r="N15" s="53" t="s">
+        <v>459</v>
+      </c>
+      <c r="O15" s="50" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C16" s="29">
+        <v>10</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>473</v>
+      </c>
+      <c r="I16" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J16" s="58" t="s">
+        <v>460</v>
+      </c>
+      <c r="K16" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="L16" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M16" s="58" t="s">
+        <v>460</v>
+      </c>
+      <c r="N16" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="O16" s="67" t="s">
+        <v>463</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C17" s="29">
+        <v>11</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="H17" s="65" t="s">
+        <v>474</v>
+      </c>
+      <c r="I17" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J17" s="47" t="s">
+        <v>466</v>
+      </c>
+      <c r="K17" s="60" t="s">
+        <v>465</v>
+      </c>
+      <c r="L17" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M17" s="47" t="s">
+        <v>466</v>
+      </c>
+      <c r="N17" s="60" t="s">
+        <v>465</v>
+      </c>
+      <c r="O17" s="33" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C18" s="29">
+        <v>12</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" t="s">
+        <v>411</v>
+      </c>
+      <c r="I18" s="69" t="s">
+        <v>467</v>
+      </c>
+      <c r="J18" s="70" t="s">
+        <v>468</v>
+      </c>
+      <c r="K18" s="70" t="s">
+        <v>469</v>
+      </c>
+      <c r="L18" s="69" t="s">
+        <v>467</v>
+      </c>
+      <c r="M18" s="71" t="s">
+        <v>468</v>
+      </c>
+      <c r="N18" s="71" t="s">
+        <v>469</v>
+      </c>
+      <c r="O18" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C19" s="29">
+        <v>13</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>306</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="H19" t="s">
+        <v>412</v>
+      </c>
+      <c r="I19" s="69" t="s">
+        <v>475</v>
+      </c>
+      <c r="J19" s="70" t="s">
+        <v>476</v>
+      </c>
+      <c r="K19" s="70" t="s">
+        <v>477</v>
+      </c>
+      <c r="L19" s="69"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="71"/>
+      <c r="O19" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C20" s="29">
+        <v>14</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="H20" t="s">
+        <v>430</v>
+      </c>
+      <c r="I20" s="74" t="s">
+        <v>480</v>
+      </c>
+      <c r="J20" s="75" t="s">
+        <v>481</v>
+      </c>
+      <c r="K20" s="75" t="s">
+        <v>482</v>
+      </c>
+      <c r="L20" s="74" t="s">
+        <v>480</v>
+      </c>
+      <c r="M20" s="75" t="s">
+        <v>481</v>
+      </c>
+      <c r="N20" s="75" t="s">
+        <v>482</v>
+      </c>
+      <c r="O20" s="74" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C21" s="29">
+        <v>15</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>307</v>
+      </c>
+      <c r="G21" s="50" t="s">
+        <v>397</v>
+      </c>
+      <c r="H21" s="51" t="s">
+        <v>415</v>
+      </c>
+      <c r="I21" s="63" t="s">
+        <v>483</v>
+      </c>
+      <c r="J21" s="72" t="s">
+        <v>483</v>
+      </c>
+      <c r="K21" s="53" t="s">
+        <v>484</v>
+      </c>
+      <c r="L21" s="63" t="s">
+        <v>483</v>
+      </c>
+      <c r="M21" s="72" t="s">
+        <v>483</v>
+      </c>
+      <c r="N21" s="53" t="s">
+        <v>484</v>
+      </c>
+      <c r="O21" s="50" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C22" s="29">
+        <v>16</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="H22" t="s">
+        <v>485</v>
+      </c>
+      <c r="I22" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J22" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="K22" s="47" t="s">
+        <v>487</v>
+      </c>
+      <c r="L22" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M22" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="N22" s="47" t="s">
+        <v>487</v>
+      </c>
+      <c r="O22" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C23" s="29">
+        <v>17</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="H23" t="s">
+        <v>492</v>
+      </c>
+      <c r="I23" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J23" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="K23" s="47" t="s">
+        <v>490</v>
+      </c>
+      <c r="L23" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M23" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="N23" s="47" t="s">
+        <v>490</v>
+      </c>
+      <c r="O23" s="50" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C24" s="29">
+        <v>18</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="F24" s="76" t="s">
+        <v>314</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>395</v>
+      </c>
+      <c r="H24" s="55" t="s">
+        <v>496</v>
+      </c>
+      <c r="I24" s="77" t="s">
+        <v>493</v>
+      </c>
+      <c r="J24" s="78" t="s">
+        <v>494</v>
+      </c>
+      <c r="K24" s="58" t="s">
+        <v>495</v>
+      </c>
+      <c r="L24" s="77" t="s">
+        <v>493</v>
+      </c>
+      <c r="M24" s="78" t="s">
+        <v>494</v>
+      </c>
+      <c r="N24" s="58" t="s">
+        <v>495</v>
+      </c>
+      <c r="O24" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C25" s="29">
+        <v>19</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="F25" s="59" t="s">
+        <v>316</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>497</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>501</v>
+      </c>
+      <c r="J25" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="K25" s="47" t="s">
+        <v>500</v>
+      </c>
+      <c r="L25" s="102" t="s">
+        <v>588</v>
+      </c>
+      <c r="M25" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="N25" s="47" t="s">
+        <v>500</v>
+      </c>
+      <c r="O25" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C26" s="29">
+        <v>20</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>317</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>498</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>502</v>
+      </c>
+      <c r="J26" s="79" t="s">
+        <v>504</v>
+      </c>
+      <c r="K26" s="79" t="s">
+        <v>499</v>
+      </c>
+      <c r="L26" s="103" t="s">
+        <v>589</v>
+      </c>
+      <c r="M26" s="79" t="s">
+        <v>504</v>
+      </c>
+      <c r="N26" s="79" t="s">
+        <v>499</v>
+      </c>
+      <c r="O26" s="80" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C27" s="29">
+        <v>21</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>275</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>275</v>
+      </c>
+      <c r="F27" s="76" t="s">
+        <v>313</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>396</v>
+      </c>
+      <c r="H27" s="55" t="s">
+        <v>505</v>
+      </c>
+      <c r="I27" s="77" t="s">
+        <v>508</v>
+      </c>
+      <c r="J27" s="78" t="s">
+        <v>509</v>
+      </c>
+      <c r="K27" s="58" t="s">
+        <v>510</v>
+      </c>
+      <c r="L27" s="77" t="s">
+        <v>508</v>
+      </c>
+      <c r="M27" s="78" t="s">
+        <v>509</v>
+      </c>
+      <c r="N27" s="58" t="s">
+        <v>510</v>
+      </c>
+      <c r="O27" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C28" s="29">
+        <v>22</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="F28" s="59" t="s">
+        <v>336</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="H28" s="46" t="s">
+        <v>507</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>511</v>
+      </c>
+      <c r="J28" s="47" t="s">
+        <v>513</v>
+      </c>
+      <c r="K28" s="82" t="s">
+        <v>516</v>
+      </c>
+      <c r="L28" s="102" t="s">
+        <v>511</v>
+      </c>
+      <c r="M28" s="47" t="s">
+        <v>513</v>
+      </c>
+      <c r="N28" s="82" t="s">
+        <v>516</v>
+      </c>
+      <c r="O28" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C29" s="29">
+        <v>23</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="F29" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="G29" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="H29" s="51" t="s">
+        <v>506</v>
+      </c>
+      <c r="I29" s="52" t="s">
+        <v>512</v>
+      </c>
+      <c r="J29" s="53" t="s">
+        <v>514</v>
+      </c>
+      <c r="K29" s="81" t="s">
+        <v>515</v>
+      </c>
+      <c r="L29" s="104" t="s">
+        <v>590</v>
+      </c>
+      <c r="M29" s="53" t="s">
+        <v>514</v>
+      </c>
+      <c r="N29" s="81" t="s">
+        <v>515</v>
+      </c>
+      <c r="O29" s="80" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C30" s="29">
+        <v>24</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="F30" s="59" t="s">
+        <v>327</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="H30" s="65" t="s">
+        <v>531</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>523</v>
+      </c>
+      <c r="J30" s="47" t="s">
+        <v>526</v>
+      </c>
+      <c r="K30" s="95" t="s">
+        <v>529</v>
+      </c>
+      <c r="L30" s="102" t="s">
+        <v>523</v>
+      </c>
+      <c r="M30" s="47" t="s">
+        <v>526</v>
+      </c>
+      <c r="N30" s="95" t="s">
+        <v>529</v>
+      </c>
+      <c r="O30" s="67" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C31" s="29">
+        <v>25</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>328</v>
+      </c>
+      <c r="G31" s="50" t="s">
+        <v>393</v>
+      </c>
+      <c r="H31" s="51" t="s">
+        <v>532</v>
+      </c>
+      <c r="I31" s="52" t="s">
+        <v>524</v>
+      </c>
+      <c r="J31" s="53" t="s">
+        <v>527</v>
+      </c>
+      <c r="K31" s="96" t="s">
+        <v>515</v>
+      </c>
+      <c r="L31" s="103" t="s">
+        <v>591</v>
+      </c>
+      <c r="M31" s="53" t="s">
+        <v>527</v>
+      </c>
+      <c r="N31" s="96" t="s">
+        <v>515</v>
+      </c>
+      <c r="O31" s="80" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C32" s="29">
+        <v>26</v>
+      </c>
+      <c r="D32" s="83" t="s">
+        <v>246</v>
+      </c>
+      <c r="E32" s="83" t="s">
+        <v>246</v>
+      </c>
+      <c r="F32" s="84" t="s">
+        <v>370</v>
+      </c>
+      <c r="G32" s="85" t="s">
+        <v>246</v>
+      </c>
+      <c r="H32" s="86" t="s">
+        <v>572</v>
+      </c>
+      <c r="I32" s="100" t="s">
+        <v>461</v>
+      </c>
+      <c r="J32" s="58" t="s">
+        <v>577</v>
+      </c>
+      <c r="K32" s="58" t="s">
+        <v>578</v>
+      </c>
+      <c r="L32" s="100" t="s">
+        <v>461</v>
+      </c>
+      <c r="M32" s="58" t="s">
+        <v>577</v>
+      </c>
+      <c r="N32" s="58" t="s">
+        <v>578</v>
+      </c>
+      <c r="O32" s="56" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C33" s="29">
+        <v>27</v>
+      </c>
+      <c r="D33" s="87" t="s">
+        <v>248</v>
+      </c>
+      <c r="E33" s="87" t="s">
+        <v>248</v>
+      </c>
+      <c r="F33" s="88" t="s">
+        <v>371</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>364</v>
+      </c>
+      <c r="H33" s="89" t="s">
+        <v>575</v>
+      </c>
+      <c r="I33" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J33" s="47" t="s">
+        <v>579</v>
+      </c>
+      <c r="K33" s="47" t="s">
+        <v>580</v>
+      </c>
+      <c r="L33" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M33" s="47" t="s">
+        <v>579</v>
+      </c>
+      <c r="N33" s="47" t="s">
+        <v>580</v>
+      </c>
+      <c r="O33" s="33" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C34" s="29">
+        <v>28</v>
+      </c>
+      <c r="D34" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="E34" s="87" t="s">
+        <v>249</v>
+      </c>
+      <c r="F34" s="88" t="s">
+        <v>322</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H34" s="89" t="s">
+        <v>573</v>
+      </c>
+      <c r="I34" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J34" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="K34" s="47" t="s">
+        <v>583</v>
+      </c>
+      <c r="L34" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M34" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="N34" s="47" t="s">
+        <v>583</v>
+      </c>
+      <c r="O34" s="33" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C35" s="29">
+        <v>29</v>
+      </c>
+      <c r="D35" s="87" t="s">
+        <v>250</v>
+      </c>
+      <c r="E35" s="87" t="s">
+        <v>250</v>
+      </c>
+      <c r="F35" s="88" t="s">
+        <v>324</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="H35" s="89" t="s">
+        <v>574</v>
+      </c>
+      <c r="I35" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J35" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="K35" s="47" t="s">
+        <v>583</v>
+      </c>
+      <c r="L35" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M35" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="N35" s="47" t="s">
+        <v>583</v>
+      </c>
+      <c r="O35" s="33" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C36" s="29">
+        <v>30</v>
+      </c>
+      <c r="D36" s="90" t="s">
+        <v>251</v>
+      </c>
+      <c r="E36" s="90" t="s">
+        <v>251</v>
+      </c>
+      <c r="F36" s="91" t="s">
+        <v>323</v>
+      </c>
+      <c r="G36" s="92" t="s">
+        <v>251</v>
+      </c>
+      <c r="H36" s="93" t="s">
+        <v>576</v>
+      </c>
+      <c r="I36" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J36" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="K36" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="L36" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M36" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="N36" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="O36" s="50"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C37" s="29">
+        <v>31</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="H37" t="s">
+        <v>533</v>
+      </c>
+      <c r="I37" s="57" t="s">
+        <v>534</v>
+      </c>
+      <c r="J37" s="58" t="s">
+        <v>534</v>
+      </c>
+      <c r="K37" s="58" t="s">
+        <v>534</v>
+      </c>
+      <c r="L37" s="57" t="s">
+        <v>534</v>
+      </c>
+      <c r="M37" s="58" t="s">
+        <v>534</v>
+      </c>
+      <c r="N37" s="58" t="s">
+        <v>534</v>
+      </c>
+      <c r="O37" s="33" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C38" s="29">
+        <v>32</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>337</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="H38" t="s">
+        <v>429</v>
+      </c>
+      <c r="I38" s="35" t="s">
+        <v>537</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="L38" s="35" t="s">
+        <v>537</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="O38" s="67" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C39" s="29">
+        <v>33</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>309</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>367</v>
+      </c>
+      <c r="H39" s="46" t="s">
+        <v>431</v>
+      </c>
+      <c r="I39" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="J39" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="K39" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="L39" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="M39" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="N39" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="O39" s="33" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C40" s="29">
+        <v>34</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="E40" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="F40" s="59" t="s">
+        <v>329</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="H40" t="s">
+        <v>519</v>
+      </c>
+      <c r="I40" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J40" s="47" t="s">
+        <v>540</v>
+      </c>
+      <c r="K40" s="47" t="s">
+        <v>541</v>
+      </c>
+      <c r="L40" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M40" s="47" t="s">
+        <v>540</v>
+      </c>
+      <c r="N40" s="47" t="s">
+        <v>541</v>
+      </c>
+      <c r="O40" s="67" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C41" s="29">
+        <v>35</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="E41" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="F41" s="59" t="s">
+        <v>331</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="H41" s="46" t="s">
+        <v>520</v>
+      </c>
+      <c r="I41" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J41" s="47" t="s">
+        <v>543</v>
+      </c>
+      <c r="K41" s="47" t="s">
+        <v>544</v>
+      </c>
+      <c r="L41" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>543</v>
+      </c>
+      <c r="N41" s="47" t="s">
+        <v>544</v>
+      </c>
+      <c r="O41" s="67" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C42" s="29">
+        <v>36</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="E42" s="45" t="s">
+        <v>422</v>
+      </c>
+      <c r="F42" s="59" t="s">
+        <v>332</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="H42" t="s">
+        <v>521</v>
+      </c>
+      <c r="I42" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="J42" s="47" t="s">
+        <v>548</v>
+      </c>
+      <c r="K42" s="47" t="s">
+        <v>547</v>
+      </c>
+      <c r="L42" s="66" t="s">
+        <v>461</v>
+      </c>
+      <c r="M42" s="47" t="s">
+        <v>548</v>
+      </c>
+      <c r="N42" s="47" t="s">
+        <v>547</v>
+      </c>
+      <c r="O42" s="67" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C43" s="29">
+        <v>37</v>
+      </c>
+      <c r="D43" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="E43" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="F43" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="G43" s="50" t="s">
+        <v>361</v>
+      </c>
+      <c r="H43" s="46" t="s">
+        <v>522</v>
+      </c>
+      <c r="I43" s="97" t="s">
+        <v>461</v>
+      </c>
+      <c r="J43" s="53" t="s">
+        <v>545</v>
+      </c>
+      <c r="K43" s="53" t="s">
+        <v>546</v>
+      </c>
+      <c r="L43" s="97" t="s">
+        <v>461</v>
+      </c>
+      <c r="M43" s="53" t="s">
+        <v>545</v>
+      </c>
+      <c r="N43" s="53" t="s">
+        <v>546</v>
+      </c>
+      <c r="O43" s="80" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C44" s="29">
+        <v>38</v>
+      </c>
+      <c r="D44" s="83" t="s">
+        <v>236</v>
+      </c>
+      <c r="E44" s="83" t="s">
+        <v>236</v>
+      </c>
+      <c r="F44" s="86" t="s">
+        <v>426</v>
+      </c>
+      <c r="G44" s="85" t="s">
+        <v>236</v>
+      </c>
+      <c r="H44" s="86" t="s">
+        <v>556</v>
+      </c>
+      <c r="I44" s="57" t="s">
+        <v>555</v>
+      </c>
+      <c r="J44" s="58" t="s">
+        <v>557</v>
+      </c>
+      <c r="K44" s="58" t="s">
+        <v>558</v>
+      </c>
+      <c r="L44" s="57" t="s">
+        <v>555</v>
+      </c>
+      <c r="M44" s="58" t="s">
+        <v>557</v>
+      </c>
+      <c r="N44" s="58" t="s">
+        <v>558</v>
+      </c>
+      <c r="O44" s="67" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C45" s="29">
+        <v>39</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="E45" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="F45" s="59" t="s">
+        <v>339</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="H45" s="46" t="s">
+        <v>549</v>
+      </c>
+      <c r="I45" s="35" t="s">
+        <v>554</v>
+      </c>
+      <c r="J45" s="47" t="s">
+        <v>559</v>
+      </c>
+      <c r="K45" s="47" t="s">
+        <v>560</v>
+      </c>
+      <c r="L45" s="35" t="s">
+        <v>554</v>
+      </c>
+      <c r="M45" s="47" t="s">
+        <v>559</v>
+      </c>
+      <c r="N45" s="47" t="s">
+        <v>560</v>
+      </c>
+      <c r="O45" s="67" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C46" s="29">
+        <v>40</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="E46" s="45" t="s">
+        <v>421</v>
+      </c>
+      <c r="F46" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>390</v>
+      </c>
+      <c r="H46" s="46" t="s">
+        <v>550</v>
+      </c>
+      <c r="I46" s="35" t="s">
+        <v>553</v>
+      </c>
+      <c r="J46" s="47" t="s">
+        <v>562</v>
+      </c>
+      <c r="K46" s="47" t="s">
+        <v>561</v>
+      </c>
+      <c r="L46" s="35" t="s">
+        <v>553</v>
+      </c>
+      <c r="M46" s="47" t="s">
+        <v>562</v>
+      </c>
+      <c r="N46" s="47" t="s">
+        <v>561</v>
+      </c>
+      <c r="O46" s="67" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C47" s="29">
+        <v>41</v>
+      </c>
+      <c r="D47" s="48" t="s">
+        <v>256</v>
+      </c>
+      <c r="E47" s="48" t="s">
+        <v>256</v>
+      </c>
+      <c r="F47" s="49" t="s">
+        <v>340</v>
+      </c>
+      <c r="G47" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="H47" s="51" t="s">
+        <v>551</v>
+      </c>
+      <c r="I47" s="52" t="s">
+        <v>552</v>
+      </c>
+      <c r="J47" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="K47" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="L47" s="52" t="s">
+        <v>552</v>
+      </c>
+      <c r="M47" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="N47" s="53" t="s">
+        <v>564</v>
+      </c>
+      <c r="O47" s="80" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C48" s="29">
+        <v>42</v>
+      </c>
+      <c r="D48" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="55" t="s">
+        <v>517</v>
+      </c>
+      <c r="I48" s="57" t="s">
+        <v>566</v>
+      </c>
+      <c r="J48" s="58" t="s">
+        <v>568</v>
+      </c>
+      <c r="K48" s="98" t="s">
+        <v>570</v>
+      </c>
+      <c r="L48" s="57" t="s">
+        <v>566</v>
+      </c>
+      <c r="M48" s="58" t="s">
+        <v>568</v>
+      </c>
+      <c r="N48" s="98" t="s">
+        <v>570</v>
+      </c>
+      <c r="O48" s="56" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C49" s="29">
+        <v>43</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="51" t="s">
+        <v>518</v>
+      </c>
+      <c r="I49" s="52" t="s">
+        <v>567</v>
+      </c>
+      <c r="J49" s="53" t="s">
+        <v>569</v>
+      </c>
+      <c r="K49" s="99" t="s">
+        <v>571</v>
+      </c>
+      <c r="L49" s="52" t="s">
+        <v>567</v>
+      </c>
+      <c r="M49" s="53" t="s">
+        <v>569</v>
+      </c>
+      <c r="N49" s="99" t="s">
+        <v>571</v>
+      </c>
+      <c r="O49" s="50" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C50" s="29">
+        <v>44</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="I50" s="66" t="s">
+        <v>432</v>
+      </c>
+      <c r="J50" s="6"/>
+      <c r="K50" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="L50" s="66" t="s">
+        <v>432</v>
+      </c>
+      <c r="M50" s="6"/>
+      <c r="N50" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="O50" s="33" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C51" s="29">
+        <v>45</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="I51" s="66" t="s">
+        <v>412</v>
+      </c>
+      <c r="J51" s="6"/>
+      <c r="K51" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="L51" s="66" t="s">
+        <v>412</v>
+      </c>
+      <c r="M51" s="6"/>
+      <c r="N51" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="O51" s="33" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="I52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="O52" s="33"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696B9836-61FA-4244-9D1D-68BEE2D396B9}">
   <dimension ref="A1:E35"/>
   <sheetViews>

</xml_diff>

<commit_message>
added cleaning of several variables of Arb.04 + updated Summary
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF768DE-B05D-4FF3-A3B2-3D7D9265E364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629FA9C3-7B01-480F-94BF-9B6AFBAE72A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="604">
   <si>
     <t>Variable</t>
   </si>
@@ -1531,9 +1531,6 @@
     <t>n= 1275, 999991.00</t>
   </si>
   <si>
-    <t>there is duuplicates but shouldn't be relevant for data (except for checking)</t>
-  </si>
-  <si>
     <t>n= 362 (class = "character")</t>
   </si>
   <si>
@@ -1600,12 +1597,6 @@
     <t>n= 1282 (999993.00)</t>
   </si>
   <si>
-    <t>n= 1453 (NULL)</t>
-  </si>
-  <si>
-    <t>n= 1448 (NULL)</t>
-  </si>
-  <si>
     <t>n= 1442 (NULL)</t>
   </si>
   <si>
@@ -1634,12 +1625,6 @@
   </si>
   <si>
     <t>severity of damage 2</t>
-  </si>
-  <si>
-    <t>n= 2461 (NULL, Character)</t>
-  </si>
-  <si>
-    <t>n= 1447 (NULL, Character)</t>
   </si>
   <si>
     <r>
@@ -1691,9 +1676,6 @@
     <t>n= 324 (NULL, 999, character)</t>
   </si>
   <si>
-    <t>n= 318 (NULL, 690?)</t>
-  </si>
-  <si>
     <t>n= 4, no NA, same spelling across ds</t>
   </si>
   <si>
@@ -1736,18 +1718,6 @@
     <t>hickness of the bark at the height of the normal diameter (1.30m) on the side of the tree pointing towards the center of the site in millimeters.</t>
   </si>
   <si>
-    <t>n= 79 (NULL)</t>
-  </si>
-  <si>
-    <t>n= 98 (NULL)</t>
-  </si>
-  <si>
-    <t>n= 130 (NULL)</t>
-  </si>
-  <si>
-    <t>n= 52 (NULL)</t>
-  </si>
-  <si>
     <t>Number of alive branches</t>
   </si>
   <si>
@@ -1775,9 +1745,6 @@
     <t>n= 92 (999991 &amp; 999993)</t>
   </si>
   <si>
-    <t>missing values == NA, integer</t>
-  </si>
-  <si>
     <t>n= 60068 (NULL)</t>
   </si>
   <si>
@@ -1854,6 +1821,75 @@
   </si>
   <si>
     <t>n= 1447 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1453 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 2461 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 2461 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 1447 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 1448 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 1453 (NULL, 2character")</t>
+  </si>
+  <si>
+    <t>might need leading zeros</t>
+  </si>
+  <si>
+    <t>might need leading zeros for T</t>
+  </si>
+  <si>
+    <t>there is duplicates but shouldn't be relevant for data (except for checking)</t>
+  </si>
+  <si>
+    <t>n= 6, NA or "no capturado", same spelling across ds</t>
+  </si>
+  <si>
+    <t>n= 6 (no capturado)</t>
+  </si>
+  <si>
+    <t>n= 251 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 52 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 318 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 52 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 130 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 130 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 98 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 98 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>n= 79 (NULL, "character")</t>
+  </si>
+  <si>
+    <t>missing values == NA, numeric (rounded)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing values == NA, numeric </t>
+  </si>
+  <si>
+    <t>n= 79 (NA, "numeric")</t>
   </si>
 </sst>
 </file>
@@ -2018,7 +2054,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -2145,11 +2181,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2217,11 +2290,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2237,48 +2305,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2288,9 +2341,20 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4468,8 +4532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4493,7 +4557,7 @@
       <c r="J1" t="s">
         <v>455</v>
       </c>
-      <c r="N1" s="68"/>
+      <c r="N1" s="61"/>
       <c r="O1" t="s">
         <v>462</v>
       </c>
@@ -4501,9 +4565,9 @@
     <row r="2" spans="3:16" x14ac:dyDescent="0.35">
       <c r="I2" s="8"/>
       <c r="J2" t="s">
-        <v>525</v>
-      </c>
-      <c r="N2" s="71"/>
+        <v>520</v>
+      </c>
+      <c r="N2" s="63"/>
       <c r="O2" t="s">
         <v>478</v>
       </c>
@@ -4514,8 +4578,8 @@
         <v>479</v>
       </c>
       <c r="N3" s="43"/>
-      <c r="O3" s="101" t="s">
-        <v>587</v>
+      <c r="O3" s="87" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.35">
@@ -4548,7 +4612,7 @@
       <c r="F6" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="89" t="s">
         <v>402</v>
       </c>
       <c r="H6" s="28" t="s">
@@ -4580,37 +4644,37 @@
       <c r="C7" s="29">
         <v>1</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" t="s">
         <v>71</v>
       </c>
       <c r="I7" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="J7" s="46" t="s">
+      <c r="J7" t="s">
         <v>435</v>
       </c>
-      <c r="K7" s="46" t="s">
+      <c r="K7" t="s">
         <v>436</v>
       </c>
       <c r="L7" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="M7" s="46" t="s">
+      <c r="M7" t="s">
         <v>435</v>
       </c>
-      <c r="N7" s="46" t="s">
+      <c r="N7" t="s">
         <v>436</v>
       </c>
       <c r="O7" s="33" t="s">
@@ -4621,37 +4685,37 @@
       <c r="C8" s="29">
         <v>2</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" t="s">
         <v>73</v>
       </c>
       <c r="I8" s="35" t="s">
         <v>437</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="K8" s="60" t="s">
+      <c r="K8" s="7" t="s">
         <v>419</v>
       </c>
       <c r="L8" s="40" t="s">
         <v>419</v>
       </c>
-      <c r="M8" s="60" t="s">
+      <c r="M8" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="N8" s="60" t="s">
+      <c r="N8" s="7" t="s">
         <v>419</v>
       </c>
       <c r="O8" s="40" t="s">
@@ -4662,37 +4726,37 @@
       <c r="C9" s="29">
         <v>3</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" t="s">
         <v>406</v>
       </c>
       <c r="I9" s="41" t="s">
         <v>445</v>
       </c>
-      <c r="J9" s="61" t="s">
+      <c r="J9" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="K9" s="61" t="s">
+      <c r="K9" s="56" t="s">
         <v>445</v>
       </c>
       <c r="L9" s="41" t="s">
         <v>445</v>
       </c>
-      <c r="M9" s="61" t="s">
+      <c r="M9" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="N9" s="61" t="s">
+      <c r="N9" s="56" t="s">
         <v>445</v>
       </c>
       <c r="O9" s="41" t="s">
@@ -4703,37 +4767,37 @@
       <c r="C10" s="29">
         <v>4</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="90" t="s">
         <v>233</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" t="s">
         <v>405</v>
       </c>
       <c r="I10" s="40" t="s">
         <v>420</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="7" t="s">
         <v>444</v>
       </c>
       <c r="L10" s="40" t="s">
         <v>420</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="7" t="s">
         <v>420</v>
       </c>
       <c r="O10" s="40" t="s">
@@ -4744,82 +4808,88 @@
       <c r="C11" s="29">
         <v>5</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="91" t="s">
         <v>234</v>
       </c>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="8" t="s">
         <v>407</v>
       </c>
       <c r="I11" s="35" t="s">
         <v>408</v>
       </c>
-      <c r="J11" s="73" t="s">
+      <c r="J11" s="65" t="s">
         <v>454</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="7" t="s">
         <v>448</v>
       </c>
       <c r="L11" s="40" t="s">
         <v>446</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="M11" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="N11" s="70" t="s">
+      <c r="N11" s="63" t="s">
         <v>448</v>
       </c>
       <c r="O11" s="35" t="s">
         <v>449</v>
+      </c>
+      <c r="P11" s="88" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C12" s="29">
         <v>6</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="48" t="s">
         <v>416</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="48" t="s">
         <v>416</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="92" t="s">
         <v>425</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="48" t="s">
         <v>424</v>
       </c>
-      <c r="I12" s="63" t="s">
+      <c r="I12" s="57" t="s">
         <v>417</v>
       </c>
-      <c r="J12" s="94" t="s">
+      <c r="J12" s="80" t="s">
         <v>417</v>
       </c>
-      <c r="K12" s="64" t="s">
+      <c r="K12" s="58" t="s">
         <v>408</v>
       </c>
-      <c r="L12" s="63" t="s">
+      <c r="L12" s="57" t="s">
         <v>417</v>
       </c>
-      <c r="M12" s="72" t="s">
+      <c r="M12" s="64" t="s">
         <v>417</v>
       </c>
-      <c r="N12" s="64" t="s">
+      <c r="N12" s="58" t="s">
         <v>408</v>
       </c>
-      <c r="O12" s="50" t="s">
+      <c r="O12" s="47" t="s">
         <v>417</v>
+      </c>
+      <c r="P12" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.35">
@@ -4835,7 +4905,7 @@
       <c r="F13" s="43" t="s">
         <v>404</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="93" t="s">
         <v>235</v>
       </c>
       <c r="H13" s="43" t="s">
@@ -4870,38 +4940,38 @@
       <c r="C14" s="29">
         <v>8</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="94" t="s">
         <v>427</v>
       </c>
-      <c r="H14" s="55"/>
-      <c r="I14" s="57" t="s">
+      <c r="H14" s="52"/>
+      <c r="I14" s="54" t="s">
         <v>457</v>
       </c>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="55" t="s">
         <v>458</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="55" t="s">
         <v>459</v>
       </c>
-      <c r="L14" s="57" t="s">
+      <c r="L14" s="54" t="s">
         <v>457</v>
       </c>
-      <c r="M14" s="58" t="s">
+      <c r="M14" s="55" t="s">
         <v>458</v>
       </c>
-      <c r="N14" s="58" t="s">
+      <c r="N14" s="55" t="s">
         <v>459</v>
       </c>
-      <c r="O14" s="56" t="s">
+      <c r="O14" s="53" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4909,38 +4979,38 @@
       <c r="C15" s="29">
         <v>9</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="G15" s="50" t="s">
+      <c r="G15" s="92" t="s">
         <v>428</v>
       </c>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52" t="s">
+      <c r="H15" s="48"/>
+      <c r="I15" s="49" t="s">
         <v>471</v>
       </c>
-      <c r="J15" s="47" t="s">
+      <c r="J15" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="K15" s="53" t="s">
+      <c r="K15" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="49" t="s">
         <v>471</v>
       </c>
-      <c r="M15" s="47" t="s">
+      <c r="M15" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="N15" s="53" t="s">
+      <c r="N15" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="O15" s="50" t="s">
+      <c r="O15" s="47" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4957,31 +5027,31 @@
       <c r="F16" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="90" t="s">
         <v>237</v>
       </c>
-      <c r="H16" s="65" t="s">
+      <c r="H16" t="s">
         <v>473</v>
       </c>
-      <c r="I16" s="66" t="s">
+      <c r="I16" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J16" s="58" t="s">
+      <c r="J16" s="55" t="s">
         <v>460</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="K16" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="L16" s="66" t="s">
+      <c r="L16" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M16" s="58" t="s">
+      <c r="M16" s="55" t="s">
         <v>460</v>
       </c>
-      <c r="N16" s="60" t="s">
+      <c r="N16" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="O16" s="67" t="s">
+      <c r="O16" s="60" t="s">
         <v>463</v>
       </c>
       <c r="P16" s="14" t="s">
@@ -5001,32 +5071,32 @@
       <c r="F17" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="90" t="s">
         <v>238</v>
       </c>
-      <c r="H17" s="65" t="s">
+      <c r="H17" t="s">
         <v>474</v>
       </c>
-      <c r="I17" s="66" t="s">
+      <c r="I17" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="K17" s="60" t="s">
+      <c r="K17" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="L17" s="66" t="s">
+      <c r="L17" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M17" s="47" t="s">
+      <c r="M17" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="N17" s="60" t="s">
+      <c r="N17" s="7" t="s">
         <v>465</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
@@ -5042,32 +5112,32 @@
       <c r="F18" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="90" t="s">
         <v>239</v>
       </c>
       <c r="H18" t="s">
         <v>411</v>
       </c>
-      <c r="I18" s="69" t="s">
+      <c r="I18" s="62" t="s">
         <v>467</v>
       </c>
-      <c r="J18" s="70" t="s">
+      <c r="J18" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="K18" s="70" t="s">
+      <c r="K18" s="63" t="s">
         <v>469</v>
       </c>
-      <c r="L18" s="69" t="s">
+      <c r="L18" s="62" t="s">
         <v>467</v>
       </c>
-      <c r="M18" s="71" t="s">
+      <c r="M18" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="N18" s="71" t="s">
+      <c r="N18" s="63" t="s">
         <v>469</v>
       </c>
-      <c r="O18" s="67" t="s">
-        <v>528</v>
+      <c r="O18" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
@@ -5083,26 +5153,26 @@
       <c r="F19" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="90" t="s">
         <v>240</v>
       </c>
       <c r="H19" t="s">
         <v>412</v>
       </c>
-      <c r="I19" s="69" t="s">
+      <c r="I19" s="62" t="s">
         <v>475</v>
       </c>
-      <c r="J19" s="70" t="s">
+      <c r="J19" s="63" t="s">
         <v>476</v>
       </c>
-      <c r="K19" s="70" t="s">
+      <c r="K19" s="63" t="s">
         <v>477</v>
       </c>
-      <c r="L19" s="69"/>
-      <c r="M19" s="71"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="67" t="s">
-        <v>528</v>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
@@ -5118,72 +5188,72 @@
       <c r="F20" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="90" t="s">
         <v>363</v>
       </c>
       <c r="H20" t="s">
         <v>430</v>
       </c>
-      <c r="I20" s="74" t="s">
+      <c r="I20" s="66" t="s">
         <v>480</v>
       </c>
-      <c r="J20" s="75" t="s">
+      <c r="J20" s="67" t="s">
         <v>481</v>
       </c>
-      <c r="K20" s="75" t="s">
+      <c r="K20" s="67" t="s">
         <v>482</v>
       </c>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="66" t="s">
         <v>480</v>
       </c>
-      <c r="M20" s="75" t="s">
+      <c r="M20" s="67" t="s">
         <v>481</v>
       </c>
-      <c r="N20" s="75" t="s">
+      <c r="N20" s="67" t="s">
         <v>482</v>
       </c>
-      <c r="O20" s="74" t="s">
-        <v>488</v>
+      <c r="O20" s="66" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C21" s="29">
         <v>15</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="45" t="s">
         <v>269</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="92" t="s">
         <v>397</v>
       </c>
-      <c r="H21" s="51" t="s">
+      <c r="H21" s="48" t="s">
         <v>415</v>
       </c>
-      <c r="I21" s="63" t="s">
+      <c r="I21" s="57" t="s">
         <v>483</v>
       </c>
-      <c r="J21" s="72" t="s">
+      <c r="J21" s="64" t="s">
         <v>483</v>
       </c>
-      <c r="K21" s="53" t="s">
+      <c r="K21" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="L21" s="63" t="s">
+      <c r="L21" s="57" t="s">
         <v>483</v>
       </c>
-      <c r="M21" s="72" t="s">
+      <c r="M21" s="64" t="s">
         <v>483</v>
       </c>
-      <c r="N21" s="53" t="s">
+      <c r="N21" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="O21" s="50" t="s">
+      <c r="O21" s="47" t="s">
         <v>483</v>
       </c>
     </row>
@@ -5200,32 +5270,32 @@
       <c r="F22" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="90" t="s">
         <v>362</v>
       </c>
       <c r="H22" t="s">
         <v>485</v>
       </c>
-      <c r="I22" s="66" t="s">
+      <c r="I22" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J22" s="47" t="s">
+      <c r="J22" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="K22" s="47" t="s">
+      <c r="K22" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="L22" s="66" t="s">
+      <c r="L22" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M22" s="47" t="s">
+      <c r="M22" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="N22" s="47" t="s">
+      <c r="N22" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="O22" s="67" t="s">
-        <v>528</v>
+      <c r="O22" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.35">
@@ -5241,564 +5311,564 @@
       <c r="F23" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="90" t="s">
         <v>253</v>
       </c>
       <c r="H23" t="s">
-        <v>492</v>
-      </c>
-      <c r="I23" s="66" t="s">
+        <v>491</v>
+      </c>
+      <c r="I23" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="K23" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="K23" s="47" t="s">
+      <c r="L23" s="59" t="s">
+        <v>461</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="O23" s="47" t="s">
         <v>490</v>
-      </c>
-      <c r="L23" s="66" t="s">
-        <v>461</v>
-      </c>
-      <c r="M23" s="47" t="s">
-        <v>489</v>
-      </c>
-      <c r="N23" s="47" t="s">
-        <v>490</v>
-      </c>
-      <c r="O23" s="50" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C24" s="29">
         <v>18</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="51" t="s">
         <v>274</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="51" t="s">
         <v>274</v>
       </c>
-      <c r="F24" s="76" t="s">
+      <c r="F24" s="68" t="s">
         <v>314</v>
       </c>
-      <c r="G24" s="56" t="s">
+      <c r="G24" s="94" t="s">
         <v>395</v>
       </c>
-      <c r="H24" s="55" t="s">
-        <v>496</v>
-      </c>
-      <c r="I24" s="77" t="s">
+      <c r="H24" s="52" t="s">
+        <v>495</v>
+      </c>
+      <c r="I24" s="69" t="s">
+        <v>492</v>
+      </c>
+      <c r="J24" s="70" t="s">
         <v>493</v>
       </c>
-      <c r="J24" s="78" t="s">
+      <c r="K24" s="55" t="s">
         <v>494</v>
       </c>
-      <c r="K24" s="58" t="s">
-        <v>495</v>
-      </c>
-      <c r="L24" s="77" t="s">
+      <c r="L24" s="98" t="s">
+        <v>492</v>
+      </c>
+      <c r="M24" s="70" t="s">
         <v>493</v>
       </c>
-      <c r="M24" s="78" t="s">
+      <c r="N24" s="55" t="s">
         <v>494</v>
       </c>
-      <c r="N24" s="58" t="s">
-        <v>495</v>
-      </c>
-      <c r="O24" s="67" t="s">
-        <v>528</v>
+      <c r="O24" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C25" s="29">
         <v>19</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="F25" s="59" t="s">
+      <c r="F25" s="31" t="s">
         <v>316</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="90" t="s">
         <v>267</v>
       </c>
-      <c r="H25" s="46" t="s">
-        <v>497</v>
+      <c r="H25" t="s">
+        <v>496</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>501</v>
-      </c>
-      <c r="J25" s="47" t="s">
-        <v>503</v>
-      </c>
-      <c r="K25" s="47" t="s">
         <v>500</v>
       </c>
-      <c r="L25" s="102" t="s">
-        <v>588</v>
-      </c>
-      <c r="M25" s="47" t="s">
-        <v>503</v>
-      </c>
-      <c r="N25" s="47" t="s">
-        <v>500</v>
-      </c>
-      <c r="O25" s="67" t="s">
-        <v>528</v>
+      <c r="J25" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="L25" s="99" t="s">
+        <v>577</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="O25" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C26" s="29">
         <v>20</v>
       </c>
-      <c r="D26" s="48" t="s">
+      <c r="D26" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="46" t="s">
         <v>317</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="92" t="s">
         <v>268</v>
       </c>
-      <c r="H26" s="51" t="s">
+      <c r="H26" s="48" t="s">
+        <v>497</v>
+      </c>
+      <c r="I26" s="49" t="s">
+        <v>501</v>
+      </c>
+      <c r="J26" s="71" t="s">
+        <v>503</v>
+      </c>
+      <c r="K26" s="71" t="s">
         <v>498</v>
       </c>
-      <c r="I26" s="52" t="s">
-        <v>502</v>
-      </c>
-      <c r="J26" s="79" t="s">
-        <v>504</v>
-      </c>
-      <c r="K26" s="79" t="s">
-        <v>499</v>
-      </c>
-      <c r="L26" s="103" t="s">
-        <v>589</v>
-      </c>
-      <c r="M26" s="79" t="s">
-        <v>504</v>
-      </c>
-      <c r="N26" s="79" t="s">
-        <v>499</v>
-      </c>
-      <c r="O26" s="80" t="s">
-        <v>528</v>
+      <c r="L26" s="100" t="s">
+        <v>578</v>
+      </c>
+      <c r="M26" s="71" t="s">
+        <v>503</v>
+      </c>
+      <c r="N26" s="71" t="s">
+        <v>498</v>
+      </c>
+      <c r="O26" s="72" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C27" s="29">
         <v>21</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="51" t="s">
         <v>275</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="51" t="s">
         <v>275</v>
       </c>
-      <c r="F27" s="76" t="s">
+      <c r="F27" s="68" t="s">
         <v>313</v>
       </c>
-      <c r="G27" s="56" t="s">
+      <c r="G27" s="94" t="s">
         <v>396</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>505</v>
-      </c>
-      <c r="I27" s="77" t="s">
+      <c r="H27" s="52" t="s">
+        <v>504</v>
+      </c>
+      <c r="I27" s="69" t="s">
+        <v>507</v>
+      </c>
+      <c r="J27" s="70" t="s">
         <v>508</v>
       </c>
-      <c r="J27" s="78" t="s">
+      <c r="K27" s="55" t="s">
         <v>509</v>
       </c>
-      <c r="K27" s="58" t="s">
-        <v>510</v>
-      </c>
-      <c r="L27" s="77" t="s">
+      <c r="L27" s="98" t="s">
+        <v>507</v>
+      </c>
+      <c r="M27" s="70" t="s">
         <v>508</v>
       </c>
-      <c r="M27" s="78" t="s">
+      <c r="N27" s="55" t="s">
         <v>509</v>
       </c>
-      <c r="N27" s="58" t="s">
-        <v>510</v>
-      </c>
-      <c r="O27" s="67" t="s">
-        <v>528</v>
+      <c r="O27" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C28" s="29">
         <v>22</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="F28" s="59" t="s">
+      <c r="F28" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="H28" s="46" t="s">
-        <v>507</v>
+      <c r="H28" t="s">
+        <v>506</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>511</v>
-      </c>
-      <c r="J28" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="K28" s="17" t="s">
         <v>513</v>
       </c>
-      <c r="K28" s="82" t="s">
-        <v>516</v>
-      </c>
-      <c r="L28" s="102" t="s">
-        <v>511</v>
-      </c>
-      <c r="M28" s="47" t="s">
+      <c r="L28" s="99" t="s">
+        <v>581</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="N28" s="17" t="s">
         <v>513</v>
       </c>
-      <c r="N28" s="82" t="s">
-        <v>516</v>
-      </c>
-      <c r="O28" s="67" t="s">
-        <v>528</v>
+      <c r="O28" s="60" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C29" s="29">
         <v>23</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="F29" s="49" t="s">
+      <c r="F29" s="46" t="s">
         <v>320</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G29" s="92" t="s">
         <v>245</v>
       </c>
-      <c r="H29" s="51" t="s">
-        <v>506</v>
-      </c>
-      <c r="I29" s="52" t="s">
+      <c r="H29" s="48" t="s">
+        <v>505</v>
+      </c>
+      <c r="I29" s="49" t="s">
+        <v>585</v>
+      </c>
+      <c r="J29" s="50" t="s">
+        <v>511</v>
+      </c>
+      <c r="K29" s="73" t="s">
         <v>512</v>
       </c>
-      <c r="J29" s="53" t="s">
-        <v>514</v>
-      </c>
-      <c r="K29" s="81" t="s">
-        <v>515</v>
-      </c>
-      <c r="L29" s="104" t="s">
-        <v>590</v>
-      </c>
-      <c r="M29" s="53" t="s">
-        <v>514</v>
-      </c>
-      <c r="N29" s="81" t="s">
-        <v>515</v>
-      </c>
-      <c r="O29" s="80" t="s">
-        <v>528</v>
+      <c r="L29" s="101" t="s">
+        <v>579</v>
+      </c>
+      <c r="M29" s="50" t="s">
+        <v>511</v>
+      </c>
+      <c r="N29" s="73" t="s">
+        <v>512</v>
+      </c>
+      <c r="O29" s="72" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C30" s="29">
         <v>24</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="F30" s="59" t="s">
+      <c r="F30" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="G30" s="33" t="s">
+      <c r="G30" s="90" t="s">
         <v>392</v>
       </c>
-      <c r="H30" s="65" t="s">
-        <v>531</v>
+      <c r="H30" t="s">
+        <v>526</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>523</v>
-      </c>
-      <c r="J30" s="47" t="s">
-        <v>526</v>
-      </c>
-      <c r="K30" s="95" t="s">
-        <v>529</v>
-      </c>
-      <c r="L30" s="102" t="s">
-        <v>523</v>
-      </c>
-      <c r="M30" s="47" t="s">
-        <v>526</v>
-      </c>
-      <c r="N30" s="95" t="s">
-        <v>529</v>
-      </c>
-      <c r="O30" s="67" t="s">
-        <v>530</v>
+        <v>583</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="K30" s="81" t="s">
+        <v>524</v>
+      </c>
+      <c r="L30" s="99" t="s">
+        <v>582</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="N30" s="81" t="s">
+        <v>524</v>
+      </c>
+      <c r="O30" s="60" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C31" s="29">
         <v>25</v>
       </c>
-      <c r="D31" s="48" t="s">
+      <c r="D31" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="F31" s="49" t="s">
+      <c r="F31" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="H31" s="51" t="s">
-        <v>532</v>
-      </c>
-      <c r="I31" s="52" t="s">
-        <v>524</v>
-      </c>
-      <c r="J31" s="53" t="s">
+      <c r="H31" s="48" t="s">
         <v>527</v>
       </c>
-      <c r="K31" s="96" t="s">
-        <v>515</v>
-      </c>
-      <c r="L31" s="103" t="s">
-        <v>591</v>
-      </c>
-      <c r="M31" s="53" t="s">
-        <v>527</v>
-      </c>
-      <c r="N31" s="96" t="s">
-        <v>515</v>
-      </c>
-      <c r="O31" s="80" t="s">
-        <v>530</v>
+      <c r="I31" s="49" t="s">
+        <v>584</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>522</v>
+      </c>
+      <c r="K31" s="82" t="s">
+        <v>512</v>
+      </c>
+      <c r="L31" s="100" t="s">
+        <v>580</v>
+      </c>
+      <c r="M31" s="50" t="s">
+        <v>522</v>
+      </c>
+      <c r="N31" s="82" t="s">
+        <v>512</v>
+      </c>
+      <c r="O31" s="72" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C32" s="29">
         <v>26</v>
       </c>
-      <c r="D32" s="83" t="s">
+      <c r="D32" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="E32" s="83" t="s">
+      <c r="E32" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="F32" s="84" t="s">
+      <c r="F32" s="75" t="s">
         <v>370</v>
       </c>
-      <c r="G32" s="85" t="s">
+      <c r="G32" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="86" t="s">
-        <v>572</v>
-      </c>
-      <c r="I32" s="100" t="s">
+      <c r="H32" s="76" t="s">
+        <v>561</v>
+      </c>
+      <c r="I32" s="86" t="s">
         <v>461</v>
       </c>
-      <c r="J32" s="58" t="s">
-        <v>577</v>
-      </c>
-      <c r="K32" s="58" t="s">
-        <v>578</v>
-      </c>
-      <c r="L32" s="100" t="s">
+      <c r="J32" s="55" t="s">
+        <v>566</v>
+      </c>
+      <c r="K32" s="55" t="s">
+        <v>567</v>
+      </c>
+      <c r="L32" s="86" t="s">
         <v>461</v>
       </c>
-      <c r="M32" s="58" t="s">
-        <v>577</v>
-      </c>
-      <c r="N32" s="58" t="s">
-        <v>578</v>
-      </c>
-      <c r="O32" s="56" t="s">
-        <v>582</v>
+      <c r="M32" s="55" t="s">
+        <v>566</v>
+      </c>
+      <c r="N32" s="55" t="s">
+        <v>567</v>
+      </c>
+      <c r="O32" s="53" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C33" s="29">
         <v>27</v>
       </c>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="E33" s="87" t="s">
+      <c r="E33" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="F33" s="88" t="s">
+      <c r="F33" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G33" s="89" t="s">
         <v>364</v>
       </c>
-      <c r="H33" s="89" t="s">
-        <v>575</v>
-      </c>
-      <c r="I33" s="66" t="s">
+      <c r="H33" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="I33" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J33" s="47" t="s">
-        <v>579</v>
-      </c>
-      <c r="K33" s="47" t="s">
-        <v>580</v>
-      </c>
-      <c r="L33" s="66" t="s">
+      <c r="J33" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="L33" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M33" s="47" t="s">
-        <v>579</v>
-      </c>
-      <c r="N33" s="47" t="s">
-        <v>580</v>
+      <c r="M33" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="N33" s="8" t="s">
+        <v>569</v>
       </c>
       <c r="O33" s="33" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C34" s="29">
         <v>28</v>
       </c>
-      <c r="D34" s="87" t="s">
+      <c r="D34" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="E34" s="87" t="s">
+      <c r="E34" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="F34" s="88" t="s">
+      <c r="F34" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="G34" s="34" t="s">
+      <c r="G34" s="89" t="s">
         <v>249</v>
       </c>
-      <c r="H34" s="89" t="s">
+      <c r="H34" s="22" t="s">
+        <v>562</v>
+      </c>
+      <c r="I34" s="59" t="s">
+        <v>461</v>
+      </c>
+      <c r="J34" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="I34" s="66" t="s">
+      <c r="K34" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="L34" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J34" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="K34" s="47" t="s">
-        <v>583</v>
-      </c>
-      <c r="L34" s="66" t="s">
-        <v>461</v>
-      </c>
-      <c r="M34" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="N34" s="47" t="s">
-        <v>583</v>
+      <c r="M34" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>572</v>
       </c>
       <c r="O34" s="33" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C35" s="29">
         <v>29</v>
       </c>
-      <c r="D35" s="87" t="s">
+      <c r="D35" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="E35" s="87" t="s">
+      <c r="E35" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="F35" s="88" t="s">
+      <c r="F35" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="G35" s="34" t="s">
+      <c r="G35" s="89" t="s">
         <v>250</v>
       </c>
-      <c r="H35" s="89" t="s">
+      <c r="H35" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="I35" s="59" t="s">
+        <v>461</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="L35" s="59" t="s">
+        <v>461</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="O35" s="33" t="s">
         <v>574</v>
-      </c>
-      <c r="I35" s="66" t="s">
-        <v>461</v>
-      </c>
-      <c r="J35" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="K35" s="47" t="s">
-        <v>583</v>
-      </c>
-      <c r="L35" s="66" t="s">
-        <v>461</v>
-      </c>
-      <c r="M35" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="N35" s="47" t="s">
-        <v>583</v>
-      </c>
-      <c r="O35" s="33" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C36" s="29">
         <v>30</v>
       </c>
-      <c r="D36" s="90" t="s">
+      <c r="D36" s="77" t="s">
         <v>251</v>
       </c>
-      <c r="E36" s="90" t="s">
+      <c r="E36" s="77" t="s">
         <v>251</v>
       </c>
-      <c r="F36" s="91" t="s">
+      <c r="F36" s="78" t="s">
         <v>323</v>
       </c>
-      <c r="G36" s="92" t="s">
+      <c r="G36" s="96" t="s">
         <v>251</v>
       </c>
-      <c r="H36" s="93" t="s">
-        <v>576</v>
-      </c>
-      <c r="I36" s="66" t="s">
+      <c r="H36" s="79" t="s">
+        <v>565</v>
+      </c>
+      <c r="I36" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J36" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="K36" s="47" t="s">
-        <v>586</v>
-      </c>
-      <c r="L36" s="66" t="s">
+      <c r="J36" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="L36" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M36" s="47" t="s">
-        <v>584</v>
-      </c>
-      <c r="N36" s="47" t="s">
-        <v>586</v>
-      </c>
-      <c r="O36" s="50"/>
+      <c r="M36" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="O36" s="47"/>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C37" s="29">
@@ -5813,32 +5883,32 @@
       <c r="F37" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="G37" s="33" t="s">
+      <c r="G37" s="90" t="s">
         <v>394</v>
       </c>
       <c r="H37" t="s">
-        <v>533</v>
-      </c>
-      <c r="I37" s="57" t="s">
-        <v>534</v>
-      </c>
-      <c r="J37" s="58" t="s">
-        <v>534</v>
-      </c>
-      <c r="K37" s="58" t="s">
-        <v>534</v>
-      </c>
-      <c r="L37" s="57" t="s">
-        <v>534</v>
-      </c>
-      <c r="M37" s="58" t="s">
-        <v>534</v>
-      </c>
-      <c r="N37" s="58" t="s">
-        <v>534</v>
+        <v>528</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>529</v>
+      </c>
+      <c r="J37" s="55" t="s">
+        <v>529</v>
+      </c>
+      <c r="K37" s="55" t="s">
+        <v>529</v>
+      </c>
+      <c r="L37" s="98" t="s">
+        <v>591</v>
+      </c>
+      <c r="M37" s="55" t="s">
+        <v>529</v>
+      </c>
+      <c r="N37" s="55" t="s">
+        <v>529</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>539</v>
+        <v>590</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.35">
@@ -5854,32 +5924,32 @@
       <c r="F38" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G38" s="90" t="s">
         <v>255</v>
       </c>
       <c r="H38" t="s">
         <v>429</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>537</v>
+        <v>594</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="L38" s="35" t="s">
-        <v>537</v>
+        <v>530</v>
+      </c>
+      <c r="L38" s="99" t="s">
+        <v>592</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="O38" s="67" t="s">
-        <v>528</v>
+        <v>530</v>
+      </c>
+      <c r="O38" s="60" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.35">
@@ -5895,400 +5965,400 @@
       <c r="F39" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G39" s="90" t="s">
         <v>367</v>
       </c>
-      <c r="H39" s="46" t="s">
+      <c r="H39" t="s">
         <v>431</v>
       </c>
       <c r="I39" s="35" t="s">
         <v>444</v>
       </c>
-      <c r="J39" s="47" t="s">
+      <c r="J39" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="K39" s="47" t="s">
+      <c r="K39" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="L39" s="35" t="s">
+      <c r="L39" s="99" t="s">
         <v>444</v>
       </c>
-      <c r="M39" s="47" t="s">
+      <c r="M39" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="N39" s="47" t="s">
+      <c r="N39" s="8" t="s">
         <v>444</v>
       </c>
       <c r="O39" s="33" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C40" s="29">
         <v>34</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="F40" s="59" t="s">
+      <c r="F40" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G40" s="90" t="s">
         <v>270</v>
       </c>
       <c r="H40" t="s">
-        <v>519</v>
-      </c>
-      <c r="I40" s="66" t="s">
+        <v>516</v>
+      </c>
+      <c r="I40" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J40" s="47" t="s">
-        <v>540</v>
-      </c>
-      <c r="K40" s="47" t="s">
-        <v>541</v>
-      </c>
-      <c r="L40" s="66" t="s">
+      <c r="J40" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="L40" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M40" s="47" t="s">
-        <v>540</v>
-      </c>
-      <c r="N40" s="47" t="s">
-        <v>541</v>
-      </c>
-      <c r="O40" s="67" t="s">
-        <v>542</v>
+      <c r="M40" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="O40" s="60" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C41" s="29">
         <v>35</v>
       </c>
-      <c r="D41" s="45" t="s">
+      <c r="D41" s="30" t="s">
         <v>271</v>
       </c>
-      <c r="E41" s="45" t="s">
+      <c r="E41" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="F41" s="59" t="s">
+      <c r="F41" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="G41" s="33" t="s">
+      <c r="G41" s="90" t="s">
         <v>360</v>
       </c>
-      <c r="H41" s="46" t="s">
-        <v>520</v>
-      </c>
-      <c r="I41" s="66" t="s">
+      <c r="H41" t="s">
+        <v>517</v>
+      </c>
+      <c r="I41" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J41" s="47" t="s">
-        <v>543</v>
-      </c>
-      <c r="K41" s="47" t="s">
-        <v>544</v>
-      </c>
-      <c r="L41" s="66" t="s">
+      <c r="J41" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="L41" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M41" s="47" t="s">
-        <v>543</v>
-      </c>
-      <c r="N41" s="47" t="s">
-        <v>544</v>
-      </c>
-      <c r="O41" s="67" t="s">
-        <v>542</v>
+      <c r="M41" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="O41" s="60" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C42" s="29">
         <v>36</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="30" t="s">
         <v>422</v>
       </c>
-      <c r="F42" s="59" t="s">
+      <c r="F42" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="G42" s="33" t="s">
+      <c r="G42" s="90" t="s">
         <v>272</v>
       </c>
       <c r="H42" t="s">
-        <v>521</v>
-      </c>
-      <c r="I42" s="66" t="s">
+        <v>518</v>
+      </c>
+      <c r="I42" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="J42" s="47" t="s">
-        <v>548</v>
-      </c>
-      <c r="K42" s="47" t="s">
-        <v>547</v>
-      </c>
-      <c r="L42" s="66" t="s">
+      <c r="J42" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="L42" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M42" s="47" t="s">
-        <v>548</v>
-      </c>
-      <c r="N42" s="47" t="s">
-        <v>547</v>
-      </c>
-      <c r="O42" s="67" t="s">
+      <c r="M42" s="8" t="s">
         <v>542</v>
+      </c>
+      <c r="N42" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="O42" s="60" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C43" s="29">
         <v>37</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D43" s="45" t="s">
         <v>273</v>
       </c>
-      <c r="E43" s="48" t="s">
+      <c r="E43" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="F43" s="49" t="s">
+      <c r="F43" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="G43" s="50" t="s">
+      <c r="G43" s="92" t="s">
         <v>361</v>
       </c>
-      <c r="H43" s="46" t="s">
-        <v>522</v>
-      </c>
-      <c r="I43" s="97" t="s">
+      <c r="H43" t="s">
+        <v>519</v>
+      </c>
+      <c r="I43" s="83" t="s">
         <v>461</v>
       </c>
-      <c r="J43" s="53" t="s">
-        <v>545</v>
-      </c>
-      <c r="K43" s="53" t="s">
-        <v>546</v>
-      </c>
-      <c r="L43" s="97" t="s">
+      <c r="J43" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="K43" s="50" t="s">
+        <v>540</v>
+      </c>
+      <c r="L43" s="83" t="s">
         <v>461</v>
       </c>
-      <c r="M43" s="53" t="s">
-        <v>545</v>
-      </c>
-      <c r="N43" s="53" t="s">
-        <v>546</v>
-      </c>
-      <c r="O43" s="80" t="s">
-        <v>542</v>
+      <c r="M43" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="N43" s="50" t="s">
+        <v>540</v>
+      </c>
+      <c r="O43" s="72" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C44" s="29">
         <v>38</v>
       </c>
-      <c r="D44" s="83" t="s">
+      <c r="D44" s="74" t="s">
         <v>236</v>
       </c>
-      <c r="E44" s="83" t="s">
+      <c r="E44" s="74" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="86" t="s">
+      <c r="F44" s="76" t="s">
         <v>426</v>
       </c>
-      <c r="G44" s="85" t="s">
+      <c r="G44" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="H44" s="86" t="s">
-        <v>556</v>
-      </c>
-      <c r="I44" s="57" t="s">
-        <v>555</v>
-      </c>
-      <c r="J44" s="58" t="s">
-        <v>557</v>
-      </c>
-      <c r="K44" s="58" t="s">
-        <v>558</v>
-      </c>
-      <c r="L44" s="57" t="s">
-        <v>555</v>
-      </c>
-      <c r="M44" s="58" t="s">
-        <v>557</v>
-      </c>
-      <c r="N44" s="58" t="s">
-        <v>558</v>
-      </c>
-      <c r="O44" s="67" t="s">
-        <v>565</v>
+      <c r="H44" s="76" t="s">
+        <v>546</v>
+      </c>
+      <c r="I44" s="54" t="s">
+        <v>593</v>
+      </c>
+      <c r="J44" s="55" t="s">
+        <v>547</v>
+      </c>
+      <c r="K44" s="55" t="s">
+        <v>548</v>
+      </c>
+      <c r="L44" s="98" t="s">
+        <v>595</v>
+      </c>
+      <c r="M44" s="55" t="s">
+        <v>547</v>
+      </c>
+      <c r="N44" s="55" t="s">
+        <v>548</v>
+      </c>
+      <c r="O44" s="60" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C45" s="29">
         <v>39</v>
       </c>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="E45" s="45" t="s">
+      <c r="E45" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="F45" s="59" t="s">
+      <c r="F45" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="G45" s="33" t="s">
+      <c r="G45" s="90" t="s">
         <v>391</v>
       </c>
-      <c r="H45" s="46" t="s">
+      <c r="H45" t="s">
+        <v>543</v>
+      </c>
+      <c r="I45" s="35" t="s">
+        <v>597</v>
+      </c>
+      <c r="J45" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="I45" s="35" t="s">
-        <v>554</v>
-      </c>
-      <c r="J45" s="47" t="s">
-        <v>559</v>
-      </c>
-      <c r="K45" s="47" t="s">
-        <v>560</v>
-      </c>
-      <c r="L45" s="35" t="s">
-        <v>554</v>
-      </c>
-      <c r="M45" s="47" t="s">
-        <v>559</v>
-      </c>
-      <c r="N45" s="47" t="s">
-        <v>560</v>
-      </c>
-      <c r="O45" s="67" t="s">
-        <v>565</v>
+      <c r="K45" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="L45" s="99" t="s">
+        <v>596</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="O45" s="60" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C46" s="29">
         <v>40</v>
       </c>
-      <c r="D46" s="45" t="s">
+      <c r="D46" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="E46" s="45" t="s">
+      <c r="E46" s="30" t="s">
         <v>421</v>
       </c>
-      <c r="F46" s="59" t="s">
+      <c r="F46" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="G46" s="33" t="s">
+      <c r="G46" s="90" t="s">
         <v>390</v>
       </c>
-      <c r="H46" s="46" t="s">
-        <v>550</v>
+      <c r="H46" t="s">
+        <v>544</v>
       </c>
       <c r="I46" s="35" t="s">
-        <v>553</v>
-      </c>
-      <c r="J46" s="47" t="s">
-        <v>562</v>
-      </c>
-      <c r="K46" s="47" t="s">
-        <v>561</v>
-      </c>
-      <c r="L46" s="35" t="s">
-        <v>553</v>
-      </c>
-      <c r="M46" s="47" t="s">
-        <v>562</v>
-      </c>
-      <c r="N46" s="47" t="s">
-        <v>561</v>
-      </c>
-      <c r="O46" s="67" t="s">
-        <v>565</v>
+        <v>599</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="L46" s="99" t="s">
+        <v>598</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="N46" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="O46" s="60" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C47" s="29">
         <v>41</v>
       </c>
-      <c r="D47" s="48" t="s">
+      <c r="D47" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="E47" s="48" t="s">
+      <c r="E47" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="F47" s="49" t="s">
+      <c r="F47" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="G47" s="50" t="s">
+      <c r="G47" s="92" t="s">
         <v>256</v>
       </c>
-      <c r="H47" s="51" t="s">
-        <v>551</v>
-      </c>
-      <c r="I47" s="52" t="s">
-        <v>552</v>
-      </c>
-      <c r="J47" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="K47" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="L47" s="52" t="s">
-        <v>552</v>
-      </c>
-      <c r="M47" s="53" t="s">
-        <v>563</v>
-      </c>
-      <c r="N47" s="53" t="s">
-        <v>564</v>
-      </c>
-      <c r="O47" s="80" t="s">
-        <v>565</v>
+      <c r="H47" s="48" t="s">
+        <v>545</v>
+      </c>
+      <c r="I47" s="49" t="s">
+        <v>600</v>
+      </c>
+      <c r="J47" s="50" t="s">
+        <v>553</v>
+      </c>
+      <c r="K47" s="50" t="s">
+        <v>554</v>
+      </c>
+      <c r="L47" s="100" t="s">
+        <v>603</v>
+      </c>
+      <c r="M47" s="50" t="s">
+        <v>553</v>
+      </c>
+      <c r="N47" s="50" t="s">
+        <v>554</v>
+      </c>
+      <c r="O47" s="72" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C48" s="29">
         <v>42</v>
       </c>
-      <c r="D48" s="54" t="s">
+      <c r="D48" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="54" t="s">
+      <c r="E48" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="F48" s="76" t="s">
+      <c r="F48" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G48" s="56" t="s">
+      <c r="G48" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="55" t="s">
-        <v>517</v>
-      </c>
-      <c r="I48" s="57" t="s">
-        <v>566</v>
-      </c>
-      <c r="J48" s="58" t="s">
-        <v>568</v>
-      </c>
-      <c r="K48" s="98" t="s">
-        <v>570</v>
-      </c>
-      <c r="L48" s="57" t="s">
-        <v>566</v>
-      </c>
-      <c r="M48" s="58" t="s">
-        <v>568</v>
-      </c>
-      <c r="N48" s="98" t="s">
-        <v>570</v>
-      </c>
-      <c r="O48" s="56" t="s">
+      <c r="H48" s="52" t="s">
+        <v>514</v>
+      </c>
+      <c r="I48" s="54" t="s">
+        <v>555</v>
+      </c>
+      <c r="J48" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="K48" s="84" t="s">
+        <v>559</v>
+      </c>
+      <c r="L48" s="54" t="s">
+        <v>555</v>
+      </c>
+      <c r="M48" s="55" t="s">
+        <v>557</v>
+      </c>
+      <c r="N48" s="84" t="s">
+        <v>559</v>
+      </c>
+      <c r="O48" s="53" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6296,40 +6366,40 @@
       <c r="C49" s="29">
         <v>43</v>
       </c>
-      <c r="D49" s="48" t="s">
+      <c r="D49" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E49" s="48" t="s">
+      <c r="E49" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="49" t="s">
+      <c r="F49" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="G49" s="50" t="s">
+      <c r="G49" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="H49" s="51" t="s">
-        <v>518</v>
-      </c>
-      <c r="I49" s="52" t="s">
-        <v>567</v>
-      </c>
-      <c r="J49" s="53" t="s">
-        <v>569</v>
-      </c>
-      <c r="K49" s="99" t="s">
-        <v>571</v>
-      </c>
-      <c r="L49" s="52" t="s">
-        <v>567</v>
-      </c>
-      <c r="M49" s="53" t="s">
-        <v>569</v>
-      </c>
-      <c r="N49" s="99" t="s">
-        <v>571</v>
-      </c>
-      <c r="O49" s="50" t="s">
+      <c r="H49" s="48" t="s">
+        <v>515</v>
+      </c>
+      <c r="I49" s="49" t="s">
+        <v>556</v>
+      </c>
+      <c r="J49" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="K49" s="85" t="s">
+        <v>560</v>
+      </c>
+      <c r="L49" s="49" t="s">
+        <v>556</v>
+      </c>
+      <c r="M49" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="N49" s="85" t="s">
+        <v>560</v>
+      </c>
+      <c r="O49" s="47" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6346,24 +6416,24 @@
       <c r="F50" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="97" t="s">
         <v>409</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="I50" s="66" t="s">
+      <c r="I50" s="59" t="s">
         <v>432</v>
       </c>
       <c r="J50" s="6"/>
-      <c r="K50" s="71" t="s">
+      <c r="K50" s="63" t="s">
         <v>351</v>
       </c>
-      <c r="L50" s="66" t="s">
+      <c r="L50" s="59" t="s">
         <v>432</v>
       </c>
       <c r="M50" s="6"/>
-      <c r="N50" s="71" t="s">
+      <c r="N50" s="63" t="s">
         <v>351</v>
       </c>
       <c r="O50" s="33" t="s">
@@ -6383,24 +6453,24 @@
       <c r="F51" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="97" t="s">
         <v>410</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="I51" s="66" t="s">
+      <c r="I51" s="59" t="s">
         <v>412</v>
       </c>
       <c r="J51" s="6"/>
-      <c r="K51" s="71" t="s">
+      <c r="K51" s="63" t="s">
         <v>351</v>
       </c>
-      <c r="L51" s="66" t="s">
+      <c r="L51" s="59" t="s">
         <v>412</v>
       </c>
       <c r="M51" s="6"/>
-      <c r="N51" s="71" t="s">
+      <c r="N51" s="63" t="s">
         <v>351</v>
       </c>
       <c r="O51" s="33" t="s">

</xml_diff>

<commit_message>
added cleaning for CveVeg_S5 and TipoVeg_S5 in Arb.04
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629FA9C3-7B01-480F-94BF-9B6AFBAE72A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A5E583-7D73-4F12-A55B-A1FBAC8CF626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="608">
   <si>
     <t>Variable</t>
   </si>
@@ -1464,9 +1464,6 @@
     <t>n= 180</t>
   </si>
   <si>
-    <t>around 126 could be right</t>
-  </si>
-  <si>
     <t>n= 62, because of inconsequent naming</t>
   </si>
   <si>
@@ -1890,6 +1887,21 @@
   </si>
   <si>
     <t>n= 79 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there are a total of 139 different values but not all are present in all ds -&gt; normalizing names in general  </t>
+  </si>
+  <si>
+    <t>there are a total of 139 different values but not all are present in all ds -&gt; normalizing names in general  -&gt; all caps no accents</t>
+  </si>
+  <si>
+    <t>n= 133 (NA)</t>
+  </si>
+  <si>
+    <t>n= 60068 (NA)</t>
+  </si>
+  <si>
+    <t>n= 58436 (NA)</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1968,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2050,6 +2062,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2222,7 +2240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2341,7 +2359,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2351,10 +2368,8 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4532,8 +4547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4565,21 +4580,21 @@
     <row r="2" spans="3:16" x14ac:dyDescent="0.35">
       <c r="I2" s="8"/>
       <c r="J2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N2" s="63"/>
       <c r="O2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.35">
       <c r="I3" s="6"/>
       <c r="J3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N3" s="43"/>
       <c r="O3" s="87" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.35">
@@ -4612,7 +4627,7 @@
       <c r="F6" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="G6" s="89" t="s">
+      <c r="G6" s="88" t="s">
         <v>402</v>
       </c>
       <c r="H6" s="28" t="s">
@@ -4653,7 +4668,7 @@
       <c r="F7" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="G7" s="90" t="s">
+      <c r="G7" s="89" t="s">
         <v>2</v>
       </c>
       <c r="H7" t="s">
@@ -4694,7 +4709,7 @@
       <c r="F8" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="G8" s="90" t="s">
+      <c r="G8" s="89" t="s">
         <v>3</v>
       </c>
       <c r="H8" t="s">
@@ -4735,7 +4750,7 @@
       <c r="F9" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="G9" s="90" t="s">
+      <c r="G9" s="89" t="s">
         <v>1</v>
       </c>
       <c r="H9" t="s">
@@ -4776,7 +4791,7 @@
       <c r="F10" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="G10" s="90" t="s">
+      <c r="G10" s="89" t="s">
         <v>233</v>
       </c>
       <c r="H10" t="s">
@@ -4817,7 +4832,7 @@
       <c r="F11" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="90" t="s">
         <v>234</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -4844,8 +4859,8 @@
       <c r="O11" s="35" t="s">
         <v>449</v>
       </c>
-      <c r="P11" s="88" t="s">
-        <v>587</v>
+      <c r="P11" s="7" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.35">
@@ -4861,7 +4876,7 @@
       <c r="F12" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="G12" s="92" t="s">
+      <c r="G12" s="91" t="s">
         <v>425</v>
       </c>
       <c r="H12" s="48" t="s">
@@ -4889,7 +4904,7 @@
         <v>417</v>
       </c>
       <c r="P12" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.35">
@@ -4905,7 +4920,7 @@
       <c r="F13" s="43" t="s">
         <v>404</v>
       </c>
-      <c r="G13" s="93" t="s">
+      <c r="G13" s="92" t="s">
         <v>235</v>
       </c>
       <c r="H13" s="43" t="s">
@@ -4949,7 +4964,7 @@
       <c r="F14" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="G14" s="94" t="s">
+      <c r="G14" s="93" t="s">
         <v>427</v>
       </c>
       <c r="H14" s="52"/>
@@ -4962,8 +4977,8 @@
       <c r="K14" s="55" t="s">
         <v>459</v>
       </c>
-      <c r="L14" s="54" t="s">
-        <v>457</v>
+      <c r="L14" s="69" t="s">
+        <v>605</v>
       </c>
       <c r="M14" s="55" t="s">
         <v>458</v>
@@ -4972,7 +4987,7 @@
         <v>459</v>
       </c>
       <c r="O14" s="53" t="s">
-        <v>470</v>
+        <v>603</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.35">
@@ -4988,30 +5003,30 @@
       <c r="F15" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="G15" s="92" t="s">
+      <c r="G15" s="91" t="s">
         <v>428</v>
       </c>
       <c r="H15" s="48"/>
       <c r="I15" s="49" t="s">
+        <v>470</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>471</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>472</v>
       </c>
       <c r="K15" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="L15" s="49" t="s">
+      <c r="L15" s="57" t="s">
+        <v>605</v>
+      </c>
+      <c r="M15" s="8" t="s">
         <v>471</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>472</v>
       </c>
       <c r="N15" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="O15" s="47" t="s">
-        <v>470</v>
+      <c r="O15" s="53" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.35">
@@ -5027,11 +5042,11 @@
       <c r="F16" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="G16" s="90" t="s">
+      <c r="G16" s="89" t="s">
         <v>237</v>
       </c>
       <c r="H16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I16" s="59" t="s">
         <v>461</v>
@@ -5071,11 +5086,11 @@
       <c r="F17" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="G17" s="90" t="s">
+      <c r="G17" s="89" t="s">
         <v>238</v>
       </c>
       <c r="H17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I17" s="59" t="s">
         <v>461</v>
@@ -5096,7 +5111,7 @@
         <v>465</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
@@ -5112,7 +5127,7 @@
       <c r="F18" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="G18" s="90" t="s">
+      <c r="G18" s="89" t="s">
         <v>239</v>
       </c>
       <c r="H18" t="s">
@@ -5137,7 +5152,7 @@
         <v>469</v>
       </c>
       <c r="O18" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
@@ -5153,26 +5168,26 @@
       <c r="F19" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="G19" s="90" t="s">
+      <c r="G19" s="89" t="s">
         <v>240</v>
       </c>
       <c r="H19" t="s">
         <v>412</v>
       </c>
       <c r="I19" s="62" t="s">
+        <v>474</v>
+      </c>
+      <c r="J19" s="63" t="s">
         <v>475</v>
       </c>
-      <c r="J19" s="63" t="s">
+      <c r="K19" s="63" t="s">
         <v>476</v>
-      </c>
-      <c r="K19" s="63" t="s">
-        <v>477</v>
       </c>
       <c r="L19" s="62"/>
       <c r="M19" s="63"/>
       <c r="N19" s="63"/>
       <c r="O19" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
@@ -5188,32 +5203,32 @@
       <c r="F20" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="G20" s="90" t="s">
+      <c r="G20" s="89" t="s">
         <v>363</v>
       </c>
       <c r="H20" t="s">
         <v>430</v>
       </c>
       <c r="I20" s="66" t="s">
+        <v>479</v>
+      </c>
+      <c r="J20" s="67" t="s">
         <v>480</v>
       </c>
-      <c r="J20" s="67" t="s">
+      <c r="K20" s="67" t="s">
         <v>481</v>
       </c>
-      <c r="K20" s="67" t="s">
-        <v>482</v>
-      </c>
       <c r="L20" s="66" t="s">
+        <v>479</v>
+      </c>
+      <c r="M20" s="67" t="s">
         <v>480</v>
       </c>
-      <c r="M20" s="67" t="s">
+      <c r="N20" s="67" t="s">
         <v>481</v>
       </c>
-      <c r="N20" s="67" t="s">
-        <v>482</v>
-      </c>
       <c r="O20" s="66" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.35">
@@ -5229,32 +5244,32 @@
       <c r="F21" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="G21" s="92" t="s">
+      <c r="G21" s="91" t="s">
         <v>397</v>
       </c>
       <c r="H21" s="48" t="s">
         <v>415</v>
       </c>
       <c r="I21" s="57" t="s">
+        <v>482</v>
+      </c>
+      <c r="J21" s="64" t="s">
+        <v>482</v>
+      </c>
+      <c r="K21" s="50" t="s">
         <v>483</v>
       </c>
-      <c r="J21" s="64" t="s">
+      <c r="L21" s="57" t="s">
+        <v>482</v>
+      </c>
+      <c r="M21" s="64" t="s">
+        <v>482</v>
+      </c>
+      <c r="N21" s="50" t="s">
         <v>483</v>
       </c>
-      <c r="K21" s="50" t="s">
-        <v>484</v>
-      </c>
-      <c r="L21" s="57" t="s">
-        <v>483</v>
-      </c>
-      <c r="M21" s="64" t="s">
-        <v>483</v>
-      </c>
-      <c r="N21" s="50" t="s">
-        <v>484</v>
-      </c>
       <c r="O21" s="47" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.35">
@@ -5270,32 +5285,32 @@
       <c r="F22" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="G22" s="90" t="s">
+      <c r="G22" s="89" t="s">
         <v>362</v>
       </c>
       <c r="H22" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I22" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J22" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>486</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>487</v>
       </c>
       <c r="L22" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M22" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="N22" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="N22" s="8" t="s">
-        <v>487</v>
-      </c>
       <c r="O22" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.35">
@@ -5311,32 +5326,32 @@
       <c r="F23" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="G23" s="90" t="s">
+      <c r="G23" s="89" t="s">
         <v>253</v>
       </c>
       <c r="H23" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I23" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J23" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="K23" s="8" t="s">
         <v>488</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>489</v>
       </c>
       <c r="L23" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M23" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="N23" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="N23" s="8" t="s">
+      <c r="O23" s="47" t="s">
         <v>489</v>
-      </c>
-      <c r="O23" s="47" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.35">
@@ -5352,32 +5367,32 @@
       <c r="F24" s="68" t="s">
         <v>314</v>
       </c>
-      <c r="G24" s="94" t="s">
+      <c r="G24" s="93" t="s">
         <v>395</v>
       </c>
       <c r="H24" s="52" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I24" s="69" t="s">
+        <v>491</v>
+      </c>
+      <c r="J24" s="70" t="s">
         <v>492</v>
       </c>
-      <c r="J24" s="70" t="s">
+      <c r="K24" s="55" t="s">
         <v>493</v>
       </c>
-      <c r="K24" s="55" t="s">
-        <v>494</v>
-      </c>
-      <c r="L24" s="98" t="s">
+      <c r="L24" s="69" t="s">
+        <v>491</v>
+      </c>
+      <c r="M24" s="70" t="s">
         <v>492</v>
       </c>
-      <c r="M24" s="70" t="s">
+      <c r="N24" s="55" t="s">
         <v>493</v>
       </c>
-      <c r="N24" s="55" t="s">
-        <v>494</v>
-      </c>
       <c r="O24" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.35">
@@ -5393,32 +5408,32 @@
       <c r="F25" s="31" t="s">
         <v>316</v>
       </c>
-      <c r="G25" s="90" t="s">
+      <c r="G25" s="89" t="s">
         <v>267</v>
       </c>
       <c r="H25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>499</v>
-      </c>
-      <c r="L25" s="99" t="s">
-        <v>577</v>
+        <v>498</v>
+      </c>
+      <c r="L25" s="40" t="s">
+        <v>576</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="O25" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.35">
@@ -5434,32 +5449,32 @@
       <c r="F26" s="46" t="s">
         <v>317</v>
       </c>
-      <c r="G26" s="92" t="s">
+      <c r="G26" s="91" t="s">
         <v>268</v>
       </c>
       <c r="H26" s="48" t="s">
+        <v>496</v>
+      </c>
+      <c r="I26" s="49" t="s">
+        <v>500</v>
+      </c>
+      <c r="J26" s="71" t="s">
+        <v>502</v>
+      </c>
+      <c r="K26" s="71" t="s">
         <v>497</v>
       </c>
-      <c r="I26" s="49" t="s">
-        <v>501</v>
-      </c>
-      <c r="J26" s="71" t="s">
-        <v>503</v>
-      </c>
-      <c r="K26" s="71" t="s">
-        <v>498</v>
-      </c>
-      <c r="L26" s="100" t="s">
-        <v>578</v>
+      <c r="L26" s="57" t="s">
+        <v>577</v>
       </c>
       <c r="M26" s="71" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N26" s="71" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="O26" s="72" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.35">
@@ -5475,32 +5490,32 @@
       <c r="F27" s="68" t="s">
         <v>313</v>
       </c>
-      <c r="G27" s="94" t="s">
+      <c r="G27" s="93" t="s">
         <v>396</v>
       </c>
       <c r="H27" s="52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I27" s="69" t="s">
+        <v>506</v>
+      </c>
+      <c r="J27" s="70" t="s">
         <v>507</v>
       </c>
-      <c r="J27" s="70" t="s">
+      <c r="K27" s="55" t="s">
         <v>508</v>
       </c>
-      <c r="K27" s="55" t="s">
-        <v>509</v>
-      </c>
-      <c r="L27" s="98" t="s">
+      <c r="L27" s="69" t="s">
+        <v>506</v>
+      </c>
+      <c r="M27" s="70" t="s">
         <v>507</v>
       </c>
-      <c r="M27" s="70" t="s">
+      <c r="N27" s="55" t="s">
         <v>508</v>
       </c>
-      <c r="N27" s="55" t="s">
-        <v>509</v>
-      </c>
       <c r="O27" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.35">
@@ -5516,32 +5531,32 @@
       <c r="F28" s="31" t="s">
         <v>336</v>
       </c>
-      <c r="G28" s="90" t="s">
+      <c r="G28" s="89" t="s">
         <v>252</v>
       </c>
       <c r="H28" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>513</v>
-      </c>
-      <c r="L28" s="99" t="s">
-        <v>581</v>
+        <v>512</v>
+      </c>
+      <c r="L28" s="40" t="s">
+        <v>580</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="O28" s="60" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.35">
@@ -5557,32 +5572,32 @@
       <c r="F29" s="46" t="s">
         <v>320</v>
       </c>
-      <c r="G29" s="92" t="s">
+      <c r="G29" s="91" t="s">
         <v>245</v>
       </c>
       <c r="H29" s="48" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J29" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K29" s="73" t="s">
         <v>511</v>
       </c>
-      <c r="K29" s="73" t="s">
-        <v>512</v>
-      </c>
-      <c r="L29" s="101" t="s">
-        <v>579</v>
+      <c r="L29" s="64" t="s">
+        <v>578</v>
       </c>
       <c r="M29" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="N29" s="73" t="s">
         <v>511</v>
       </c>
-      <c r="N29" s="73" t="s">
-        <v>512</v>
-      </c>
       <c r="O29" s="72" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.35">
@@ -5598,32 +5613,32 @@
       <c r="F30" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="G30" s="90" t="s">
+      <c r="G30" s="89" t="s">
         <v>392</v>
       </c>
       <c r="H30" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K30" s="81" t="s">
+        <v>523</v>
+      </c>
+      <c r="L30" s="40" t="s">
+        <v>581</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="N30" s="81" t="s">
+        <v>523</v>
+      </c>
+      <c r="O30" s="60" t="s">
         <v>524</v>
-      </c>
-      <c r="L30" s="99" t="s">
-        <v>582</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>521</v>
-      </c>
-      <c r="N30" s="81" t="s">
-        <v>524</v>
-      </c>
-      <c r="O30" s="60" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.35">
@@ -5639,32 +5654,32 @@
       <c r="F31" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="G31" s="92" t="s">
+      <c r="G31" s="91" t="s">
         <v>393</v>
       </c>
       <c r="H31" s="48" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I31" s="49" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J31" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>512</v>
-      </c>
-      <c r="L31" s="100" t="s">
-        <v>580</v>
+        <v>511</v>
+      </c>
+      <c r="L31" s="57" t="s">
+        <v>579</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N31" s="82" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="O31" s="72" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.35">
@@ -5680,32 +5695,32 @@
       <c r="F32" s="75" t="s">
         <v>370</v>
       </c>
-      <c r="G32" s="95" t="s">
+      <c r="G32" s="94" t="s">
         <v>246</v>
       </c>
       <c r="H32" s="76" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I32" s="86" t="s">
         <v>461</v>
       </c>
       <c r="J32" s="55" t="s">
+        <v>565</v>
+      </c>
+      <c r="K32" s="55" t="s">
         <v>566</v>
-      </c>
-      <c r="K32" s="55" t="s">
-        <v>567</v>
       </c>
       <c r="L32" s="86" t="s">
         <v>461</v>
       </c>
       <c r="M32" s="55" t="s">
+        <v>565</v>
+      </c>
+      <c r="N32" s="55" t="s">
         <v>566</v>
       </c>
-      <c r="N32" s="55" t="s">
-        <v>567</v>
-      </c>
       <c r="O32" s="53" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.35">
@@ -5721,32 +5736,32 @@
       <c r="F33" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="G33" s="89" t="s">
+      <c r="G33" s="88" t="s">
         <v>364</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I33" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J33" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="K33" s="8" t="s">
         <v>568</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>569</v>
       </c>
       <c r="L33" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M33" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="N33" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="N33" s="8" t="s">
+      <c r="O33" s="33" t="s">
         <v>569</v>
-      </c>
-      <c r="O33" s="33" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.35">
@@ -5762,32 +5777,32 @@
       <c r="F34" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="G34" s="89" t="s">
+      <c r="G34" s="88" t="s">
         <v>249</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I34" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L34" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M34" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="O34" s="33" t="s">
         <v>573</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>572</v>
-      </c>
-      <c r="O34" s="33" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.35">
@@ -5803,32 +5818,32 @@
       <c r="F35" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="G35" s="89" t="s">
+      <c r="G35" s="88" t="s">
         <v>250</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I35" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L35" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M35" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="O35" s="33" t="s">
         <v>573</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>572</v>
-      </c>
-      <c r="O35" s="33" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.35">
@@ -5844,29 +5859,29 @@
       <c r="F36" s="78" t="s">
         <v>323</v>
       </c>
-      <c r="G36" s="96" t="s">
+      <c r="G36" s="95" t="s">
         <v>251</v>
       </c>
       <c r="H36" s="79" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I36" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L36" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O36" s="47"/>
     </row>
@@ -5883,32 +5898,32 @@
       <c r="F37" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="G37" s="90" t="s">
+      <c r="G37" s="89" t="s">
         <v>394</v>
       </c>
       <c r="H37" t="s">
+        <v>527</v>
+      </c>
+      <c r="I37" s="54" t="s">
         <v>528</v>
       </c>
-      <c r="I37" s="54" t="s">
-        <v>529</v>
-      </c>
       <c r="J37" s="55" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K37" s="55" t="s">
-        <v>529</v>
-      </c>
-      <c r="L37" s="98" t="s">
-        <v>591</v>
+        <v>528</v>
+      </c>
+      <c r="L37" s="69" t="s">
+        <v>590</v>
       </c>
       <c r="M37" s="55" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="N37" s="55" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.35">
@@ -5924,32 +5939,32 @@
       <c r="F38" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="G38" s="90" t="s">
+      <c r="G38" s="89" t="s">
         <v>255</v>
       </c>
       <c r="H38" t="s">
         <v>429</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K38" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="L38" s="40" t="s">
+        <v>591</v>
+      </c>
+      <c r="M38" s="8" t="s">
         <v>530</v>
       </c>
-      <c r="L38" s="99" t="s">
-        <v>592</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>531</v>
-      </c>
       <c r="N38" s="8" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O38" s="60" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.35">
@@ -5965,7 +5980,7 @@
       <c r="F39" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="G39" s="90" t="s">
+      <c r="G39" s="89" t="s">
         <v>367</v>
       </c>
       <c r="H39" t="s">
@@ -5980,7 +5995,7 @@
       <c r="K39" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="L39" s="99" t="s">
+      <c r="L39" s="40" t="s">
         <v>444</v>
       </c>
       <c r="M39" s="8" t="s">
@@ -5990,7 +6005,7 @@
         <v>444</v>
       </c>
       <c r="O39" s="33" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.35">
@@ -6006,32 +6021,32 @@
       <c r="F40" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="G40" s="90" t="s">
+      <c r="G40" s="89" t="s">
         <v>270</v>
       </c>
       <c r="H40" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I40" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J40" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="K40" s="8" t="s">
         <v>534</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>535</v>
       </c>
       <c r="L40" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M40" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="N40" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="N40" s="8" t="s">
+      <c r="O40" s="60" t="s">
         <v>535</v>
-      </c>
-      <c r="O40" s="60" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.35">
@@ -6047,32 +6062,32 @@
       <c r="F41" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="G41" s="90" t="s">
+      <c r="G41" s="89" t="s">
         <v>360</v>
       </c>
       <c r="H41" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I41" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J41" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="K41" s="8" t="s">
         <v>537</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>538</v>
       </c>
       <c r="L41" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M41" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="N41" s="8" t="s">
         <v>537</v>
       </c>
-      <c r="N41" s="8" t="s">
-        <v>538</v>
-      </c>
       <c r="O41" s="60" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.35">
@@ -6088,32 +6103,32 @@
       <c r="F42" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="G42" s="90" t="s">
+      <c r="G42" s="89" t="s">
         <v>272</v>
       </c>
       <c r="H42" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I42" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L42" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O42" s="60" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.35">
@@ -6129,32 +6144,32 @@
       <c r="F43" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="G43" s="92" t="s">
+      <c r="G43" s="91" t="s">
         <v>361</v>
       </c>
       <c r="H43" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I43" s="83" t="s">
         <v>461</v>
       </c>
       <c r="J43" s="50" t="s">
+        <v>538</v>
+      </c>
+      <c r="K43" s="50" t="s">
         <v>539</v>
-      </c>
-      <c r="K43" s="50" t="s">
-        <v>540</v>
       </c>
       <c r="L43" s="83" t="s">
         <v>461</v>
       </c>
       <c r="M43" s="50" t="s">
+        <v>538</v>
+      </c>
+      <c r="N43" s="50" t="s">
         <v>539</v>
       </c>
-      <c r="N43" s="50" t="s">
-        <v>540</v>
-      </c>
       <c r="O43" s="72" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.35">
@@ -6170,32 +6185,32 @@
       <c r="F44" s="76" t="s">
         <v>426</v>
       </c>
-      <c r="G44" s="95" t="s">
+      <c r="G44" s="94" t="s">
         <v>236</v>
       </c>
       <c r="H44" s="76" t="s">
+        <v>545</v>
+      </c>
+      <c r="I44" s="54" t="s">
+        <v>592</v>
+      </c>
+      <c r="J44" s="55" t="s">
         <v>546</v>
       </c>
-      <c r="I44" s="54" t="s">
-        <v>593</v>
-      </c>
-      <c r="J44" s="55" t="s">
+      <c r="K44" s="55" t="s">
         <v>547</v>
       </c>
-      <c r="K44" s="55" t="s">
-        <v>548</v>
-      </c>
-      <c r="L44" s="98" t="s">
-        <v>595</v>
+      <c r="L44" s="69" t="s">
+        <v>594</v>
       </c>
       <c r="M44" s="55" t="s">
+        <v>546</v>
+      </c>
+      <c r="N44" s="55" t="s">
         <v>547</v>
       </c>
-      <c r="N44" s="55" t="s">
-        <v>548</v>
-      </c>
       <c r="O44" s="60" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
@@ -6211,32 +6226,32 @@
       <c r="F45" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="G45" s="90" t="s">
+      <c r="G45" s="89" t="s">
         <v>391</v>
       </c>
       <c r="H45" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J45" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="K45" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="K45" s="8" t="s">
-        <v>550</v>
-      </c>
-      <c r="L45" s="99" t="s">
-        <v>596</v>
+      <c r="L45" s="40" t="s">
+        <v>595</v>
       </c>
       <c r="M45" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="N45" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="N45" s="8" t="s">
-        <v>550</v>
-      </c>
       <c r="O45" s="60" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.35">
@@ -6252,32 +6267,32 @@
       <c r="F46" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="G46" s="90" t="s">
+      <c r="G46" s="89" t="s">
         <v>390</v>
       </c>
       <c r="H46" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I46" s="35" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="K46" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="L46" s="40" t="s">
+        <v>597</v>
+      </c>
+      <c r="M46" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="L46" s="99" t="s">
-        <v>598</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>552</v>
-      </c>
       <c r="N46" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="O46" s="60" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.35">
@@ -6293,32 +6308,32 @@
       <c r="F47" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="G47" s="92" t="s">
+      <c r="G47" s="91" t="s">
         <v>256</v>
       </c>
       <c r="H47" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I47" s="49" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="J47" s="50" t="s">
+        <v>552</v>
+      </c>
+      <c r="K47" s="50" t="s">
         <v>553</v>
       </c>
-      <c r="K47" s="50" t="s">
-        <v>554</v>
-      </c>
-      <c r="L47" s="100" t="s">
-        <v>603</v>
+      <c r="L47" s="57" t="s">
+        <v>602</v>
       </c>
       <c r="M47" s="50" t="s">
+        <v>552</v>
+      </c>
+      <c r="N47" s="50" t="s">
         <v>553</v>
       </c>
-      <c r="N47" s="50" t="s">
-        <v>554</v>
-      </c>
       <c r="O47" s="72" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.35">
@@ -6334,29 +6349,29 @@
       <c r="F48" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G48" s="94" t="s">
+      <c r="G48" s="93" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="52" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J48" s="55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K48" s="84" t="s">
-        <v>559</v>
-      </c>
-      <c r="L48" s="54" t="s">
-        <v>555</v>
+        <v>558</v>
+      </c>
+      <c r="L48" s="97" t="s">
+        <v>606</v>
       </c>
       <c r="M48" s="55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N48" s="84" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="O48" s="53" t="s">
         <v>351</v>
@@ -6375,29 +6390,29 @@
       <c r="F49" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="G49" s="92" t="s">
+      <c r="G49" s="91" t="s">
         <v>30</v>
       </c>
       <c r="H49" s="48" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I49" s="49" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J49" s="50" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K49" s="85" t="s">
-        <v>560</v>
-      </c>
-      <c r="L49" s="49" t="s">
-        <v>556</v>
+        <v>559</v>
+      </c>
+      <c r="L49" s="98" t="s">
+        <v>607</v>
       </c>
       <c r="M49" s="50" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N49" s="85" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O49" s="47" t="s">
         <v>351</v>
@@ -6416,7 +6431,7 @@
       <c r="F50" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="G50" s="97" t="s">
+      <c r="G50" s="96" t="s">
         <v>409</v>
       </c>
       <c r="H50" s="8" t="s">
@@ -6453,7 +6468,7 @@
       <c r="F51" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="G51" s="97" t="s">
+      <c r="G51" s="96" t="s">
         <v>410</v>
       </c>
       <c r="H51" s="8" t="s">

</xml_diff>

<commit_message>
adapted and added some cleaning steps to Arb.09
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A5E583-7D73-4F12-A55B-A1FBAC8CF626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F1BD36-F302-4FB7-B27F-E07FA9E01C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="625">
   <si>
     <t>Variable</t>
   </si>
@@ -1522,15 +1522,9 @@
     <t>Distance measured in meters from the center of the site to the intersection of the normal diameter and the central axis of the individual</t>
   </si>
   <si>
-    <t>n= 2667, NULL</t>
-  </si>
-  <si>
     <t>n= 1275, 999991.00</t>
   </si>
   <si>
-    <t>n= 362 (class = "character")</t>
-  </si>
-  <si>
     <t>n= 363 (2 values for NA)</t>
   </si>
   <si>
@@ -1570,12 +1564,6 @@
     <t>n= 1646 (NULL, "character")</t>
   </si>
   <si>
-    <t>n= 1712 (NULL, "character")</t>
-  </si>
-  <si>
-    <t>n= 1384 (NULL, "character")</t>
-  </si>
-  <si>
     <t>Diameter in centimeters with tree bark at a height of 1.30 meters above the maximum slope of the surrounding terrain.</t>
   </si>
   <si>
@@ -1592,12 +1580,6 @@
   </si>
   <si>
     <t>n= 1282 (999993.00)</t>
-  </si>
-  <si>
-    <t>n= 1442 (NULL)</t>
-  </si>
-  <si>
-    <t>n= 1250 (NULL)</t>
   </si>
   <si>
     <t>n= 1324 (999991.00 &amp; 999993.00)</t>
@@ -1670,9 +1652,6 @@
     <t>n= 190 (999991.00 &amp; 999993.00)</t>
   </si>
   <si>
-    <t>n= 324 (NULL, 999, character)</t>
-  </si>
-  <si>
     <t>n= 4, no NA, same spelling across ds</t>
   </si>
   <si>
@@ -1718,27 +1697,15 @@
     <t>Number of alive branches</t>
   </si>
   <si>
-    <t>n= 37 (NULL, 999, 9999)</t>
-  </si>
-  <si>
     <t>n= 225 (999993, 2 weirdly high values 2134 &amp; 5357)</t>
   </si>
   <si>
-    <t>n= 124 (NULL, 999)</t>
-  </si>
-  <si>
     <t>n= 151 (999991 &amp; 999993)</t>
   </si>
   <si>
     <t>n= 117 (999991 &amp; 999993)</t>
   </si>
   <si>
-    <t>n= 104 (NULL, 999)</t>
-  </si>
-  <si>
-    <t>n= 84 (NULL)</t>
-  </si>
-  <si>
     <t>n= 92 (999991 &amp; 999993)</t>
   </si>
   <si>
@@ -1902,6 +1869,90 @@
   </si>
   <si>
     <t>n= 58436 (NA)</t>
+  </si>
+  <si>
+    <t>n= 131 (NA)</t>
+  </si>
+  <si>
+    <t>n= 60, because of inceonsequent naming (NA)</t>
+  </si>
+  <si>
+    <t>n= 1712 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1384 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1442 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1250 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1712 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1384 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n= 362 (NA,"integer") </t>
+  </si>
+  <si>
+    <t>n= 1442 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1250 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 362 (NULL, "integer")</t>
+  </si>
+  <si>
+    <t>n= 2667 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 2667 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 2599 (NA, Character)</t>
+  </si>
+  <si>
+    <t>n= 1699 (NA, Character)</t>
+  </si>
+  <si>
+    <t>n= 324 (NA,  character)</t>
+  </si>
+  <si>
+    <t>n= 324 (NULL, character)</t>
+  </si>
+  <si>
+    <t>n= 37 (NA, 999, 9999)</t>
+  </si>
+  <si>
+    <t>n= 124 (NA, 999)</t>
+  </si>
+  <si>
+    <t>n= 104 (NA, 999)</t>
+  </si>
+  <si>
+    <t>n= 84 (NA)</t>
+  </si>
+  <si>
+    <t>n= 37 (NULL, 999, 9999, "integer")</t>
+  </si>
+  <si>
+    <t>n= 124 (NULL, 999, "integer")</t>
+  </si>
+  <si>
+    <t>n= 104 (NULL, 999, "integer")</t>
+  </si>
+  <si>
+    <t>n= 84 (NULL, "integer")</t>
+  </si>
+  <si>
+    <t>n= 64447 (NA)</t>
+  </si>
+  <si>
+    <t>n= 63193 (NA)</t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2370,6 +2421,12 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4547,8 +4604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4580,7 +4637,7 @@
     <row r="2" spans="3:16" x14ac:dyDescent="0.35">
       <c r="I2" s="8"/>
       <c r="J2" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="N2" s="63"/>
       <c r="O2" t="s">
@@ -4594,7 +4651,7 @@
       </c>
       <c r="N3" s="43"/>
       <c r="O3" s="87" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.35">
@@ -4860,7 +4917,7 @@
         <v>449</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.35">
@@ -4904,7 +4961,7 @@
         <v>417</v>
       </c>
       <c r="P12" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.35">
@@ -4978,16 +5035,16 @@
         <v>459</v>
       </c>
       <c r="L14" s="69" t="s">
-        <v>605</v>
-      </c>
-      <c r="M14" s="55" t="s">
-        <v>458</v>
+        <v>594</v>
+      </c>
+      <c r="M14" s="99" t="s">
+        <v>597</v>
       </c>
       <c r="N14" s="55" t="s">
         <v>459</v>
       </c>
       <c r="O14" s="53" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.35">
@@ -5017,16 +5074,16 @@
         <v>459</v>
       </c>
       <c r="L15" s="57" t="s">
-        <v>605</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>471</v>
+        <v>594</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>598</v>
       </c>
       <c r="N15" s="50" t="s">
         <v>459</v>
       </c>
       <c r="O15" s="53" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.35">
@@ -5111,7 +5168,7 @@
         <v>465</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
@@ -5152,7 +5209,7 @@
         <v>469</v>
       </c>
       <c r="O18" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
@@ -5187,7 +5244,7 @@
       <c r="M19" s="63"/>
       <c r="N19" s="63"/>
       <c r="O19" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
@@ -5228,7 +5285,7 @@
         <v>481</v>
       </c>
       <c r="O20" s="66" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.35">
@@ -5295,22 +5352,22 @@
         <v>461</v>
       </c>
       <c r="J22" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>485</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>486</v>
       </c>
       <c r="L22" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="N22" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="N22" s="8" t="s">
-        <v>486</v>
-      </c>
       <c r="O22" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.35">
@@ -5330,28 +5387,28 @@
         <v>253</v>
       </c>
       <c r="H23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I23" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>487</v>
+        <v>608</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="L23" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="M23" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="O23" s="47" t="s">
         <v>487</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="O23" s="47" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.35">
@@ -5371,28 +5428,28 @@
         <v>395</v>
       </c>
       <c r="H24" s="52" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I24" s="69" t="s">
+        <v>489</v>
+      </c>
+      <c r="J24" s="70" t="s">
+        <v>490</v>
+      </c>
+      <c r="K24" s="55" t="s">
         <v>491</v>
       </c>
-      <c r="J24" s="70" t="s">
-        <v>492</v>
-      </c>
-      <c r="K24" s="55" t="s">
-        <v>493</v>
-      </c>
       <c r="L24" s="69" t="s">
+        <v>489</v>
+      </c>
+      <c r="M24" s="70" t="s">
+        <v>490</v>
+      </c>
+      <c r="N24" s="55" t="s">
         <v>491</v>
       </c>
-      <c r="M24" s="70" t="s">
-        <v>492</v>
-      </c>
-      <c r="N24" s="55" t="s">
-        <v>493</v>
-      </c>
       <c r="O24" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.35">
@@ -5412,28 +5469,28 @@
         <v>267</v>
       </c>
       <c r="H25" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>501</v>
+        <v>603</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="L25" s="40" t="s">
-        <v>576</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>501</v>
+        <v>565</v>
+      </c>
+      <c r="M25" s="101" t="s">
+        <v>599</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="O25" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.35">
@@ -5453,28 +5510,28 @@
         <v>268</v>
       </c>
       <c r="H26" s="48" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I26" s="49" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="J26" s="71" t="s">
-        <v>502</v>
+        <v>604</v>
       </c>
       <c r="K26" s="71" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="L26" s="57" t="s">
-        <v>577</v>
-      </c>
-      <c r="M26" s="71" t="s">
-        <v>502</v>
+        <v>566</v>
+      </c>
+      <c r="M26" s="100" t="s">
+        <v>600</v>
       </c>
       <c r="N26" s="71" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="O26" s="72" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.35">
@@ -5494,28 +5551,28 @@
         <v>396</v>
       </c>
       <c r="H27" s="52" t="s">
+        <v>499</v>
+      </c>
+      <c r="I27" s="69" t="s">
+        <v>502</v>
+      </c>
+      <c r="J27" s="70" t="s">
         <v>503</v>
       </c>
-      <c r="I27" s="69" t="s">
-        <v>506</v>
-      </c>
-      <c r="J27" s="70" t="s">
-        <v>507</v>
-      </c>
       <c r="K27" s="55" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="L27" s="69" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="M27" s="70" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="N27" s="55" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="O27" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.35">
@@ -5535,28 +5592,28 @@
         <v>252</v>
       </c>
       <c r="H28" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>509</v>
+        <v>606</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="L28" s="40" t="s">
-        <v>580</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>509</v>
+        <v>569</v>
+      </c>
+      <c r="M28" s="101" t="s">
+        <v>601</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="O28" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.35">
@@ -5576,28 +5633,28 @@
         <v>245</v>
       </c>
       <c r="H29" s="48" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="J29" s="50" t="s">
-        <v>510</v>
+        <v>607</v>
       </c>
       <c r="K29" s="73" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="L29" s="64" t="s">
-        <v>578</v>
-      </c>
-      <c r="M29" s="50" t="s">
-        <v>510</v>
+        <v>567</v>
+      </c>
+      <c r="M29" s="102" t="s">
+        <v>602</v>
       </c>
       <c r="N29" s="73" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="O29" s="72" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.35">
@@ -5617,28 +5674,28 @@
         <v>392</v>
       </c>
       <c r="H30" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="K30" s="81" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>581</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>520</v>
+        <v>570</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>611</v>
       </c>
       <c r="N30" s="81" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="O30" s="60" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.35">
@@ -5658,28 +5715,28 @@
         <v>393</v>
       </c>
       <c r="H31" s="48" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="I31" s="49" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="J31" s="50" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="L31" s="57" t="s">
-        <v>579</v>
-      </c>
-      <c r="M31" s="50" t="s">
-        <v>521</v>
+        <v>568</v>
+      </c>
+      <c r="M31" s="64" t="s">
+        <v>612</v>
       </c>
       <c r="N31" s="82" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="O31" s="72" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.35">
@@ -5699,28 +5756,28 @@
         <v>246</v>
       </c>
       <c r="H32" s="76" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="I32" s="86" t="s">
         <v>461</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="K32" s="55" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="L32" s="86" t="s">
         <v>461</v>
       </c>
       <c r="M32" s="55" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="N32" s="55" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="O32" s="53" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.35">
@@ -5740,28 +5797,28 @@
         <v>364</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="I33" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="L33" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="O33" s="33" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.35">
@@ -5781,28 +5838,28 @@
         <v>249</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="I34" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="L34" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="O34" s="33" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.35">
@@ -5822,28 +5879,28 @@
         <v>250</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="I35" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="L35" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="O35" s="33" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.35">
@@ -5863,25 +5920,25 @@
         <v>251</v>
       </c>
       <c r="H36" s="79" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="I36" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="L36" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="O36" s="47"/>
     </row>
@@ -5902,28 +5959,28 @@
         <v>394</v>
       </c>
       <c r="H37" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="I37" s="54" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="K37" s="55" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="L37" s="69" t="s">
-        <v>590</v>
-      </c>
-      <c r="M37" s="55" t="s">
-        <v>528</v>
+        <v>579</v>
+      </c>
+      <c r="M37" s="70" t="s">
+        <v>522</v>
       </c>
       <c r="N37" s="55" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.35">
@@ -5946,25 +6003,25 @@
         <v>429</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>530</v>
+        <v>614</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="L38" s="40" t="s">
-        <v>591</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>530</v>
+        <v>580</v>
+      </c>
+      <c r="M38" s="26" t="s">
+        <v>613</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="O38" s="60" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.35">
@@ -5998,14 +6055,14 @@
       <c r="L39" s="40" t="s">
         <v>444</v>
       </c>
-      <c r="M39" s="8" t="s">
+      <c r="M39" s="7" t="s">
         <v>444</v>
       </c>
       <c r="N39" s="8" t="s">
         <v>444</v>
       </c>
       <c r="O39" s="33" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.35">
@@ -6025,28 +6082,28 @@
         <v>270</v>
       </c>
       <c r="H40" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="I40" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="L40" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="O40" s="60" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.35">
@@ -6066,28 +6123,28 @@
         <v>360</v>
       </c>
       <c r="H41" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="I41" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="L41" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="O41" s="60" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.35">
@@ -6107,28 +6164,28 @@
         <v>272</v>
       </c>
       <c r="H42" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="I42" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="L42" s="59" t="s">
         <v>461</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="O42" s="60" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.35">
@@ -6148,28 +6205,28 @@
         <v>361</v>
       </c>
       <c r="H43" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="I43" s="83" t="s">
         <v>461</v>
       </c>
       <c r="J43" s="50" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="K43" s="50" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="L43" s="83" t="s">
         <v>461</v>
       </c>
       <c r="M43" s="50" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="O43" s="72" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.35">
@@ -6189,28 +6246,28 @@
         <v>236</v>
       </c>
       <c r="H44" s="76" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="J44" s="55" t="s">
-        <v>546</v>
+        <v>619</v>
       </c>
       <c r="K44" s="55" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="L44" s="69" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="M44" s="55" t="s">
-        <v>546</v>
+        <v>615</v>
       </c>
       <c r="N44" s="55" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="O44" s="60" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
@@ -6230,28 +6287,28 @@
         <v>391</v>
       </c>
       <c r="H45" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>548</v>
+        <v>620</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="L45" s="40" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>548</v>
+        <v>616</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="O45" s="60" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.35">
@@ -6271,28 +6328,28 @@
         <v>390</v>
       </c>
       <c r="H46" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="I46" s="35" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>551</v>
+        <v>621</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="L46" s="40" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>551</v>
+        <v>617</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="O46" s="60" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.35">
@@ -6312,28 +6369,28 @@
         <v>256</v>
       </c>
       <c r="H47" s="48" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="I47" s="49" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="J47" s="50" t="s">
-        <v>552</v>
+        <v>622</v>
       </c>
       <c r="K47" s="50" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="L47" s="57" t="s">
-        <v>602</v>
-      </c>
-      <c r="M47" s="50" t="s">
-        <v>552</v>
+        <v>591</v>
+      </c>
+      <c r="M47" s="64" t="s">
+        <v>618</v>
       </c>
       <c r="N47" s="50" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="O47" s="72" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.35">
@@ -6353,25 +6410,25 @@
         <v>29</v>
       </c>
       <c r="H48" s="52" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="J48" s="55" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="K48" s="84" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="L48" s="97" t="s">
-        <v>606</v>
-      </c>
-      <c r="M48" s="55" t="s">
-        <v>556</v>
+        <v>595</v>
+      </c>
+      <c r="M48" s="103" t="s">
+        <v>623</v>
       </c>
       <c r="N48" s="84" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="O48" s="53" t="s">
         <v>351</v>
@@ -6394,25 +6451,25 @@
         <v>30</v>
       </c>
       <c r="H49" s="48" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="I49" s="49" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="J49" s="50" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="K49" s="85" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="L49" s="98" t="s">
-        <v>607</v>
-      </c>
-      <c r="M49" s="50" t="s">
-        <v>557</v>
+        <v>596</v>
+      </c>
+      <c r="M49" s="104" t="s">
+        <v>624</v>
       </c>
       <c r="N49" s="85" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="O49" s="47" t="s">
         <v>351</v>

</xml_diff>

<commit_message>
added further cleaning steps to Arb.09
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F1BD36-F302-4FB7-B27F-E07FA9E01C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4BB028-1705-42CF-A5F7-7AC743AF2FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
+    <workbookView xWindow="19455" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Secciones_Data" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="631">
   <si>
     <t>Variable</t>
   </si>
@@ -1925,15 +1925,6 @@
     <t>n= 324 (NULL, character)</t>
   </si>
   <si>
-    <t>n= 37 (NA, 999, 9999)</t>
-  </si>
-  <si>
-    <t>n= 124 (NA, 999)</t>
-  </si>
-  <si>
-    <t>n= 104 (NA, 999)</t>
-  </si>
-  <si>
     <t>n= 84 (NA)</t>
   </si>
   <si>
@@ -1953,6 +1944,33 @@
   </si>
   <si>
     <t>n= 63193 (NA)</t>
+  </si>
+  <si>
+    <t>n= 6 (NA)</t>
+  </si>
+  <si>
+    <t>n= 13 (NA)</t>
+  </si>
+  <si>
+    <t>n= 7 (NA)</t>
+  </si>
+  <si>
+    <t>n= 8 (NA, + Posicion recta)</t>
+  </si>
+  <si>
+    <t>n= 8 (NA)</t>
+  </si>
+  <si>
+    <t>n= 9 (NA, + SI)</t>
+  </si>
+  <si>
+    <t>n= 35 (NA)</t>
+  </si>
+  <si>
+    <t>n= 123 (NA)</t>
+  </si>
+  <si>
+    <t>n= 103 (NA)</t>
   </si>
 </sst>
 </file>
@@ -2422,11 +2440,11 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4604,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5117,8 +5135,8 @@
       <c r="L16" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M16" s="55" t="s">
-        <v>460</v>
+      <c r="M16" s="104" t="s">
+        <v>623</v>
       </c>
       <c r="N16" s="7" t="s">
         <v>444</v>
@@ -5161,8 +5179,8 @@
       <c r="L17" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M17" s="8" t="s">
-        <v>466</v>
+      <c r="M17" s="7" t="s">
+        <v>622</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>465</v>
@@ -5483,7 +5501,7 @@
       <c r="L25" s="40" t="s">
         <v>565</v>
       </c>
-      <c r="M25" s="101" t="s">
+      <c r="M25" s="7" t="s">
         <v>599</v>
       </c>
       <c r="N25" s="8" t="s">
@@ -5606,7 +5624,7 @@
       <c r="L28" s="40" t="s">
         <v>569</v>
       </c>
-      <c r="M28" s="101" t="s">
+      <c r="M28" s="7" t="s">
         <v>601</v>
       </c>
       <c r="N28" s="17" t="s">
@@ -5647,7 +5665,7 @@
       <c r="L29" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="M29" s="102" t="s">
+      <c r="M29" s="64" t="s">
         <v>602</v>
       </c>
       <c r="N29" s="73" t="s">
@@ -5770,11 +5788,11 @@
       <c r="L32" s="86" t="s">
         <v>461</v>
       </c>
-      <c r="M32" s="55" t="s">
-        <v>554</v>
-      </c>
-      <c r="N32" s="55" t="s">
-        <v>555</v>
+      <c r="M32" s="70" t="s">
+        <v>624</v>
+      </c>
+      <c r="N32" s="99" t="s">
+        <v>625</v>
       </c>
       <c r="O32" s="53" t="s">
         <v>559</v>
@@ -5811,11 +5829,11 @@
       <c r="L33" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M33" s="8" t="s">
-        <v>556</v>
-      </c>
-      <c r="N33" s="8" t="s">
-        <v>557</v>
+      <c r="M33" s="103" t="s">
+        <v>626</v>
+      </c>
+      <c r="N33" s="26" t="s">
+        <v>627</v>
       </c>
       <c r="O33" s="33" t="s">
         <v>558</v>
@@ -6014,7 +6032,7 @@
       <c r="L38" s="40" t="s">
         <v>580</v>
       </c>
-      <c r="M38" s="26" t="s">
+      <c r="M38" s="103" t="s">
         <v>613</v>
       </c>
       <c r="N38" s="8" t="s">
@@ -6252,7 +6270,7 @@
         <v>581</v>
       </c>
       <c r="J44" s="55" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="K44" s="55" t="s">
         <v>539</v>
@@ -6260,8 +6278,8 @@
       <c r="L44" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="M44" s="55" t="s">
-        <v>615</v>
+      <c r="M44" s="104" t="s">
+        <v>628</v>
       </c>
       <c r="N44" s="55" t="s">
         <v>539</v>
@@ -6293,7 +6311,7 @@
         <v>585</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>540</v>
@@ -6301,8 +6319,8 @@
       <c r="L45" s="40" t="s">
         <v>584</v>
       </c>
-      <c r="M45" s="8" t="s">
-        <v>616</v>
+      <c r="M45" s="103" t="s">
+        <v>629</v>
       </c>
       <c r="N45" s="8" t="s">
         <v>540</v>
@@ -6334,7 +6352,7 @@
         <v>587</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="K46" s="8" t="s">
         <v>541</v>
@@ -6342,8 +6360,8 @@
       <c r="L46" s="40" t="s">
         <v>586</v>
       </c>
-      <c r="M46" s="8" t="s">
-        <v>617</v>
+      <c r="M46" s="103" t="s">
+        <v>630</v>
       </c>
       <c r="N46" s="8" t="s">
         <v>541</v>
@@ -6375,7 +6393,7 @@
         <v>588</v>
       </c>
       <c r="J47" s="50" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="K47" s="50" t="s">
         <v>542</v>
@@ -6384,7 +6402,7 @@
         <v>591</v>
       </c>
       <c r="M47" s="64" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="N47" s="50" t="s">
         <v>542</v>
@@ -6424,8 +6442,8 @@
       <c r="L48" s="97" t="s">
         <v>595</v>
       </c>
-      <c r="M48" s="103" t="s">
-        <v>623</v>
+      <c r="M48" s="101" t="s">
+        <v>620</v>
       </c>
       <c r="N48" s="84" t="s">
         <v>547</v>
@@ -6465,8 +6483,8 @@
       <c r="L49" s="98" t="s">
         <v>596</v>
       </c>
-      <c r="M49" s="104" t="s">
-        <v>624</v>
+      <c r="M49" s="102" t="s">
+        <v>621</v>
       </c>
       <c r="N49" s="85" t="s">
         <v>548</v>

</xml_diff>

<commit_message>
added preliminary final cleaning to Arb.09
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4BB028-1705-42CF-A5F7-7AC743AF2FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A9BEA4-75FD-440F-AE36-047D6FC7BE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19455" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="637">
   <si>
     <t>Variable</t>
   </si>
@@ -1622,12 +1622,6 @@
     </r>
   </si>
   <si>
-    <t>n= 2599 (NULL, Character)</t>
-  </si>
-  <si>
-    <t>n= 1699 (NULL, Character)</t>
-  </si>
-  <si>
     <t>missing values == NA, numeric</t>
   </si>
   <si>
@@ -1742,15 +1736,9 @@
     <t>Estimate the severity of recent tree stress. Estimate this variable as a percentage of the live crown area, including the area with dieback.</t>
   </si>
   <si>
-    <t>n= 7 (NULL)</t>
-  </si>
-  <si>
     <t>n= 9 (No aplicacion = no aplica, no capturado + Posicion recta)</t>
   </si>
   <si>
-    <t>n= 8 (NULL)</t>
-  </si>
-  <si>
     <t>n= 9 (No capturado, SI)</t>
   </si>
   <si>
@@ -1871,12 +1859,6 @@
     <t>n= 58436 (NA)</t>
   </si>
   <si>
-    <t>n= 131 (NA)</t>
-  </si>
-  <si>
-    <t>n= 60, because of inceonsequent naming (NA)</t>
-  </si>
-  <si>
     <t>n= 1712 (NA, "numeric")</t>
   </si>
   <si>
@@ -1913,12 +1895,6 @@
     <t>n= 2667 (NA, "numeric")</t>
   </si>
   <si>
-    <t>n= 2599 (NA, Character)</t>
-  </si>
-  <si>
-    <t>n= 1699 (NA, Character)</t>
-  </si>
-  <si>
     <t>n= 324 (NA,  character)</t>
   </si>
   <si>
@@ -1958,9 +1934,6 @@
     <t>n= 8 (NA, + Posicion recta)</t>
   </si>
   <si>
-    <t>n= 8 (NA)</t>
-  </si>
-  <si>
     <t>n= 9 (NA, + SI)</t>
   </si>
   <si>
@@ -1971,6 +1944,51 @@
   </si>
   <si>
     <t>n= 103 (NA)</t>
+  </si>
+  <si>
+    <t>n= 44 (NA)</t>
+  </si>
+  <si>
+    <t>n= 41 (NA)</t>
+  </si>
+  <si>
+    <t>n= 26 (NA)</t>
+  </si>
+  <si>
+    <t>n= 25 (NA, missing 85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n= 131 </t>
+  </si>
+  <si>
+    <t>n= 2599 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1699 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 2599 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 1699 (NULL, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 7 (NULL + No aplica)</t>
+  </si>
+  <si>
+    <t>n= 8 (NULL + No aplica)</t>
+  </si>
+  <si>
+    <t>no aplica check</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>n= 22 (NA + ranges, "character")</t>
+  </si>
+  <si>
+    <t>n= 22  (NA + ranges, "character")</t>
   </si>
 </sst>
 </file>
@@ -2141,7 +2159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2305,11 +2323,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2444,7 +2475,17 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4622,8 +4663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4669,7 +4710,7 @@
       </c>
       <c r="N3" s="43"/>
       <c r="O3" s="87" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.35">
@@ -4935,7 +4976,7 @@
         <v>449</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.35">
@@ -4979,7 +5020,7 @@
         <v>417</v>
       </c>
       <c r="P12" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.35">
@@ -5053,16 +5094,16 @@
         <v>459</v>
       </c>
       <c r="L14" s="69" t="s">
-        <v>594</v>
-      </c>
-      <c r="M14" s="99" t="s">
-        <v>597</v>
+        <v>590</v>
+      </c>
+      <c r="M14" s="105" t="s">
+        <v>626</v>
       </c>
       <c r="N14" s="55" t="s">
         <v>459</v>
       </c>
       <c r="O14" s="53" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.35">
@@ -5092,16 +5133,16 @@
         <v>459</v>
       </c>
       <c r="L15" s="57" t="s">
-        <v>594</v>
-      </c>
-      <c r="M15" s="26" t="s">
-        <v>598</v>
+        <v>590</v>
+      </c>
+      <c r="M15" s="103" t="s">
+        <v>458</v>
       </c>
       <c r="N15" s="50" t="s">
         <v>459</v>
       </c>
       <c r="O15" s="53" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.35">
@@ -5135,8 +5176,8 @@
       <c r="L16" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M16" s="104" t="s">
-        <v>623</v>
+      <c r="M16" s="70" t="s">
+        <v>615</v>
       </c>
       <c r="N16" s="7" t="s">
         <v>444</v>
@@ -5180,13 +5221,13 @@
         <v>461</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>465</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
@@ -5227,7 +5268,7 @@
         <v>469</v>
       </c>
       <c r="O18" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
@@ -5262,7 +5303,7 @@
       <c r="M19" s="63"/>
       <c r="N19" s="63"/>
       <c r="O19" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
@@ -5303,7 +5344,7 @@
         <v>481</v>
       </c>
       <c r="O20" s="66" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.35">
@@ -5370,7 +5411,7 @@
         <v>461</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>485</v>
@@ -5379,13 +5420,13 @@
         <v>461</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="N22" s="8" t="s">
         <v>485</v>
       </c>
       <c r="O22" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.35">
@@ -5411,7 +5452,7 @@
         <v>461</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>486</v>
@@ -5420,7 +5461,7 @@
         <v>461</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="N23" s="8" t="s">
         <v>486</v>
@@ -5467,7 +5508,7 @@
         <v>491</v>
       </c>
       <c r="O24" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.35">
@@ -5493,22 +5534,22 @@
         <v>497</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>496</v>
       </c>
       <c r="L25" s="40" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="N25" s="8" t="s">
         <v>496</v>
       </c>
       <c r="O25" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.35">
@@ -5534,22 +5575,22 @@
         <v>498</v>
       </c>
       <c r="J26" s="71" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="K26" s="71" t="s">
         <v>495</v>
       </c>
       <c r="L26" s="57" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="M26" s="100" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="N26" s="71" t="s">
         <v>495</v>
       </c>
       <c r="O26" s="72" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.35">
@@ -5590,7 +5631,7 @@
         <v>504</v>
       </c>
       <c r="O27" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.35">
@@ -5613,25 +5654,25 @@
         <v>501</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>506</v>
       </c>
       <c r="L28" s="40" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="N28" s="17" t="s">
         <v>506</v>
       </c>
       <c r="O28" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.35">
@@ -5654,25 +5695,25 @@
         <v>500</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="J29" s="50" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="K29" s="73" t="s">
         <v>505</v>
       </c>
       <c r="L29" s="64" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="M29" s="64" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="N29" s="73" t="s">
         <v>505</v>
       </c>
       <c r="O29" s="72" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.35">
@@ -5692,28 +5733,28 @@
         <v>392</v>
       </c>
       <c r="H30" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>514</v>
+        <v>629</v>
       </c>
       <c r="K30" s="81" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>611</v>
+        <v>627</v>
       </c>
       <c r="N30" s="81" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="O30" s="60" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.35">
@@ -5733,28 +5774,28 @@
         <v>393</v>
       </c>
       <c r="H31" s="48" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I31" s="49" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="J31" s="50" t="s">
-        <v>515</v>
+        <v>630</v>
       </c>
       <c r="K31" s="82" t="s">
         <v>505</v>
       </c>
       <c r="L31" s="57" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="M31" s="64" t="s">
-        <v>612</v>
+        <v>628</v>
       </c>
       <c r="N31" s="82" t="s">
         <v>505</v>
       </c>
       <c r="O31" s="72" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.35">
@@ -5774,28 +5815,28 @@
         <v>246</v>
       </c>
       <c r="H32" s="76" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="I32" s="86" t="s">
         <v>461</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>554</v>
+        <v>631</v>
       </c>
       <c r="K32" s="55" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="L32" s="86" t="s">
         <v>461</v>
       </c>
       <c r="M32" s="70" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="N32" s="99" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="O32" s="53" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.35">
@@ -5815,28 +5856,28 @@
         <v>364</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="I33" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>556</v>
+        <v>632</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="L33" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M33" s="103" t="s">
-        <v>626</v>
+      <c r="M33" s="7" t="s">
+        <v>616</v>
       </c>
       <c r="N33" s="26" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="O33" s="33" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.35">
@@ -5856,28 +5897,28 @@
         <v>249</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I34" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="L34" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M34" s="8" t="s">
-        <v>561</v>
+      <c r="M34" s="7" t="s">
+        <v>635</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="O34" s="33" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.35">
@@ -5897,28 +5938,28 @@
         <v>250</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="I35" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="L35" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M35" s="8" t="s">
-        <v>561</v>
+      <c r="M35" s="103" t="s">
+        <v>636</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="O35" s="33" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.35">
@@ -5938,25 +5979,25 @@
         <v>251</v>
       </c>
       <c r="H36" s="79" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I36" s="59" t="s">
         <v>461</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="L36" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M36" s="8" t="s">
-        <v>561</v>
+      <c r="M36" s="103" t="s">
+        <v>636</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="O36" s="47"/>
     </row>
@@ -5977,28 +6018,28 @@
         <v>394</v>
       </c>
       <c r="H37" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I37" s="54" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="K37" s="55" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="L37" s="69" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="M37" s="70" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="N37" s="55" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.35">
@@ -6021,25 +6062,25 @@
         <v>429</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="L38" s="40" t="s">
-        <v>580</v>
-      </c>
-      <c r="M38" s="103" t="s">
-        <v>613</v>
+        <v>576</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>605</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="O38" s="60" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.35">
@@ -6080,7 +6121,7 @@
         <v>444</v>
       </c>
       <c r="O39" s="33" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.35">
@@ -6106,22 +6147,22 @@
         <v>461</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="L40" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M40" s="8" t="s">
+      <c r="M40" s="103" t="s">
+        <v>622</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="O40" s="60" t="s">
         <v>526</v>
-      </c>
-      <c r="N40" s="8" t="s">
-        <v>527</v>
-      </c>
-      <c r="O40" s="60" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.35">
@@ -6147,22 +6188,22 @@
         <v>461</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="L41" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M41" s="8" t="s">
-        <v>529</v>
+      <c r="M41" s="7" t="s">
+        <v>624</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O41" s="60" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.35">
@@ -6188,22 +6229,22 @@
         <v>461</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="L42" s="59" t="s">
         <v>461</v>
       </c>
-      <c r="M42" s="8" t="s">
-        <v>534</v>
+      <c r="M42" s="103" t="s">
+        <v>623</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="O42" s="60" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.35">
@@ -6229,22 +6270,22 @@
         <v>461</v>
       </c>
       <c r="J43" s="50" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K43" s="50" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="L43" s="83" t="s">
         <v>461</v>
       </c>
-      <c r="M43" s="50" t="s">
-        <v>531</v>
+      <c r="M43" s="104" t="s">
+        <v>625</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="O43" s="72" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.35">
@@ -6264,28 +6305,28 @@
         <v>236</v>
       </c>
       <c r="H44" s="76" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="J44" s="55" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="K44" s="55" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="L44" s="69" t="s">
-        <v>583</v>
-      </c>
-      <c r="M44" s="104" t="s">
-        <v>628</v>
+        <v>579</v>
+      </c>
+      <c r="M44" s="70" t="s">
+        <v>619</v>
       </c>
       <c r="N44" s="55" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O44" s="60" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
@@ -6305,28 +6346,28 @@
         <v>391</v>
       </c>
       <c r="H45" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L45" s="40" t="s">
-        <v>584</v>
-      </c>
-      <c r="M45" s="103" t="s">
-        <v>629</v>
+        <v>580</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>620</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="O45" s="60" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.35">
@@ -6346,28 +6387,28 @@
         <v>390</v>
       </c>
       <c r="H46" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="I46" s="35" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="L46" s="40" t="s">
-        <v>586</v>
-      </c>
-      <c r="M46" s="103" t="s">
-        <v>630</v>
+        <v>582</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>621</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="O46" s="60" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.35">
@@ -6387,28 +6428,28 @@
         <v>256</v>
       </c>
       <c r="H47" s="48" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I47" s="49" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="J47" s="50" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="K47" s="50" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L47" s="57" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="M47" s="64" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="N47" s="50" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="O47" s="72" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.35">
@@ -6431,22 +6472,22 @@
         <v>507</v>
       </c>
       <c r="I48" s="54" t="s">
+        <v>541</v>
+      </c>
+      <c r="J48" s="55" t="s">
         <v>543</v>
       </c>
-      <c r="J48" s="55" t="s">
+      <c r="K48" s="84" t="s">
         <v>545</v>
       </c>
-      <c r="K48" s="84" t="s">
-        <v>547</v>
-      </c>
       <c r="L48" s="97" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="M48" s="101" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="N48" s="84" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="O48" s="53" t="s">
         <v>351</v>
@@ -6472,22 +6513,22 @@
         <v>508</v>
       </c>
       <c r="I49" s="49" t="s">
+        <v>542</v>
+      </c>
+      <c r="J49" s="50" t="s">
         <v>544</v>
       </c>
-      <c r="J49" s="50" t="s">
+      <c r="K49" s="85" t="s">
         <v>546</v>
       </c>
-      <c r="K49" s="85" t="s">
-        <v>548</v>
-      </c>
       <c r="L49" s="98" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="M49" s="102" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="N49" s="85" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="O49" s="47" t="s">
         <v>351</v>
@@ -6569,8 +6610,16 @@
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.35">
       <c r="I52" s="33"/>
-      <c r="L52" s="33"/>
-      <c r="O52" s="33"/>
+      <c r="L52" s="108" t="s">
+        <v>634</v>
+      </c>
+      <c r="M52" s="106" t="s">
+        <v>634</v>
+      </c>
+      <c r="N52" s="107"/>
+      <c r="O52" s="33" t="s">
+        <v>633</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
added all cleaning steps to Arb.14
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A9BEA4-75FD-440F-AE36-047D6FC7BE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDC2758-466A-4E06-B4DA-7B500F348B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19455" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Secciones_Data" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="656">
   <si>
     <t>Variable</t>
   </si>
@@ -1422,9 +1422,6 @@
     </r>
   </si>
   <si>
-    <t>maybe cut it from ds?</t>
-  </si>
-  <si>
     <t>n= 133</t>
   </si>
   <si>
@@ -1525,9 +1522,6 @@
     <t>n= 1275, 999991.00</t>
   </si>
   <si>
-    <t>n= 363 (2 values for NA)</t>
-  </si>
-  <si>
     <t>n= 362 (360, 0, NA) + class numeric</t>
   </si>
   <si>
@@ -1538,9 +1532,6 @@
   </si>
   <si>
     <t>n= 401</t>
-  </si>
-  <si>
-    <t>n= 1674</t>
   </si>
   <si>
     <t>height in meters of the entire tree</t>
@@ -1664,15 +1655,9 @@
     <t>n= 30 (NULL, n/a, -9999, 05, "")</t>
   </si>
   <si>
-    <t>n= 27 (no aplica, no capturado)</t>
-  </si>
-  <si>
     <t>n= 29 (NULL, n/a, -9999, 05, "", missing 85)</t>
   </si>
   <si>
-    <t>n= 25(no aplica, no capturado, missing 75, missing 95)</t>
-  </si>
-  <si>
     <t>n= 39 (no definido, no capturado)</t>
   </si>
   <si>
@@ -1931,12 +1916,6 @@
     <t>n= 7 (NA)</t>
   </si>
   <si>
-    <t>n= 8 (NA, + Posicion recta)</t>
-  </si>
-  <si>
-    <t>n= 9 (NA, + SI)</t>
-  </si>
-  <si>
     <t>n= 35 (NA)</t>
   </si>
   <si>
@@ -1985,10 +1964,88 @@
     <t>x</t>
   </si>
   <si>
-    <t>n= 22 (NA + ranges, "character")</t>
-  </si>
-  <si>
-    <t>n= 22  (NA + ranges, "character")</t>
+    <t>n= 1275 (NA)</t>
+  </si>
+  <si>
+    <t>n= 363 (NA, 999993)</t>
+  </si>
+  <si>
+    <t>n= 362 (NA)</t>
+  </si>
+  <si>
+    <t>n= 1674 (999993)</t>
+  </si>
+  <si>
+    <t>n= 1674 (NA)</t>
+  </si>
+  <si>
+    <t>n= 1186 (NA)</t>
+  </si>
+  <si>
+    <t>n= 1282 (NA)</t>
+  </si>
+  <si>
+    <t>n= 1032 (NA)</t>
+  </si>
+  <si>
+    <t>n= 1324 (NA)</t>
+  </si>
+  <si>
+    <t>n= 2254 (NA)</t>
+  </si>
+  <si>
+    <t>n= 11 (NA + kept "Indeterminante" -&gt; different things imo)</t>
+  </si>
+  <si>
+    <t>n= 7 (NA, + Posicion recta)</t>
+  </si>
+  <si>
+    <t>n= 8 (NA, + SI)</t>
+  </si>
+  <si>
+    <t>n= 22 (NA, sin parametro + ranges)</t>
+  </si>
+  <si>
+    <t>n= 22 (NA, sin parámetro + ranges, "character")</t>
+  </si>
+  <si>
+    <t>n= 22 (NA , sin párametro + ranges, "character")</t>
+  </si>
+  <si>
+    <t>n= 22 (NA, sin parámetroa + ranges, "character")</t>
+  </si>
+  <si>
+    <t>n= 22 (NA, 42309, 44682, 44840 instead of 1-15,  sin parametro + ranges)</t>
+  </si>
+  <si>
+    <t>n= 190 (NA)</t>
+  </si>
+  <si>
+    <t>n= 27 (no aplica, no capturado, "character")</t>
+  </si>
+  <si>
+    <t>n= 25(no aplica, no capturado, missing 75, missing 95, "character")</t>
+  </si>
+  <si>
+    <t>n= 39 (NA, no definido)</t>
+  </si>
+  <si>
+    <t>n= 24 (NA, missing 75, missing 95, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 26 (NA, "numeric")</t>
+  </si>
+  <si>
+    <t>n= 225 (NA)</t>
+  </si>
+  <si>
+    <t>n= 151 (NA)</t>
+  </si>
+  <si>
+    <t>n= 117 (NA)</t>
+  </si>
+  <si>
+    <t>n= 92 (NA)</t>
   </si>
 </sst>
 </file>
@@ -2340,7 +2397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2470,20 +2527,21 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4663,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4690,27 +4748,27 @@
       </c>
       <c r="N1" s="61"/>
       <c r="O1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2" spans="3:16" x14ac:dyDescent="0.35">
       <c r="I2" s="8"/>
       <c r="J2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="N2" s="63"/>
       <c r="O2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.35">
       <c r="I3" s="6"/>
       <c r="J3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N3" s="43"/>
       <c r="O3" s="87" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.35">
@@ -4976,7 +5034,7 @@
         <v>449</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.35">
@@ -5020,7 +5078,7 @@
         <v>417</v>
       </c>
       <c r="P12" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.35">
@@ -5063,9 +5121,7 @@
       <c r="O13" s="44" t="s">
         <v>453</v>
       </c>
-      <c r="P13" s="43" t="s">
-        <v>456</v>
-      </c>
+      <c r="P13" s="43"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C14" s="29">
@@ -5085,25 +5141,25 @@
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="54" t="s">
+        <v>456</v>
+      </c>
+      <c r="J14" s="55" t="s">
         <v>457</v>
       </c>
-      <c r="J14" s="55" t="s">
+      <c r="K14" s="70" t="s">
         <v>458</v>
       </c>
-      <c r="K14" s="55" t="s">
-        <v>459</v>
-      </c>
       <c r="L14" s="69" t="s">
-        <v>590</v>
-      </c>
-      <c r="M14" s="105" t="s">
-        <v>626</v>
-      </c>
-      <c r="N14" s="55" t="s">
-        <v>459</v>
+        <v>585</v>
+      </c>
+      <c r="M14" s="70" t="s">
+        <v>619</v>
+      </c>
+      <c r="N14" s="70" t="s">
+        <v>458</v>
       </c>
       <c r="O14" s="53" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.35">
@@ -5124,25 +5180,25 @@
       </c>
       <c r="H15" s="48"/>
       <c r="I15" s="49" t="s">
+        <v>469</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="K15" s="50" t="s">
-        <v>459</v>
+      <c r="K15" s="64" t="s">
+        <v>458</v>
       </c>
       <c r="L15" s="57" t="s">
-        <v>590</v>
-      </c>
-      <c r="M15" s="103" t="s">
+        <v>585</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="N15" s="64" t="s">
         <v>458</v>
       </c>
-      <c r="N15" s="50" t="s">
-        <v>459</v>
-      </c>
       <c r="O15" s="53" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.35">
@@ -5162,31 +5218,31 @@
         <v>237</v>
       </c>
       <c r="H16" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I16" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J16" s="55" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>444</v>
       </c>
       <c r="L16" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M16" s="70" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="N16" s="7" t="s">
         <v>444</v>
       </c>
       <c r="O16" s="60" t="s">
+        <v>462</v>
+      </c>
+      <c r="P16" s="14" t="s">
         <v>463</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.35">
@@ -5206,28 +5262,28 @@
         <v>238</v>
       </c>
       <c r="H17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I17" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="L17" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
@@ -5250,25 +5306,25 @@
         <v>411</v>
       </c>
       <c r="I18" s="62" t="s">
+        <v>466</v>
+      </c>
+      <c r="J18" s="63" t="s">
         <v>467</v>
       </c>
-      <c r="J18" s="63" t="s">
+      <c r="K18" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="K18" s="63" t="s">
-        <v>469</v>
-      </c>
       <c r="L18" s="62" t="s">
+        <v>466</v>
+      </c>
+      <c r="M18" s="63" t="s">
         <v>467</v>
       </c>
-      <c r="M18" s="63" t="s">
+      <c r="N18" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="N18" s="63" t="s">
-        <v>469</v>
-      </c>
       <c r="O18" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
@@ -5291,19 +5347,19 @@
         <v>412</v>
       </c>
       <c r="I19" s="62" t="s">
+        <v>473</v>
+      </c>
+      <c r="J19" s="63" t="s">
         <v>474</v>
       </c>
-      <c r="J19" s="63" t="s">
+      <c r="K19" s="63" t="s">
         <v>475</v>
-      </c>
-      <c r="K19" s="63" t="s">
-        <v>476</v>
       </c>
       <c r="L19" s="62"/>
       <c r="M19" s="63"/>
       <c r="N19" s="63"/>
       <c r="O19" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
@@ -5326,25 +5382,25 @@
         <v>430</v>
       </c>
       <c r="I20" s="66" t="s">
+        <v>478</v>
+      </c>
+      <c r="J20" s="67" t="s">
         <v>479</v>
       </c>
-      <c r="J20" s="67" t="s">
+      <c r="K20" s="67" t="s">
         <v>480</v>
       </c>
-      <c r="K20" s="67" t="s">
-        <v>481</v>
-      </c>
       <c r="L20" s="66" t="s">
+        <v>478</v>
+      </c>
+      <c r="M20" s="67" t="s">
         <v>479</v>
       </c>
-      <c r="M20" s="67" t="s">
+      <c r="N20" s="67" t="s">
         <v>480</v>
       </c>
-      <c r="N20" s="67" t="s">
-        <v>481</v>
-      </c>
       <c r="O20" s="66" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.35">
@@ -5367,25 +5423,25 @@
         <v>415</v>
       </c>
       <c r="I21" s="57" t="s">
+        <v>481</v>
+      </c>
+      <c r="J21" s="64" t="s">
+        <v>481</v>
+      </c>
+      <c r="K21" s="50" t="s">
         <v>482</v>
       </c>
-      <c r="J21" s="64" t="s">
-        <v>482</v>
-      </c>
-      <c r="K21" s="50" t="s">
-        <v>483</v>
-      </c>
       <c r="L21" s="57" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M21" s="64" t="s">
-        <v>482</v>
-      </c>
-      <c r="N21" s="50" t="s">
-        <v>483</v>
+        <v>481</v>
+      </c>
+      <c r="N21" s="64" t="s">
+        <v>638</v>
       </c>
       <c r="O21" s="47" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.35">
@@ -5405,28 +5461,28 @@
         <v>362</v>
       </c>
       <c r="H22" t="s">
+        <v>483</v>
+      </c>
+      <c r="I22" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="I22" s="59" t="s">
-        <v>461</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>603</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>485</v>
-      </c>
       <c r="L22" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>604</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>485</v>
+        <v>599</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>628</v>
       </c>
       <c r="O22" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.35">
@@ -5446,28 +5502,28 @@
         <v>253</v>
       </c>
       <c r="H23" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I23" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>486</v>
+        <v>629</v>
       </c>
       <c r="L23" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>599</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>486</v>
+        <v>594</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>630</v>
       </c>
       <c r="O23" s="47" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.35">
@@ -5487,28 +5543,28 @@
         <v>395</v>
       </c>
       <c r="H24" s="52" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I24" s="69" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J24" s="70" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>491</v>
+        <v>631</v>
       </c>
       <c r="L24" s="69" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="M24" s="70" t="s">
-        <v>490</v>
-      </c>
-      <c r="N24" s="55" t="s">
-        <v>491</v>
+        <v>488</v>
+      </c>
+      <c r="N24" s="70" t="s">
+        <v>632</v>
       </c>
       <c r="O24" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.35">
@@ -5528,28 +5584,28 @@
         <v>267</v>
       </c>
       <c r="H25" t="s">
+        <v>490</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="K25" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="I25" s="35" t="s">
-        <v>497</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>597</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>496</v>
-      </c>
       <c r="L25" s="40" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>593</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>496</v>
+        <v>588</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>633</v>
       </c>
       <c r="O25" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.35">
@@ -5569,28 +5625,28 @@
         <v>268</v>
       </c>
       <c r="H26" s="48" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I26" s="49" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="J26" s="71" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="K26" s="71" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="L26" s="57" t="s">
-        <v>562</v>
-      </c>
-      <c r="M26" s="100" t="s">
-        <v>594</v>
-      </c>
-      <c r="N26" s="71" t="s">
-        <v>495</v>
+        <v>557</v>
+      </c>
+      <c r="M26" s="99" t="s">
+        <v>589</v>
+      </c>
+      <c r="N26" s="99" t="s">
+        <v>634</v>
       </c>
       <c r="O26" s="72" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.35">
@@ -5610,28 +5666,28 @@
         <v>396</v>
       </c>
       <c r="H27" s="52" t="s">
+        <v>496</v>
+      </c>
+      <c r="I27" s="69" t="s">
         <v>499</v>
       </c>
-      <c r="I27" s="69" t="s">
-        <v>502</v>
-      </c>
       <c r="J27" s="70" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="K27" s="55" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="L27" s="69" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="M27" s="70" t="s">
-        <v>503</v>
-      </c>
-      <c r="N27" s="55" t="s">
-        <v>504</v>
+        <v>500</v>
+      </c>
+      <c r="N27" s="70" t="s">
+        <v>634</v>
       </c>
       <c r="O27" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.35">
@@ -5651,28 +5707,28 @@
         <v>252</v>
       </c>
       <c r="H28" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="L28" s="40" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>595</v>
-      </c>
-      <c r="N28" s="17" t="s">
-        <v>506</v>
+        <v>590</v>
+      </c>
+      <c r="N28" s="16" t="s">
+        <v>635</v>
       </c>
       <c r="O28" s="60" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.35">
@@ -5692,28 +5748,28 @@
         <v>245</v>
       </c>
       <c r="H29" s="48" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="J29" s="50" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="K29" s="73" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="L29" s="64" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="M29" s="64" t="s">
-        <v>596</v>
-      </c>
-      <c r="N29" s="73" t="s">
-        <v>505</v>
+        <v>591</v>
+      </c>
+      <c r="N29" s="104" t="s">
+        <v>636</v>
       </c>
       <c r="O29" s="72" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.35">
@@ -5733,28 +5789,28 @@
         <v>392</v>
       </c>
       <c r="H30" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="K30" s="81" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="N30" s="81" t="s">
-        <v>515</v>
+        <v>620</v>
+      </c>
+      <c r="N30" s="105" t="s">
+        <v>637</v>
       </c>
       <c r="O30" s="60" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.35">
@@ -5774,28 +5830,28 @@
         <v>393</v>
       </c>
       <c r="H31" s="48" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I31" s="49" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="J31" s="50" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="L31" s="57" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="M31" s="64" t="s">
-        <v>628</v>
-      </c>
-      <c r="N31" s="82" t="s">
-        <v>505</v>
+        <v>621</v>
+      </c>
+      <c r="N31" s="106" t="s">
+        <v>636</v>
       </c>
       <c r="O31" s="72" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.35">
@@ -5815,28 +5871,28 @@
         <v>246</v>
       </c>
       <c r="H32" s="76" t="s">
+        <v>542</v>
+      </c>
+      <c r="I32" s="86" t="s">
+        <v>460</v>
+      </c>
+      <c r="J32" s="55" t="s">
+        <v>624</v>
+      </c>
+      <c r="K32" s="55" t="s">
         <v>547</v>
       </c>
-      <c r="I32" s="86" t="s">
-        <v>461</v>
-      </c>
-      <c r="J32" s="55" t="s">
-        <v>631</v>
-      </c>
-      <c r="K32" s="55" t="s">
-        <v>552</v>
-      </c>
       <c r="L32" s="86" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M32" s="70" t="s">
-        <v>614</v>
-      </c>
-      <c r="N32" s="99" t="s">
-        <v>617</v>
+        <v>609</v>
+      </c>
+      <c r="N32" s="107" t="s">
+        <v>639</v>
       </c>
       <c r="O32" s="53" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.35">
@@ -5856,28 +5912,28 @@
         <v>364</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="I33" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="L33" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>616</v>
-      </c>
-      <c r="N33" s="26" t="s">
-        <v>618</v>
+        <v>611</v>
+      </c>
+      <c r="N33" s="108" t="s">
+        <v>640</v>
       </c>
       <c r="O33" s="33" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.35">
@@ -5897,28 +5953,28 @@
         <v>249</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="I34" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="L34" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>556</v>
+        <v>644</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>641</v>
       </c>
       <c r="O34" s="33" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.35">
@@ -5938,28 +5994,28 @@
         <v>250</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="I35" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="L35" s="59" t="s">
-        <v>461</v>
-      </c>
-      <c r="M35" s="103" t="s">
-        <v>636</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>556</v>
+        <v>460</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>641</v>
       </c>
       <c r="O35" s="33" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.35">
@@ -5979,25 +6035,25 @@
         <v>251</v>
       </c>
       <c r="H36" s="79" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="I36" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="L36" s="59" t="s">
-        <v>461</v>
-      </c>
-      <c r="M36" s="103" t="s">
-        <v>636</v>
-      </c>
-      <c r="N36" s="8" t="s">
-        <v>559</v>
+        <v>460</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>645</v>
       </c>
       <c r="O36" s="47"/>
     </row>
@@ -6018,28 +6074,28 @@
         <v>394</v>
       </c>
       <c r="H37" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I37" s="54" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="K37" s="55" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="L37" s="69" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="M37" s="70" t="s">
-        <v>520</v>
-      </c>
-      <c r="N37" s="55" t="s">
-        <v>520</v>
+        <v>570</v>
+      </c>
+      <c r="N37" s="70" t="s">
+        <v>570</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.35">
@@ -6062,25 +6118,25 @@
         <v>429</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="L38" s="40" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>605</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>521</v>
+        <v>600</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>646</v>
       </c>
       <c r="O38" s="60" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.35">
@@ -6108,7 +6164,7 @@
       <c r="J39" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="K39" s="8" t="s">
+      <c r="K39" s="7" t="s">
         <v>444</v>
       </c>
       <c r="L39" s="40" t="s">
@@ -6117,11 +6173,11 @@
       <c r="M39" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="N39" s="8" t="s">
+      <c r="N39" s="7" t="s">
         <v>444</v>
       </c>
       <c r="O39" s="33" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.35">
@@ -6141,28 +6197,28 @@
         <v>270</v>
       </c>
       <c r="H40" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="I40" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="L40" s="59" t="s">
-        <v>461</v>
-      </c>
-      <c r="M40" s="103" t="s">
-        <v>622</v>
-      </c>
-      <c r="N40" s="8" t="s">
-        <v>525</v>
+        <v>460</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>522</v>
       </c>
       <c r="O40" s="60" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.35">
@@ -6182,28 +6238,28 @@
         <v>360</v>
       </c>
       <c r="H41" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="I41" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>528</v>
+        <v>647</v>
       </c>
       <c r="L41" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>624</v>
-      </c>
-      <c r="N41" s="8" t="s">
-        <v>528</v>
+        <v>617</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>651</v>
       </c>
       <c r="O41" s="60" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.35">
@@ -6223,28 +6279,28 @@
         <v>272</v>
       </c>
       <c r="H42" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="I42" s="59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="L42" s="59" t="s">
-        <v>461</v>
-      </c>
-      <c r="M42" s="103" t="s">
-        <v>623</v>
-      </c>
-      <c r="N42" s="8" t="s">
-        <v>531</v>
+        <v>460</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>649</v>
       </c>
       <c r="O42" s="60" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.35">
@@ -6264,28 +6320,28 @@
         <v>361</v>
       </c>
       <c r="H43" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="I43" s="83" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J43" s="50" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="K43" s="50" t="s">
-        <v>530</v>
+        <v>648</v>
       </c>
       <c r="L43" s="83" t="s">
-        <v>461</v>
-      </c>
-      <c r="M43" s="104" t="s">
-        <v>625</v>
-      </c>
-      <c r="N43" s="50" t="s">
-        <v>530</v>
+        <v>460</v>
+      </c>
+      <c r="M43" s="64" t="s">
+        <v>618</v>
+      </c>
+      <c r="N43" s="64" t="s">
+        <v>650</v>
       </c>
       <c r="O43" s="72" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.35">
@@ -6305,28 +6361,28 @@
         <v>236</v>
       </c>
       <c r="H44" s="76" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="J44" s="55" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="K44" s="55" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="L44" s="69" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="M44" s="70" t="s">
-        <v>619</v>
-      </c>
-      <c r="N44" s="55" t="s">
-        <v>537</v>
+        <v>612</v>
+      </c>
+      <c r="N44" s="70" t="s">
+        <v>652</v>
       </c>
       <c r="O44" s="60" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
@@ -6346,28 +6402,28 @@
         <v>391</v>
       </c>
       <c r="H45" t="s">
+        <v>528</v>
+      </c>
+      <c r="I45" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="K45" s="8" t="s">
         <v>533</v>
       </c>
-      <c r="I45" s="35" t="s">
+      <c r="L45" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="O45" s="60" t="s">
         <v>581</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>609</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="L45" s="40" t="s">
-        <v>580</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>620</v>
-      </c>
-      <c r="N45" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="O45" s="60" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.35">
@@ -6387,28 +6443,28 @@
         <v>390</v>
       </c>
       <c r="H46" t="s">
+        <v>529</v>
+      </c>
+      <c r="I46" s="35" t="s">
+        <v>578</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="K46" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="I46" s="35" t="s">
-        <v>583</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>610</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>539</v>
-      </c>
       <c r="L46" s="40" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>539</v>
+        <v>614</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>654</v>
       </c>
       <c r="O46" s="60" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.35">
@@ -6428,28 +6484,28 @@
         <v>256</v>
       </c>
       <c r="H47" s="48" t="s">
+        <v>530</v>
+      </c>
+      <c r="I47" s="49" t="s">
+        <v>579</v>
+      </c>
+      <c r="J47" s="50" t="s">
+        <v>606</v>
+      </c>
+      <c r="K47" s="50" t="s">
         <v>535</v>
       </c>
-      <c r="I47" s="49" t="s">
-        <v>584</v>
-      </c>
-      <c r="J47" s="50" t="s">
-        <v>611</v>
-      </c>
-      <c r="K47" s="50" t="s">
-        <v>540</v>
-      </c>
       <c r="L47" s="57" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="M47" s="64" t="s">
-        <v>607</v>
-      </c>
-      <c r="N47" s="50" t="s">
-        <v>540</v>
+        <v>602</v>
+      </c>
+      <c r="N47" s="64" t="s">
+        <v>655</v>
       </c>
       <c r="O47" s="72" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="3:15" x14ac:dyDescent="0.35">
@@ -6469,25 +6525,25 @@
         <v>29</v>
       </c>
       <c r="H48" s="52" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="J48" s="55" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="K48" s="84" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="L48" s="97" t="s">
-        <v>591</v>
-      </c>
-      <c r="M48" s="101" t="s">
-        <v>612</v>
+        <v>586</v>
+      </c>
+      <c r="M48" s="100" t="s">
+        <v>607</v>
       </c>
       <c r="N48" s="84" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="O48" s="53" t="s">
         <v>351</v>
@@ -6510,25 +6566,25 @@
         <v>30</v>
       </c>
       <c r="H49" s="48" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I49" s="49" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="J49" s="50" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="K49" s="85" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="L49" s="98" t="s">
-        <v>592</v>
-      </c>
-      <c r="M49" s="102" t="s">
-        <v>613</v>
+        <v>587</v>
+      </c>
+      <c r="M49" s="101" t="s">
+        <v>608</v>
       </c>
       <c r="N49" s="85" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="O49" s="47" t="s">
         <v>351</v>
@@ -6610,15 +6666,17 @@
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.35">
       <c r="I52" s="33"/>
-      <c r="L52" s="108" t="s">
-        <v>634</v>
-      </c>
-      <c r="M52" s="106" t="s">
-        <v>634</v>
-      </c>
-      <c r="N52" s="107"/>
+      <c r="L52" s="103" t="s">
+        <v>627</v>
+      </c>
+      <c r="M52" s="102" t="s">
+        <v>627</v>
+      </c>
+      <c r="N52" s="109" t="s">
+        <v>627</v>
+      </c>
       <c r="O52" s="33" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to NombreCientifico_APG NA values
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDC2758-466A-4E06-B4DA-7B500F348B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609F877E-539F-46B8-99E4-9A46991CB7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="692">
   <si>
     <t>Variable</t>
   </si>
@@ -1670,9 +1670,6 @@
     <t>Number of growth rings in the last 2.5cm of chip length.</t>
   </si>
   <si>
-    <t>hickness of the bark at the height of the normal diameter (1.30m) on the side of the tree pointing towards the center of the site in millimeters.</t>
-  </si>
-  <si>
     <t>Number of alive branches</t>
   </si>
   <si>
@@ -2046,6 +2043,117 @@
   </si>
   <si>
     <t>n= 92 (NA)</t>
+  </si>
+  <si>
+    <t>EnglishName</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>ClusterID</t>
+  </si>
+  <si>
+    <t>SiteNumber</t>
+  </si>
+  <si>
+    <t>RegisterNumber</t>
+  </si>
+  <si>
+    <t>clu_sit_reg</t>
+  </si>
+  <si>
+    <t>CveVeg</t>
+  </si>
+  <si>
+    <t>TypeVeg</t>
+  </si>
+  <si>
+    <t>Family_APG</t>
+  </si>
+  <si>
+    <t>ScientificName_APG</t>
+  </si>
+  <si>
+    <t>CommonName</t>
+  </si>
+  <si>
+    <t>BiologicalForm</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>HeightTotal</t>
+  </si>
+  <si>
+    <t>GrowthStage</t>
+  </si>
+  <si>
+    <t>HeightNoBranches</t>
+  </si>
+  <si>
+    <t>HeightCommercial</t>
+  </si>
+  <si>
+    <t>DiameterNormal</t>
+  </si>
+  <si>
+    <t>DiameterBase</t>
+  </si>
+  <si>
+    <t>DiameterCrown</t>
+  </si>
+  <si>
+    <t>AreaBase</t>
+  </si>
+  <si>
+    <t>AreaCrown</t>
+  </si>
+  <si>
+    <t>PositionCrown</t>
+  </si>
+  <si>
+    <t>ExposicionCrown</t>
+  </si>
+  <si>
+    <t>DensityCrown</t>
+  </si>
+  <si>
+    <t>TranparencyCrown</t>
+  </si>
+  <si>
+    <t>LiveCrownArea</t>
+  </si>
+  <si>
+    <t>Damage1</t>
+  </si>
+  <si>
+    <t>Damage2</t>
+  </si>
+  <si>
+    <t>Severity1</t>
+  </si>
+  <si>
+    <t>Severity2</t>
+  </si>
+  <si>
+    <t>NumberBranches</t>
+  </si>
+  <si>
+    <t>LengthRing10</t>
+  </si>
+  <si>
+    <t>NumberRing25</t>
+  </si>
+  <si>
+    <t>thickness of the bark at the height of the normal diameter (1.30m) on the side of the tree pointing towards the center of the site in millimeters.</t>
+  </si>
+  <si>
+    <t>BarkThickness</t>
+  </si>
+  <si>
+    <t>StumpType</t>
   </si>
 </sst>
 </file>
@@ -2397,7 +2505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2539,11 +2647,20 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4719,10 +4836,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
-  <dimension ref="C1:P52"/>
+  <dimension ref="C1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4731,64 +4848,66 @@
     <col min="5" max="5" width="26.36328125" customWidth="1"/>
     <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="11.08984375" customWidth="1"/>
-    <col min="15" max="15" width="65.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1796875" style="111" customWidth="1"/>
+    <col min="9" max="9" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="11.08984375" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="11.08984375" customWidth="1"/>
+    <col min="16" max="16" width="65.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="I1" s="7"/>
-      <c r="J1" t="s">
+    <row r="1" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="J1" s="7"/>
+      <c r="K1" t="s">
         <v>455</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" t="s">
+      <c r="O1" s="61"/>
+      <c r="P1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="I2" s="8"/>
-      <c r="J2" t="s">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="J2" s="8"/>
+      <c r="K2" t="s">
         <v>510</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="I3" s="6"/>
-      <c r="J3" t="s">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="J3" s="6"/>
+      <c r="K3" t="s">
         <v>477</v>
       </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="87" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="O3" s="43"/>
+      <c r="P3" s="87" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
       <c r="G5" s="34"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="28" t="s">
+      <c r="H5" s="109"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="28" t="s">
         <v>440</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="28" t="s">
+      <c r="L5" s="28"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="28" t="s">
         <v>439</v>
       </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="28"/>
+      <c r="P5" s="38" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C6" s="29" t="s">
         <v>403</v>
       </c>
@@ -4804,32 +4923,35 @@
       <c r="G6" s="88" t="s">
         <v>402</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="108" t="s">
+        <v>655</v>
+      </c>
+      <c r="I6" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="J6" s="36" t="s">
         <v>399</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="K6" s="37" t="s">
         <v>400</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="L6" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="M6" s="36" t="s">
         <v>399</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="N6" s="37" t="s">
         <v>400</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="O6" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="O6" s="39" t="s">
+      <c r="P6" s="39" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C7" s="29">
         <v>1</v>
       </c>
@@ -4845,32 +4967,35 @@
       <c r="G7" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="110" t="s">
+        <v>656</v>
+      </c>
+      <c r="I7" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="J7" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>435</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>436</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="M7" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>435</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>436</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="P7" s="33" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C8" s="29">
         <v>2</v>
       </c>
@@ -4886,32 +5011,35 @@
       <c r="G8" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="35" t="s">
         <v>437</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="K8" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="L8" s="40" t="s">
-        <v>419</v>
-      </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="40" t="s">
         <v>419</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="O8" s="40" t="s">
+      <c r="O8" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="P8" s="40" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C9" s="29">
         <v>3</v>
       </c>
@@ -4927,32 +5055,35 @@
       <c r="G9" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="118" t="s">
+        <v>657</v>
+      </c>
+      <c r="I9" t="s">
         <v>406</v>
       </c>
-      <c r="I9" s="41" t="s">
-        <v>445</v>
-      </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="41" t="s">
         <v>445</v>
       </c>
       <c r="K9" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="M9" s="56" t="s">
+      <c r="M9" s="41" t="s">
         <v>445</v>
       </c>
       <c r="N9" s="56" t="s">
         <v>445</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="56" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="P9" s="41" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C10" s="29">
         <v>4</v>
       </c>
@@ -4968,32 +5099,35 @@
       <c r="G10" s="89" t="s">
         <v>233</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="118" t="s">
+        <v>658</v>
+      </c>
+      <c r="I10" t="s">
         <v>405</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="J10" s="40" t="s">
         <v>420</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>444</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="L10" s="40" t="s">
-        <v>420</v>
-      </c>
-      <c r="M10" s="7" t="s">
+      <c r="L10" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="M10" s="40" t="s">
         <v>420</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="O10" s="7" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="P10" s="40" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C11" s="29">
         <v>5</v>
       </c>
@@ -5009,35 +5143,38 @@
       <c r="G11" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="112" t="s">
+        <v>659</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="I11" s="35" t="s">
+      <c r="J11" s="35" t="s">
         <v>408</v>
       </c>
-      <c r="J11" s="65" t="s">
+      <c r="K11" s="65" t="s">
         <v>454</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="L11" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="M11" s="40" t="s">
         <v>446</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="N11" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="N11" s="63" t="s">
+      <c r="O11" s="63" t="s">
         <v>448</v>
       </c>
-      <c r="O11" s="35" t="s">
+      <c r="P11" s="35" t="s">
         <v>449</v>
       </c>
-      <c r="P11" s="7" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="Q11" s="7" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C12" s="29">
         <v>6</v>
       </c>
@@ -5053,35 +5190,38 @@
       <c r="G12" s="91" t="s">
         <v>425</v>
       </c>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="113" t="s">
+        <v>660</v>
+      </c>
+      <c r="I12" s="48" t="s">
         <v>424</v>
       </c>
-      <c r="I12" s="57" t="s">
+      <c r="J12" s="57" t="s">
         <v>417</v>
       </c>
-      <c r="J12" s="80" t="s">
+      <c r="K12" s="80" t="s">
         <v>417</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="L12" s="58" t="s">
         <v>408</v>
       </c>
-      <c r="L12" s="57" t="s">
+      <c r="M12" s="57" t="s">
         <v>417</v>
       </c>
-      <c r="M12" s="64" t="s">
+      <c r="N12" s="64" t="s">
         <v>417</v>
       </c>
-      <c r="N12" s="58" t="s">
+      <c r="O12" s="58" t="s">
         <v>408</v>
       </c>
-      <c r="O12" s="47" t="s">
+      <c r="P12" s="47" t="s">
         <v>417</v>
       </c>
-      <c r="P12" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="Q12" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C13" s="29">
         <v>7</v>
       </c>
@@ -5097,33 +5237,34 @@
       <c r="G13" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="H13" s="114"/>
+      <c r="I13" s="43" t="s">
         <v>408</v>
       </c>
-      <c r="I13" s="44" t="s">
+      <c r="J13" s="44" t="s">
         <v>450</v>
       </c>
-      <c r="J13" s="43" t="s">
+      <c r="K13" s="43" t="s">
         <v>451</v>
       </c>
-      <c r="K13" s="43" t="s">
+      <c r="L13" s="43" t="s">
         <v>452</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="M13" s="44" t="s">
         <v>450</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="N13" s="43" t="s">
         <v>451</v>
       </c>
-      <c r="N13" s="43" t="s">
+      <c r="O13" s="43" t="s">
         <v>452</v>
       </c>
-      <c r="O13" s="44" t="s">
+      <c r="P13" s="44" t="s">
         <v>453</v>
       </c>
-      <c r="P13" s="43"/>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="Q13" s="43"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C14" s="29">
         <v>8</v>
       </c>
@@ -5139,30 +5280,33 @@
       <c r="G14" s="93" t="s">
         <v>427</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="54" t="s">
+      <c r="H14" s="115" t="s">
+        <v>661</v>
+      </c>
+      <c r="I14" s="52"/>
+      <c r="J14" s="54" t="s">
         <v>456</v>
       </c>
-      <c r="J14" s="55" t="s">
+      <c r="K14" s="55" t="s">
         <v>457</v>
       </c>
-      <c r="K14" s="70" t="s">
+      <c r="L14" s="70" t="s">
         <v>458</v>
       </c>
-      <c r="L14" s="69" t="s">
-        <v>585</v>
-      </c>
-      <c r="M14" s="70" t="s">
-        <v>619</v>
+      <c r="M14" s="69" t="s">
+        <v>584</v>
       </c>
       <c r="N14" s="70" t="s">
+        <v>618</v>
+      </c>
+      <c r="O14" s="70" t="s">
         <v>458</v>
       </c>
-      <c r="O14" s="53" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="P14" s="53" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C15" s="29">
         <v>9</v>
       </c>
@@ -5178,30 +5322,33 @@
       <c r="G15" s="91" t="s">
         <v>428</v>
       </c>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49" t="s">
+      <c r="H15" s="113" t="s">
+        <v>662</v>
+      </c>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49" t="s">
         <v>469</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="K15" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="K15" s="64" t="s">
+      <c r="L15" s="64" t="s">
         <v>458</v>
       </c>
-      <c r="L15" s="57" t="s">
-        <v>585</v>
-      </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="57" t="s">
+        <v>584</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="N15" s="64" t="s">
+      <c r="O15" s="64" t="s">
         <v>458</v>
       </c>
-      <c r="O15" s="53" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="P15" s="53" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C16" s="29">
         <v>10</v>
       </c>
@@ -5217,35 +5364,38 @@
       <c r="G16" s="89" t="s">
         <v>237</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="118" t="s">
+        <v>237</v>
+      </c>
+      <c r="I16" t="s">
         <v>471</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="J16" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J16" s="55" t="s">
+      <c r="K16" s="55" t="s">
         <v>459</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="L16" s="59" t="s">
+      <c r="M16" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M16" s="70" t="s">
-        <v>610</v>
-      </c>
-      <c r="N16" s="7" t="s">
+      <c r="N16" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="O16" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="O16" s="60" t="s">
+      <c r="P16" s="60" t="s">
         <v>462</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="Q16" s="14" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C17" s="29">
         <v>11</v>
       </c>
@@ -5261,32 +5411,35 @@
       <c r="G17" s="89" t="s">
         <v>238</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="118" t="s">
+        <v>691</v>
+      </c>
+      <c r="I17" t="s">
         <v>472</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="J17" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="K17" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="L17" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="L17" s="59" t="s">
+      <c r="M17" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M17" s="7" t="s">
-        <v>609</v>
-      </c>
       <c r="N17" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="O17" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="O17" s="33" t="s">
+      <c r="P17" s="33" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C18" s="29">
         <v>12</v>
       </c>
@@ -5302,32 +5455,35 @@
       <c r="G18" s="89" t="s">
         <v>239</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="110" t="s">
+        <v>663</v>
+      </c>
+      <c r="I18" t="s">
         <v>411</v>
       </c>
-      <c r="I18" s="62" t="s">
+      <c r="J18" s="62" t="s">
         <v>466</v>
       </c>
-      <c r="J18" s="63" t="s">
+      <c r="K18" s="63" t="s">
         <v>467</v>
       </c>
-      <c r="K18" s="63" t="s">
+      <c r="L18" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="L18" s="62" t="s">
+      <c r="M18" s="62" t="s">
         <v>466</v>
       </c>
-      <c r="M18" s="63" t="s">
+      <c r="N18" s="63" t="s">
         <v>467</v>
       </c>
-      <c r="N18" s="63" t="s">
+      <c r="O18" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="O18" s="60" t="s">
+      <c r="P18" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="29">
         <v>13</v>
       </c>
@@ -5343,26 +5499,29 @@
       <c r="G19" s="89" t="s">
         <v>240</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="118" t="s">
+        <v>664</v>
+      </c>
+      <c r="I19" t="s">
         <v>412</v>
       </c>
-      <c r="I19" s="62" t="s">
+      <c r="J19" s="62" t="s">
         <v>473</v>
       </c>
-      <c r="J19" s="63" t="s">
+      <c r="K19" s="63" t="s">
         <v>474</v>
       </c>
-      <c r="K19" s="63" t="s">
+      <c r="L19" s="63" t="s">
         <v>475</v>
       </c>
-      <c r="L19" s="62"/>
-      <c r="M19" s="63"/>
+      <c r="M19" s="62"/>
       <c r="N19" s="63"/>
-      <c r="O19" s="60" t="s">
+      <c r="O19" s="63"/>
+      <c r="P19" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="29">
         <v>14</v>
       </c>
@@ -5378,32 +5537,35 @@
       <c r="G20" s="89" t="s">
         <v>363</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="118" t="s">
+        <v>665</v>
+      </c>
+      <c r="I20" t="s">
         <v>430</v>
       </c>
-      <c r="I20" s="66" t="s">
+      <c r="J20" s="66" t="s">
         <v>478</v>
       </c>
-      <c r="J20" s="67" t="s">
+      <c r="K20" s="67" t="s">
         <v>479</v>
       </c>
-      <c r="K20" s="67" t="s">
+      <c r="L20" s="67" t="s">
         <v>480</v>
       </c>
-      <c r="L20" s="66" t="s">
+      <c r="M20" s="66" t="s">
         <v>478</v>
       </c>
-      <c r="M20" s="67" t="s">
+      <c r="N20" s="67" t="s">
         <v>479</v>
       </c>
-      <c r="N20" s="67" t="s">
+      <c r="O20" s="67" t="s">
         <v>480</v>
       </c>
-      <c r="O20" s="66" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="P20" s="66" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="29">
         <v>15</v>
       </c>
@@ -5419,32 +5581,35 @@
       <c r="G21" s="91" t="s">
         <v>397</v>
       </c>
-      <c r="H21" s="48" t="s">
+      <c r="H21" s="113" t="s">
+        <v>666</v>
+      </c>
+      <c r="I21" s="48" t="s">
         <v>415</v>
       </c>
-      <c r="I21" s="57" t="s">
+      <c r="J21" s="57" t="s">
         <v>481</v>
       </c>
-      <c r="J21" s="64" t="s">
+      <c r="K21" s="64" t="s">
         <v>481</v>
       </c>
-      <c r="K21" s="50" t="s">
+      <c r="L21" s="50" t="s">
         <v>482</v>
       </c>
-      <c r="L21" s="57" t="s">
+      <c r="M21" s="57" t="s">
         <v>481</v>
       </c>
-      <c r="M21" s="64" t="s">
+      <c r="N21" s="64" t="s">
         <v>481</v>
       </c>
-      <c r="N21" s="64" t="s">
-        <v>638</v>
-      </c>
-      <c r="O21" s="47" t="s">
+      <c r="O21" s="64" t="s">
+        <v>637</v>
+      </c>
+      <c r="P21" s="47" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="29">
         <v>16</v>
       </c>
@@ -5460,32 +5625,35 @@
       <c r="G22" s="89" t="s">
         <v>362</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="118" t="s">
+        <v>667</v>
+      </c>
+      <c r="I22" t="s">
         <v>483</v>
       </c>
-      <c r="I22" s="59" t="s">
+      <c r="J22" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="K22" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="M22" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="N22" s="7" t="s">
         <v>598</v>
       </c>
-      <c r="K22" s="8" t="s">
-        <v>484</v>
-      </c>
-      <c r="L22" s="59" t="s">
-        <v>460</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>599</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>628</v>
-      </c>
-      <c r="O22" s="60" t="s">
+      <c r="O22" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="P22" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="29">
         <v>17</v>
       </c>
@@ -5501,32 +5669,35 @@
       <c r="G23" s="89" t="s">
         <v>253</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="118" t="s">
+        <v>253</v>
+      </c>
+      <c r="I23" t="s">
         <v>486</v>
       </c>
-      <c r="I23" s="59" t="s">
+      <c r="J23" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>597</v>
-      </c>
       <c r="K23" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="M23" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="O23" s="7" t="s">
         <v>629</v>
       </c>
-      <c r="L23" s="59" t="s">
-        <v>460</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>594</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>630</v>
-      </c>
-      <c r="O23" s="47" t="s">
+      <c r="P23" s="47" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="29">
         <v>18</v>
       </c>
@@ -5542,32 +5713,35 @@
       <c r="G24" s="93" t="s">
         <v>395</v>
       </c>
-      <c r="H24" s="52" t="s">
+      <c r="H24" s="115" t="s">
+        <v>668</v>
+      </c>
+      <c r="I24" s="52" t="s">
         <v>489</v>
       </c>
-      <c r="I24" s="69" t="s">
+      <c r="J24" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="J24" s="70" t="s">
+      <c r="K24" s="70" t="s">
         <v>488</v>
       </c>
-      <c r="K24" s="55" t="s">
+      <c r="L24" s="55" t="s">
+        <v>630</v>
+      </c>
+      <c r="M24" s="69" t="s">
+        <v>487</v>
+      </c>
+      <c r="N24" s="70" t="s">
+        <v>488</v>
+      </c>
+      <c r="O24" s="70" t="s">
         <v>631</v>
       </c>
-      <c r="L24" s="69" t="s">
-        <v>487</v>
-      </c>
-      <c r="M24" s="70" t="s">
-        <v>488</v>
-      </c>
-      <c r="N24" s="70" t="s">
-        <v>632</v>
-      </c>
-      <c r="O24" s="60" t="s">
+      <c r="P24" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C25" s="29">
         <v>19</v>
       </c>
@@ -5583,32 +5757,35 @@
       <c r="G25" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="118" t="s">
+        <v>670</v>
+      </c>
+      <c r="I25" t="s">
         <v>490</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="J25" s="35" t="s">
         <v>494</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>592</v>
-      </c>
       <c r="K25" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="L25" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="L25" s="40" t="s">
-        <v>556</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>588</v>
+      <c r="M25" s="40" t="s">
+        <v>555</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>633</v>
-      </c>
-      <c r="O25" s="60" t="s">
+        <v>587</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="P25" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C26" s="29">
         <v>20</v>
       </c>
@@ -5624,32 +5801,35 @@
       <c r="G26" s="91" t="s">
         <v>268</v>
       </c>
-      <c r="H26" s="48" t="s">
+      <c r="H26" s="113" t="s">
+        <v>671</v>
+      </c>
+      <c r="I26" s="48" t="s">
         <v>491</v>
       </c>
-      <c r="I26" s="49" t="s">
+      <c r="J26" s="49" t="s">
         <v>495</v>
       </c>
-      <c r="J26" s="71" t="s">
-        <v>593</v>
-      </c>
       <c r="K26" s="71" t="s">
+        <v>592</v>
+      </c>
+      <c r="L26" s="71" t="s">
         <v>492</v>
       </c>
-      <c r="L26" s="57" t="s">
-        <v>557</v>
-      </c>
-      <c r="M26" s="99" t="s">
-        <v>589</v>
+      <c r="M26" s="57" t="s">
+        <v>556</v>
       </c>
       <c r="N26" s="99" t="s">
-        <v>634</v>
-      </c>
-      <c r="O26" s="72" t="s">
+        <v>588</v>
+      </c>
+      <c r="O26" s="99" t="s">
+        <v>633</v>
+      </c>
+      <c r="P26" s="72" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C27" s="29">
         <v>21</v>
       </c>
@@ -5665,32 +5845,35 @@
       <c r="G27" s="93" t="s">
         <v>396</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="115" t="s">
+        <v>672</v>
+      </c>
+      <c r="I27" s="52" t="s">
         <v>496</v>
       </c>
-      <c r="I27" s="69" t="s">
+      <c r="J27" s="69" t="s">
         <v>499</v>
       </c>
-      <c r="J27" s="70" t="s">
+      <c r="K27" s="70" t="s">
         <v>500</v>
       </c>
-      <c r="K27" s="55" t="s">
+      <c r="L27" s="55" t="s">
         <v>501</v>
       </c>
-      <c r="L27" s="69" t="s">
+      <c r="M27" s="69" t="s">
         <v>499</v>
       </c>
-      <c r="M27" s="70" t="s">
+      <c r="N27" s="70" t="s">
         <v>500</v>
       </c>
-      <c r="N27" s="70" t="s">
-        <v>634</v>
-      </c>
-      <c r="O27" s="60" t="s">
+      <c r="O27" s="70" t="s">
+        <v>633</v>
+      </c>
+      <c r="P27" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C28" s="29">
         <v>22</v>
       </c>
@@ -5706,32 +5889,35 @@
       <c r="G28" s="89" t="s">
         <v>252</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="118" t="s">
+        <v>673</v>
+      </c>
+      <c r="I28" t="s">
         <v>498</v>
       </c>
-      <c r="I28" s="35" t="s">
-        <v>565</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>595</v>
-      </c>
-      <c r="K28" s="17" t="s">
+      <c r="J28" s="35" t="s">
+        <v>564</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="L28" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="L28" s="40" t="s">
-        <v>560</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>590</v>
-      </c>
-      <c r="N28" s="16" t="s">
-        <v>635</v>
-      </c>
-      <c r="O28" s="60" t="s">
+      <c r="M28" s="40" t="s">
+        <v>559</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="O28" s="16" t="s">
+        <v>634</v>
+      </c>
+      <c r="P28" s="60" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C29" s="29">
         <v>23</v>
       </c>
@@ -5747,32 +5933,35 @@
       <c r="G29" s="91" t="s">
         <v>245</v>
       </c>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="113" t="s">
+        <v>674</v>
+      </c>
+      <c r="I29" s="48" t="s">
         <v>497</v>
       </c>
-      <c r="I29" s="49" t="s">
-        <v>564</v>
-      </c>
-      <c r="J29" s="50" t="s">
-        <v>596</v>
-      </c>
-      <c r="K29" s="73" t="s">
+      <c r="J29" s="49" t="s">
+        <v>563</v>
+      </c>
+      <c r="K29" s="50" t="s">
+        <v>595</v>
+      </c>
+      <c r="L29" s="73" t="s">
         <v>502</v>
       </c>
-      <c r="L29" s="64" t="s">
-        <v>558</v>
-      </c>
       <c r="M29" s="64" t="s">
-        <v>591</v>
-      </c>
-      <c r="N29" s="104" t="s">
-        <v>636</v>
-      </c>
-      <c r="O29" s="72" t="s">
+        <v>557</v>
+      </c>
+      <c r="N29" s="64" t="s">
+        <v>590</v>
+      </c>
+      <c r="O29" s="104" t="s">
+        <v>635</v>
+      </c>
+      <c r="P29" s="72" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C30" s="29">
         <v>24</v>
       </c>
@@ -5788,32 +5977,35 @@
       <c r="G30" s="89" t="s">
         <v>392</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="118" t="s">
+        <v>675</v>
+      </c>
+      <c r="I30" t="s">
         <v>514</v>
       </c>
-      <c r="I30" s="35" t="s">
-        <v>562</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>622</v>
-      </c>
-      <c r="K30" s="81" t="s">
+      <c r="J30" s="35" t="s">
+        <v>561</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="L30" s="81" t="s">
         <v>512</v>
       </c>
-      <c r="L30" s="40" t="s">
-        <v>561</v>
-      </c>
-      <c r="M30" s="7" t="s">
-        <v>620</v>
-      </c>
-      <c r="N30" s="105" t="s">
-        <v>637</v>
-      </c>
-      <c r="O30" s="60" t="s">
+      <c r="M30" s="40" t="s">
+        <v>560</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="O30" s="105" t="s">
+        <v>636</v>
+      </c>
+      <c r="P30" s="60" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C31" s="29">
         <v>25</v>
       </c>
@@ -5829,32 +6021,35 @@
       <c r="G31" s="91" t="s">
         <v>393</v>
       </c>
-      <c r="H31" s="48" t="s">
+      <c r="H31" s="113" t="s">
+        <v>676</v>
+      </c>
+      <c r="I31" s="48" t="s">
         <v>515</v>
       </c>
-      <c r="I31" s="49" t="s">
-        <v>563</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>623</v>
-      </c>
-      <c r="K31" s="82" t="s">
+      <c r="J31" s="49" t="s">
+        <v>562</v>
+      </c>
+      <c r="K31" s="50" t="s">
+        <v>622</v>
+      </c>
+      <c r="L31" s="82" t="s">
         <v>502</v>
       </c>
-      <c r="L31" s="57" t="s">
-        <v>559</v>
-      </c>
-      <c r="M31" s="64" t="s">
-        <v>621</v>
-      </c>
-      <c r="N31" s="106" t="s">
-        <v>636</v>
-      </c>
-      <c r="O31" s="72" t="s">
+      <c r="M31" s="57" t="s">
+        <v>558</v>
+      </c>
+      <c r="N31" s="64" t="s">
+        <v>620</v>
+      </c>
+      <c r="O31" s="106" t="s">
+        <v>635</v>
+      </c>
+      <c r="P31" s="72" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C32" s="29">
         <v>26</v>
       </c>
@@ -5870,32 +6065,35 @@
       <c r="G32" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="76" t="s">
-        <v>542</v>
-      </c>
-      <c r="I32" s="86" t="s">
+      <c r="H32" s="116" t="s">
+        <v>677</v>
+      </c>
+      <c r="I32" s="76" t="s">
+        <v>541</v>
+      </c>
+      <c r="J32" s="86" t="s">
         <v>460</v>
       </c>
-      <c r="J32" s="55" t="s">
-        <v>624</v>
-      </c>
       <c r="K32" s="55" t="s">
-        <v>547</v>
-      </c>
-      <c r="L32" s="86" t="s">
+        <v>623</v>
+      </c>
+      <c r="L32" s="55" t="s">
+        <v>546</v>
+      </c>
+      <c r="M32" s="86" t="s">
         <v>460</v>
       </c>
-      <c r="M32" s="70" t="s">
-        <v>609</v>
-      </c>
-      <c r="N32" s="107" t="s">
-        <v>639</v>
-      </c>
-      <c r="O32" s="53" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="N32" s="70" t="s">
+        <v>608</v>
+      </c>
+      <c r="O32" s="70" t="s">
+        <v>638</v>
+      </c>
+      <c r="P32" s="53" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C33" s="29">
         <v>27</v>
       </c>
@@ -5911,32 +6109,35 @@
       <c r="G33" s="88" t="s">
         <v>364</v>
       </c>
-      <c r="H33" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="I33" s="59" t="s">
+      <c r="H33" s="109" t="s">
+        <v>678</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="J33" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J33" s="8" t="s">
-        <v>625</v>
-      </c>
       <c r="K33" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="M33" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="P33" s="33" t="s">
         <v>548</v>
       </c>
-      <c r="L33" s="59" t="s">
-        <v>460</v>
-      </c>
-      <c r="M33" s="7" t="s">
-        <v>611</v>
-      </c>
-      <c r="N33" s="108" t="s">
-        <v>640</v>
-      </c>
-      <c r="O33" s="33" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C34" s="29">
         <v>28</v>
       </c>
@@ -5952,32 +6153,35 @@
       <c r="G34" s="88" t="s">
         <v>249</v>
       </c>
-      <c r="H34" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="I34" s="59" t="s">
+      <c r="H34" s="109" t="s">
+        <v>679</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="J34" s="59" t="s">
         <v>460</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>552</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="L34" s="59" t="s">
+      <c r="L34" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="M34" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M34" s="7" t="s">
-        <v>644</v>
-      </c>
       <c r="N34" s="7" t="s">
-        <v>641</v>
-      </c>
-      <c r="O34" s="33" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+        <v>643</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="P34" s="33" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C35" s="29">
         <v>29</v>
       </c>
@@ -5993,32 +6197,35 @@
       <c r="G35" s="88" t="s">
         <v>250</v>
       </c>
-      <c r="H35" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="I35" s="59" t="s">
+      <c r="H35" s="109" t="s">
+        <v>680</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="J35" s="59" t="s">
         <v>460</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>552</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="L35" s="59" t="s">
+      <c r="L35" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="M35" s="59" t="s">
         <v>460</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>642</v>
       </c>
       <c r="N35" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="O35" s="33" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="O35" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="P35" s="33" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C36" s="29">
         <v>30</v>
       </c>
@@ -6034,30 +6241,33 @@
       <c r="G36" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="H36" s="79" t="s">
-        <v>546</v>
-      </c>
-      <c r="I36" s="59" t="s">
+      <c r="H36" s="117" t="s">
+        <v>681</v>
+      </c>
+      <c r="I36" s="79" t="s">
+        <v>545</v>
+      </c>
+      <c r="J36" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J36" s="8" t="s">
-        <v>552</v>
-      </c>
       <c r="K36" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="L36" s="59" t="s">
+        <v>551</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="M36" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M36" s="7" t="s">
-        <v>643</v>
-      </c>
       <c r="N36" s="7" t="s">
-        <v>645</v>
-      </c>
-      <c r="O36" s="47"/>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+        <v>642</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="P36" s="47"/>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C37" s="29">
         <v>31</v>
       </c>
@@ -6073,32 +6283,35 @@
       <c r="G37" s="89" t="s">
         <v>394</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="118" t="s">
+        <v>669</v>
+      </c>
+      <c r="I37" t="s">
         <v>516</v>
       </c>
-      <c r="I37" s="54" t="s">
-        <v>517</v>
-      </c>
-      <c r="J37" s="55" t="s">
+      <c r="J37" s="54" t="s">
         <v>517</v>
       </c>
       <c r="K37" s="55" t="s">
         <v>517</v>
       </c>
-      <c r="L37" s="69" t="s">
-        <v>570</v>
-      </c>
-      <c r="M37" s="70" t="s">
-        <v>570</v>
+      <c r="L37" s="55" t="s">
+        <v>517</v>
+      </c>
+      <c r="M37" s="69" t="s">
+        <v>569</v>
       </c>
       <c r="N37" s="70" t="s">
-        <v>570</v>
-      </c>
-      <c r="O37" s="33" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="O37" s="70" t="s">
+        <v>569</v>
+      </c>
+      <c r="P37" s="33" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="38" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C38" s="29">
         <v>32</v>
       </c>
@@ -6114,32 +6327,35 @@
       <c r="G38" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="118" t="s">
+        <v>656</v>
+      </c>
+      <c r="I38" t="s">
         <v>429</v>
       </c>
-      <c r="I38" s="35" t="s">
-        <v>573</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>601</v>
+      <c r="J38" s="35" t="s">
+        <v>572</v>
       </c>
       <c r="K38" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="L38" s="8" t="s">
         <v>518</v>
       </c>
-      <c r="L38" s="40" t="s">
-        <v>571</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>600</v>
+      <c r="M38" s="40" t="s">
+        <v>570</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="O38" s="60" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+        <v>599</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="P38" s="60" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="39" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C39" s="29">
         <v>33</v>
       </c>
@@ -6155,32 +6371,35 @@
       <c r="G39" s="89" t="s">
         <v>367</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="118" t="s">
         <v>431</v>
       </c>
-      <c r="I39" s="35" t="s">
+      <c r="I39" t="s">
+        <v>431</v>
+      </c>
+      <c r="J39" s="35" t="s">
         <v>444</v>
       </c>
-      <c r="J39" s="8" t="s">
+      <c r="K39" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="L39" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="L39" s="40" t="s">
-        <v>444</v>
-      </c>
-      <c r="M39" s="7" t="s">
+      <c r="M39" s="40" t="s">
         <v>444</v>
       </c>
       <c r="N39" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="O39" s="33" t="s">
+      <c r="O39" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="P39" s="33" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C40" s="29">
         <v>34</v>
       </c>
@@ -6196,32 +6415,35 @@
       <c r="G40" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="118" t="s">
+        <v>682</v>
+      </c>
+      <c r="I40" t="s">
         <v>506</v>
       </c>
-      <c r="I40" s="59" t="s">
+      <c r="J40" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J40" s="8" t="s">
+      <c r="K40" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="L40" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="L40" s="59" t="s">
+      <c r="M40" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M40" s="7" t="s">
-        <v>615</v>
-      </c>
       <c r="N40" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="O40" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="O40" s="60" t="s">
+      <c r="P40" s="60" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C41" s="29">
         <v>35</v>
       </c>
@@ -6237,32 +6459,35 @@
       <c r="G41" s="89" t="s">
         <v>360</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="118" t="s">
+        <v>684</v>
+      </c>
+      <c r="I41" t="s">
         <v>507</v>
       </c>
-      <c r="I41" s="59" t="s">
+      <c r="J41" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="K41" s="8" t="s">
         <v>524</v>
       </c>
-      <c r="K41" s="8" t="s">
-        <v>647</v>
-      </c>
-      <c r="L41" s="59" t="s">
+      <c r="L41" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="M41" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M41" s="7" t="s">
-        <v>617</v>
-      </c>
       <c r="N41" s="7" t="s">
-        <v>651</v>
-      </c>
-      <c r="O41" s="60" t="s">
+        <v>616</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="P41" s="60" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C42" s="29">
         <v>36</v>
       </c>
@@ -6278,32 +6503,35 @@
       <c r="G42" s="89" t="s">
         <v>272</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="118" t="s">
+        <v>683</v>
+      </c>
+      <c r="I42" t="s">
         <v>508</v>
       </c>
-      <c r="I42" s="59" t="s">
+      <c r="J42" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="J42" s="8" t="s">
+      <c r="K42" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="L42" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="L42" s="59" t="s">
+      <c r="M42" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="M42" s="7" t="s">
-        <v>616</v>
-      </c>
       <c r="N42" s="7" t="s">
-        <v>649</v>
-      </c>
-      <c r="O42" s="60" t="s">
+        <v>615</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="P42" s="60" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C43" s="29">
         <v>37</v>
       </c>
@@ -6319,32 +6547,35 @@
       <c r="G43" s="91" t="s">
         <v>361</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="118" t="s">
+        <v>685</v>
+      </c>
+      <c r="I43" t="s">
         <v>509</v>
       </c>
-      <c r="I43" s="83" t="s">
+      <c r="J43" s="83" t="s">
         <v>460</v>
       </c>
-      <c r="J43" s="50" t="s">
+      <c r="K43" s="50" t="s">
         <v>525</v>
       </c>
-      <c r="K43" s="50" t="s">
-        <v>648</v>
-      </c>
-      <c r="L43" s="83" t="s">
+      <c r="L43" s="50" t="s">
+        <v>647</v>
+      </c>
+      <c r="M43" s="83" t="s">
         <v>460</v>
       </c>
-      <c r="M43" s="64" t="s">
-        <v>618</v>
-      </c>
       <c r="N43" s="64" t="s">
-        <v>650</v>
-      </c>
-      <c r="O43" s="72" t="s">
+        <v>617</v>
+      </c>
+      <c r="O43" s="64" t="s">
+        <v>649</v>
+      </c>
+      <c r="P43" s="72" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C44" s="29">
         <v>38</v>
       </c>
@@ -6360,32 +6591,35 @@
       <c r="G44" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="H44" s="76" t="s">
+      <c r="H44" s="116" t="s">
+        <v>686</v>
+      </c>
+      <c r="I44" s="76" t="s">
+        <v>530</v>
+      </c>
+      <c r="J44" s="54" t="s">
+        <v>571</v>
+      </c>
+      <c r="K44" s="55" t="s">
+        <v>602</v>
+      </c>
+      <c r="L44" s="55" t="s">
         <v>531</v>
       </c>
-      <c r="I44" s="54" t="s">
-        <v>572</v>
-      </c>
-      <c r="J44" s="55" t="s">
-        <v>603</v>
-      </c>
-      <c r="K44" s="55" t="s">
-        <v>532</v>
-      </c>
-      <c r="L44" s="69" t="s">
-        <v>574</v>
-      </c>
-      <c r="M44" s="70" t="s">
-        <v>612</v>
+      <c r="M44" s="69" t="s">
+        <v>573</v>
       </c>
       <c r="N44" s="70" t="s">
-        <v>652</v>
-      </c>
-      <c r="O44" s="60" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.35">
+        <v>611</v>
+      </c>
+      <c r="O44" s="70" t="s">
+        <v>651</v>
+      </c>
+      <c r="P44" s="60" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C45" s="29">
         <v>39</v>
       </c>
@@ -6401,32 +6635,35 @@
       <c r="G45" s="89" t="s">
         <v>391</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="118" t="s">
+        <v>687</v>
+      </c>
+      <c r="I45" t="s">
         <v>528</v>
       </c>
-      <c r="I45" s="35" t="s">
-        <v>576</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>604</v>
+      <c r="J45" s="35" t="s">
+        <v>575</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="L45" s="40" t="s">
-        <v>575</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>613</v>
+        <v>603</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="M45" s="40" t="s">
+        <v>574</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="O45" s="60" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.35">
+        <v>612</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="P45" s="60" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C46" s="29">
         <v>40</v>
       </c>
@@ -6442,32 +6679,35 @@
       <c r="G46" s="89" t="s">
         <v>390</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="118" t="s">
+        <v>688</v>
+      </c>
+      <c r="I46" t="s">
         <v>529</v>
       </c>
-      <c r="I46" s="35" t="s">
-        <v>578</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>605</v>
+      <c r="J46" s="35" t="s">
+        <v>577</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="L46" s="40" t="s">
-        <v>577</v>
-      </c>
-      <c r="M46" s="7" t="s">
-        <v>614</v>
+        <v>604</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="M46" s="40" t="s">
+        <v>576</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="O46" s="60" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.35">
+        <v>613</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="P46" s="60" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="47" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C47" s="29">
         <v>41</v>
       </c>
@@ -6483,32 +6723,35 @@
       <c r="G47" s="91" t="s">
         <v>256</v>
       </c>
-      <c r="H47" s="48" t="s">
-        <v>530</v>
-      </c>
-      <c r="I47" s="49" t="s">
-        <v>579</v>
-      </c>
-      <c r="J47" s="50" t="s">
-        <v>606</v>
+      <c r="H47" s="113" t="s">
+        <v>690</v>
+      </c>
+      <c r="I47" s="48" t="s">
+        <v>689</v>
+      </c>
+      <c r="J47" s="49" t="s">
+        <v>578</v>
       </c>
       <c r="K47" s="50" t="s">
-        <v>535</v>
-      </c>
-      <c r="L47" s="57" t="s">
-        <v>582</v>
-      </c>
-      <c r="M47" s="64" t="s">
-        <v>602</v>
+        <v>605</v>
+      </c>
+      <c r="L47" s="50" t="s">
+        <v>534</v>
+      </c>
+      <c r="M47" s="57" t="s">
+        <v>581</v>
       </c>
       <c r="N47" s="64" t="s">
-        <v>655</v>
-      </c>
-      <c r="O47" s="72" t="s">
+        <v>601</v>
+      </c>
+      <c r="O47" s="64" t="s">
+        <v>654</v>
+      </c>
+      <c r="P47" s="72" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C48" s="29">
         <v>42</v>
       </c>
@@ -6524,32 +6767,35 @@
       <c r="G48" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="52" t="s">
+      <c r="H48" s="115" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="52" t="s">
         <v>504</v>
       </c>
-      <c r="I48" s="54" t="s">
-        <v>536</v>
-      </c>
-      <c r="J48" s="55" t="s">
-        <v>538</v>
-      </c>
-      <c r="K48" s="84" t="s">
-        <v>540</v>
-      </c>
-      <c r="L48" s="97" t="s">
-        <v>586</v>
-      </c>
-      <c r="M48" s="100" t="s">
-        <v>607</v>
-      </c>
-      <c r="N48" s="84" t="s">
-        <v>540</v>
-      </c>
-      <c r="O48" s="53" t="s">
+      <c r="J48" s="54" t="s">
+        <v>535</v>
+      </c>
+      <c r="K48" s="55" t="s">
+        <v>537</v>
+      </c>
+      <c r="L48" s="84" t="s">
+        <v>539</v>
+      </c>
+      <c r="M48" s="97" t="s">
+        <v>585</v>
+      </c>
+      <c r="N48" s="100" t="s">
+        <v>606</v>
+      </c>
+      <c r="O48" s="84" t="s">
+        <v>539</v>
+      </c>
+      <c r="P48" s="53" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C49" s="29">
         <v>43</v>
       </c>
@@ -6565,32 +6811,35 @@
       <c r="G49" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="H49" s="48" t="s">
+      <c r="H49" s="113" t="s">
+        <v>30</v>
+      </c>
+      <c r="I49" s="48" t="s">
         <v>505</v>
       </c>
-      <c r="I49" s="49" t="s">
-        <v>537</v>
-      </c>
-      <c r="J49" s="50" t="s">
-        <v>539</v>
-      </c>
-      <c r="K49" s="85" t="s">
-        <v>541</v>
-      </c>
-      <c r="L49" s="98" t="s">
-        <v>587</v>
-      </c>
-      <c r="M49" s="101" t="s">
-        <v>608</v>
-      </c>
-      <c r="N49" s="85" t="s">
-        <v>541</v>
-      </c>
-      <c r="O49" s="47" t="s">
+      <c r="J49" s="49" t="s">
+        <v>536</v>
+      </c>
+      <c r="K49" s="50" t="s">
+        <v>538</v>
+      </c>
+      <c r="L49" s="85" t="s">
+        <v>540</v>
+      </c>
+      <c r="M49" s="98" t="s">
+        <v>586</v>
+      </c>
+      <c r="N49" s="101" t="s">
+        <v>607</v>
+      </c>
+      <c r="O49" s="85" t="s">
+        <v>540</v>
+      </c>
+      <c r="P49" s="47" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C50" s="29">
         <v>44</v>
       </c>
@@ -6606,28 +6855,29 @@
       <c r="G50" s="96" t="s">
         <v>409</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="H50" s="112"/>
+      <c r="I50" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="I50" s="59" t="s">
+      <c r="J50" s="59" t="s">
         <v>432</v>
       </c>
-      <c r="J50" s="6"/>
-      <c r="K50" s="63" t="s">
+      <c r="K50" s="6"/>
+      <c r="L50" s="63" t="s">
         <v>351</v>
       </c>
-      <c r="L50" s="59" t="s">
+      <c r="M50" s="59" t="s">
         <v>432</v>
       </c>
-      <c r="M50" s="6"/>
-      <c r="N50" s="63" t="s">
+      <c r="N50" s="6"/>
+      <c r="O50" s="63" t="s">
         <v>351</v>
       </c>
-      <c r="O50" s="33" t="s">
+      <c r="P50" s="33" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C51" s="29">
         <v>45</v>
       </c>
@@ -6643,40 +6893,41 @@
       <c r="G51" s="96" t="s">
         <v>410</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="112"/>
+      <c r="I51" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="I51" s="59" t="s">
+      <c r="J51" s="59" t="s">
         <v>412</v>
       </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="63" t="s">
+      <c r="K51" s="6"/>
+      <c r="L51" s="63" t="s">
         <v>351</v>
       </c>
-      <c r="L51" s="59" t="s">
+      <c r="M51" s="59" t="s">
         <v>412</v>
       </c>
-      <c r="M51" s="6"/>
-      <c r="N51" s="63" t="s">
+      <c r="N51" s="6"/>
+      <c r="O51" s="63" t="s">
         <v>351</v>
       </c>
-      <c r="O51" s="33" t="s">
+      <c r="P51" s="33" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="I52" s="33"/>
-      <c r="L52" s="103" t="s">
-        <v>627</v>
-      </c>
-      <c r="M52" s="102" t="s">
-        <v>627</v>
-      </c>
-      <c r="N52" s="109" t="s">
-        <v>627</v>
-      </c>
-      <c r="O52" s="33" t="s">
+    <row r="52" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="J52" s="33"/>
+      <c r="M52" s="103" t="s">
         <v>626</v>
+      </c>
+      <c r="N52" s="102" t="s">
+        <v>626</v>
+      </c>
+      <c r="O52" s="107" t="s">
+        <v>626</v>
+      </c>
+      <c r="P52" s="33" t="s">
+        <v>625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further changes to File 1 (Arb.04) tidying
</commit_message>
<xml_diff>
--- a/data/Summary_of_Variables.xlsx
+++ b/data/Summary_of_Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Desktop\Projects\MxForest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609F877E-539F-46B8-99E4-9A46991CB7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F870CFD-46CC-4D41-B43E-803741DCFB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
+    <workbookView xWindow="-9345" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{F1C2BD34-C46F-44F5-AEA0-480E2EBB14BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Secciones_Data" sheetId="2" r:id="rId1"/>
@@ -2505,7 +2505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2650,17 +2650,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3702,8 +3691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7AB688-5A0A-4572-BDE5-9C92B4B738E7}">
   <dimension ref="A4:J85"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4838,8 +4827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2580206-0FD8-4CAE-B2B1-CAAA55FA099E}">
   <dimension ref="C1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4847,8 +4836,7 @@
     <col min="4" max="4" width="26.1796875" customWidth="1"/>
     <col min="5" max="5" width="26.36328125" customWidth="1"/>
     <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.1796875" style="111" customWidth="1"/>
+    <col min="7" max="8" width="26.1796875" customWidth="1"/>
     <col min="9" max="9" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.08984375" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
@@ -4891,7 +4879,7 @@
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.35">
       <c r="G5" s="34"/>
-      <c r="H5" s="109"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="22"/>
       <c r="J5" s="32"/>
       <c r="K5" s="28" t="s">
@@ -4923,7 +4911,7 @@
       <c r="G6" s="88" t="s">
         <v>402</v>
       </c>
-      <c r="H6" s="108" t="s">
+      <c r="H6" s="28" t="s">
         <v>655</v>
       </c>
       <c r="I6" s="28" t="s">
@@ -4967,7 +4955,7 @@
       <c r="G7" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="110" t="s">
+      <c r="H7" t="s">
         <v>656</v>
       </c>
       <c r="I7" t="s">
@@ -5011,7 +4999,7 @@
       <c r="G8" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="110" t="s">
+      <c r="H8" t="s">
         <v>73</v>
       </c>
       <c r="I8" t="s">
@@ -5055,7 +5043,7 @@
       <c r="G9" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="118" t="s">
+      <c r="H9" t="s">
         <v>657</v>
       </c>
       <c r="I9" t="s">
@@ -5099,7 +5087,7 @@
       <c r="G10" s="89" t="s">
         <v>233</v>
       </c>
-      <c r="H10" s="118" t="s">
+      <c r="H10" t="s">
         <v>658</v>
       </c>
       <c r="I10" t="s">
@@ -5143,7 +5131,7 @@
       <c r="G11" s="90" t="s">
         <v>234</v>
       </c>
-      <c r="H11" s="112" t="s">
+      <c r="H11" s="8" t="s">
         <v>659</v>
       </c>
       <c r="I11" s="8" t="s">
@@ -5190,7 +5178,7 @@
       <c r="G12" s="91" t="s">
         <v>425</v>
       </c>
-      <c r="H12" s="113" t="s">
+      <c r="H12" s="48" t="s">
         <v>660</v>
       </c>
       <c r="I12" s="48" t="s">
@@ -5237,7 +5225,7 @@
       <c r="G13" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="H13" s="114"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="43" t="s">
         <v>408</v>
       </c>
@@ -5280,7 +5268,7 @@
       <c r="G14" s="93" t="s">
         <v>427</v>
       </c>
-      <c r="H14" s="115" t="s">
+      <c r="H14" s="52" t="s">
         <v>661</v>
       </c>
       <c r="I14" s="52"/>
@@ -5322,7 +5310,7 @@
       <c r="G15" s="91" t="s">
         <v>428</v>
       </c>
-      <c r="H15" s="113" t="s">
+      <c r="H15" s="48" t="s">
         <v>662</v>
       </c>
       <c r="I15" s="48"/>
@@ -5364,7 +5352,7 @@
       <c r="G16" s="89" t="s">
         <v>237</v>
       </c>
-      <c r="H16" s="118" t="s">
+      <c r="H16" t="s">
         <v>237</v>
       </c>
       <c r="I16" t="s">
@@ -5411,7 +5399,7 @@
       <c r="G17" s="89" t="s">
         <v>238</v>
       </c>
-      <c r="H17" s="118" t="s">
+      <c r="H17" t="s">
         <v>691</v>
       </c>
       <c r="I17" t="s">
@@ -5455,7 +5443,7 @@
       <c r="G18" s="89" t="s">
         <v>239</v>
       </c>
-      <c r="H18" s="110" t="s">
+      <c r="H18" t="s">
         <v>663</v>
       </c>
       <c r="I18" t="s">
@@ -5499,7 +5487,7 @@
       <c r="G19" s="89" t="s">
         <v>240</v>
       </c>
-      <c r="H19" s="118" t="s">
+      <c r="H19" t="s">
         <v>664</v>
       </c>
       <c r="I19" t="s">
@@ -5537,7 +5525,7 @@
       <c r="G20" s="89" t="s">
         <v>363</v>
       </c>
-      <c r="H20" s="118" t="s">
+      <c r="H20" t="s">
         <v>665</v>
       </c>
       <c r="I20" t="s">
@@ -5581,7 +5569,7 @@
       <c r="G21" s="91" t="s">
         <v>397</v>
       </c>
-      <c r="H21" s="113" t="s">
+      <c r="H21" s="48" t="s">
         <v>666</v>
       </c>
       <c r="I21" s="48" t="s">
@@ -5625,7 +5613,7 @@
       <c r="G22" s="89" t="s">
         <v>362</v>
       </c>
-      <c r="H22" s="118" t="s">
+      <c r="H22" t="s">
         <v>667</v>
       </c>
       <c r="I22" t="s">
@@ -5669,7 +5657,7 @@
       <c r="G23" s="89" t="s">
         <v>253</v>
       </c>
-      <c r="H23" s="118" t="s">
+      <c r="H23" t="s">
         <v>253</v>
       </c>
       <c r="I23" t="s">
@@ -5713,7 +5701,7 @@
       <c r="G24" s="93" t="s">
         <v>395</v>
       </c>
-      <c r="H24" s="115" t="s">
+      <c r="H24" s="52" t="s">
         <v>668</v>
       </c>
       <c r="I24" s="52" t="s">
@@ -5757,7 +5745,7 @@
       <c r="G25" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="H25" s="118" t="s">
+      <c r="H25" t="s">
         <v>670</v>
       </c>
       <c r="I25" t="s">
@@ -5801,7 +5789,7 @@
       <c r="G26" s="91" t="s">
         <v>268</v>
       </c>
-      <c r="H26" s="113" t="s">
+      <c r="H26" s="48" t="s">
         <v>671</v>
       </c>
       <c r="I26" s="48" t="s">
@@ -5845,7 +5833,7 @@
       <c r="G27" s="93" t="s">
         <v>396</v>
       </c>
-      <c r="H27" s="115" t="s">
+      <c r="H27" s="52" t="s">
         <v>672</v>
       </c>
       <c r="I27" s="52" t="s">
@@ -5889,7 +5877,7 @@
       <c r="G28" s="89" t="s">
         <v>252</v>
       </c>
-      <c r="H28" s="118" t="s">
+      <c r="H28" t="s">
         <v>673</v>
       </c>
       <c r="I28" t="s">
@@ -5933,7 +5921,7 @@
       <c r="G29" s="91" t="s">
         <v>245</v>
       </c>
-      <c r="H29" s="113" t="s">
+      <c r="H29" s="48" t="s">
         <v>674</v>
       </c>
       <c r="I29" s="48" t="s">
@@ -5977,7 +5965,7 @@
       <c r="G30" s="89" t="s">
         <v>392</v>
       </c>
-      <c r="H30" s="118" t="s">
+      <c r="H30" t="s">
         <v>675</v>
       </c>
       <c r="I30" t="s">
@@ -6021,7 +6009,7 @@
       <c r="G31" s="91" t="s">
         <v>393</v>
       </c>
-      <c r="H31" s="113" t="s">
+      <c r="H31" s="48" t="s">
         <v>676</v>
       </c>
       <c r="I31" s="48" t="s">
@@ -6065,7 +6053,7 @@
       <c r="G32" s="94" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="116" t="s">
+      <c r="H32" s="76" t="s">
         <v>677</v>
       </c>
       <c r="I32" s="76" t="s">
@@ -6109,7 +6097,7 @@
       <c r="G33" s="88" t="s">
         <v>364</v>
       </c>
-      <c r="H33" s="109" t="s">
+      <c r="H33" s="22" t="s">
         <v>678</v>
       </c>
       <c r="I33" s="22" t="s">
@@ -6153,7 +6141,7 @@
       <c r="G34" s="88" t="s">
         <v>249</v>
       </c>
-      <c r="H34" s="109" t="s">
+      <c r="H34" s="22" t="s">
         <v>679</v>
       </c>
       <c r="I34" s="22" t="s">
@@ -6197,7 +6185,7 @@
       <c r="G35" s="88" t="s">
         <v>250</v>
       </c>
-      <c r="H35" s="109" t="s">
+      <c r="H35" s="22" t="s">
         <v>680</v>
       </c>
       <c r="I35" s="22" t="s">
@@ -6241,7 +6229,7 @@
       <c r="G36" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="H36" s="117" t="s">
+      <c r="H36" s="79" t="s">
         <v>681</v>
       </c>
       <c r="I36" s="79" t="s">
@@ -6283,7 +6271,7 @@
       <c r="G37" s="89" t="s">
         <v>394</v>
       </c>
-      <c r="H37" s="118" t="s">
+      <c r="H37" t="s">
         <v>669</v>
       </c>
       <c r="I37" t="s">
@@ -6327,7 +6315,7 @@
       <c r="G38" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="H38" s="118" t="s">
+      <c r="H38" t="s">
         <v>656</v>
       </c>
       <c r="I38" t="s">
@@ -6371,7 +6359,7 @@
       <c r="G39" s="89" t="s">
         <v>367</v>
       </c>
-      <c r="H39" s="118" t="s">
+      <c r="H39" t="s">
         <v>431</v>
       </c>
       <c r="I39" t="s">
@@ -6415,7 +6403,7 @@
       <c r="G40" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="H40" s="118" t="s">
+      <c r="H40" t="s">
         <v>682</v>
       </c>
       <c r="I40" t="s">
@@ -6459,7 +6447,7 @@
       <c r="G41" s="89" t="s">
         <v>360</v>
       </c>
-      <c r="H41" s="118" t="s">
+      <c r="H41" t="s">
         <v>684</v>
       </c>
       <c r="I41" t="s">
@@ -6503,7 +6491,7 @@
       <c r="G42" s="89" t="s">
         <v>272</v>
       </c>
-      <c r="H42" s="118" t="s">
+      <c r="H42" t="s">
         <v>683</v>
       </c>
       <c r="I42" t="s">
@@ -6547,7 +6535,7 @@
       <c r="G43" s="91" t="s">
         <v>361</v>
       </c>
-      <c r="H43" s="118" t="s">
+      <c r="H43" t="s">
         <v>685</v>
       </c>
       <c r="I43" t="s">
@@ -6591,7 +6579,7 @@
       <c r="G44" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="H44" s="116" t="s">
+      <c r="H44" s="76" t="s">
         <v>686</v>
       </c>
       <c r="I44" s="76" t="s">
@@ -6635,7 +6623,7 @@
       <c r="G45" s="89" t="s">
         <v>391</v>
       </c>
-      <c r="H45" s="118" t="s">
+      <c r="H45" t="s">
         <v>687</v>
       </c>
       <c r="I45" t="s">
@@ -6679,7 +6667,7 @@
       <c r="G46" s="89" t="s">
         <v>390</v>
       </c>
-      <c r="H46" s="118" t="s">
+      <c r="H46" t="s">
         <v>688</v>
       </c>
       <c r="I46" t="s">
@@ -6723,7 +6711,7 @@
       <c r="G47" s="91" t="s">
         <v>256</v>
       </c>
-      <c r="H47" s="113" t="s">
+      <c r="H47" s="48" t="s">
         <v>690</v>
       </c>
       <c r="I47" s="48" t="s">
@@ -6767,7 +6755,7 @@
       <c r="G48" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="115" t="s">
+      <c r="H48" s="52" t="s">
         <v>29</v>
       </c>
       <c r="I48" s="52" t="s">
@@ -6811,7 +6799,7 @@
       <c r="G49" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="H49" s="113" t="s">
+      <c r="H49" s="48" t="s">
         <v>30</v>
       </c>
       <c r="I49" s="48" t="s">
@@ -6855,7 +6843,7 @@
       <c r="G50" s="96" t="s">
         <v>409</v>
       </c>
-      <c r="H50" s="112"/>
+      <c r="H50" s="8"/>
       <c r="I50" s="8" t="s">
         <v>413</v>
       </c>
@@ -6893,7 +6881,7 @@
       <c r="G51" s="96" t="s">
         <v>410</v>
       </c>
-      <c r="H51" s="112"/>
+      <c r="H51" s="8"/>
       <c r="I51" s="8" t="s">
         <v>414</v>
       </c>

</xml_diff>